<commit_message>
redo lme4 modeling to get pvals for population. Working on heat maps. 4 different ones?
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13095" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="intGOterms" sheetId="1" r:id="rId1"/>
@@ -1582,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:R25"/>
     </sheetView>
   </sheetViews>
@@ -2375,7 +2375,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A16"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2566,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G235" sqref="G235"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3850,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tables of GO terms! wooo...?
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,20 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13095"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20520" windowHeight="7515" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="intGOterms" sheetId="1" r:id="rId1"/>
-    <sheet name="OriginGOterms" sheetId="2" r:id="rId2"/>
-    <sheet name="TrtGOterms" sheetId="3" r:id="rId3"/>
-    <sheet name="PC1GOterms" sheetId="4" r:id="rId4"/>
+    <sheet name="int_invUp2d" sheetId="6" r:id="rId2"/>
+    <sheet name="int_invDn2d" sheetId="7" r:id="rId3"/>
+    <sheet name="OriginGOterms" sheetId="2" r:id="rId4"/>
+    <sheet name="o_invUp0" sheetId="8" r:id="rId5"/>
+    <sheet name="o_invDn0" sheetId="9" r:id="rId6"/>
+    <sheet name="TrtGOterms" sheetId="3" r:id="rId7"/>
+    <sheet name="PC1GOterms" sheetId="4" r:id="rId8"/>
+    <sheet name="FromInvSyn" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="544">
   <si>
     <t>GO:0006412</t>
   </si>
@@ -1241,13 +1246,421 @@
   </si>
   <si>
     <t>22 GO:0055114                 oxidation-reduction process      2131          56    41.85     0.00819</t>
+  </si>
+  <si>
+    <t>C. diffusa</t>
+  </si>
+  <si>
+    <t>GO:0017126</t>
+  </si>
+  <si>
+    <t>nucleologenesis</t>
+  </si>
+  <si>
+    <t>GO:0010019</t>
+  </si>
+  <si>
+    <t>chloroplast-nucleus signaling pathway</t>
+  </si>
+  <si>
+    <t>GO:0051302</t>
+  </si>
+  <si>
+    <t>regulation of cell division</t>
+  </si>
+  <si>
+    <t>GO:0009451</t>
+  </si>
+  <si>
+    <t>RNA modification</t>
+  </si>
+  <si>
+    <t>GO:0051202</t>
+  </si>
+  <si>
+    <t>phytochromobilin metabolic process</t>
+  </si>
+  <si>
+    <t>GO:0033014</t>
+  </si>
+  <si>
+    <t>tetrapyrrole biosynthetic process</t>
+  </si>
+  <si>
+    <t>GO:0006997</t>
+  </si>
+  <si>
+    <t>nucleus organization</t>
+  </si>
+  <si>
+    <t>GO:0010024</t>
+  </si>
+  <si>
+    <t>phytochromobilin biosynthetic process</t>
+  </si>
+  <si>
+    <t>GO:0006413</t>
+  </si>
+  <si>
+    <t>translational initiation</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>parentchildFisher P value</t>
+  </si>
+  <si>
+    <t>significantly enriched GO terms for quickly evolving genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -  GO analysis of Cdif microarrays; genes with sig Origin*Trt effect </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60863 available genes (all genes from the array):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - symbol:  DKTR001_white_c11792 DKTR001_white_s64574 DKUS022_white_c32880 DKUS022_white_c43404 DKUS022_white_rep_c59243  ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 146  significant genes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56957 feasible genes (genes that can be used in the analysis):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - symbol:  DKTR001_white_c11792 DKTR001_white_s64574 DKUS022_white_c32880 DKUS022_white_rep_c59243 Contig8320  ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 137  significant genes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - number of nodes = 2748 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - number of edges = 5862 </t>
+  </si>
+  <si>
+    <t>2748 GO terms scored: 32 terms with p &lt; 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Annotated genes: 56957 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant genes: 137 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nontrivial nodes: 516 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 49  significant genes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 43  significant genes. </t>
+  </si>
+  <si>
+    <t>1  GO:0006412                                 translation      3074          73     7.39     &lt; 1e-30</t>
+  </si>
+  <si>
+    <t>2  GO:0009059          macromolecule biosynthetic process      8317          76    20.01     1.5e-20</t>
+  </si>
+  <si>
+    <t>3  GO:0019538                   protein metabolic process     11448          84    27.54     4.9e-19</t>
+  </si>
+  <si>
+    <t>4  GO:0010467                             gene expression      7467          76    17.96     9.0e-18</t>
+  </si>
+  <si>
+    <t>5  GO:0034645 cellular macromolecule biosynthetic proc...      8261          76    19.87     1.2e-16</t>
+  </si>
+  <si>
+    <t>6  GO:0044267          cellular protein metabolic process     10299          84    24.77     4.6e-15</t>
+  </si>
+  <si>
+    <t>7  GO:0009058                        biosynthetic process     13528          80    32.54     2.9e-13</t>
+  </si>
+  <si>
+    <t>8  GO:0044249               cellular biosynthetic process     12666          80    30.47     2.6e-12</t>
+  </si>
+  <si>
+    <t>9  GO:0044260    cellular macromolecule metabolic process     15809          87    38.03     1.3e-11</t>
+  </si>
+  <si>
+    <t>10 GO:0071840 cellular component organization or bioge...      5793          42    13.93     3.3e-11</t>
+  </si>
+  <si>
+    <t>11 GO:1901576      organic substance biosynthetic process     12929          77    31.10     1.2e-10</t>
+  </si>
+  <si>
+    <t>12 GO:0043170             macromolecule metabolic process     17320          87    41.66     2.8e-10</t>
+  </si>
+  <si>
+    <t>13 GO:0022613        ribonucleoprotein complex biogenesis       879          28     2.11     5.4e-10</t>
+  </si>
+  <si>
+    <t>14 GO:0009987                            cellular process     31131         103    74.88     5.4e-07</t>
+  </si>
+  <si>
+    <t>15 GO:0044237                  cellular metabolic process     24782          95    59.61     1.7e-06</t>
+  </si>
+  <si>
+    <t>16 GO:0008152                           metabolic process     30488         100    73.33     2.3e-06</t>
+  </si>
+  <si>
+    <t>17 GO:0045039 protein import into mitochondrial inner ...        14           3     0.03     6.6e-06</t>
+  </si>
+  <si>
+    <t>18 GO:0090151 establishment of protein localization to...        19           3     0.05     2.3e-05</t>
+  </si>
+  <si>
+    <t>19 GO:0044085               cellular component biogenesis      2718          33     6.54     2.6e-05</t>
+  </si>
+  <si>
+    <t>20 GO:0007006         mitochondrial membrane organization        21           3     0.05     4.5e-05</t>
+  </si>
+  <si>
+    <t>21 GO:0044238                   primary metabolic process     23325          91    56.10     0.00015</t>
+  </si>
+  <si>
+    <t>22 GO:0034660                     ncRNA metabolic process       701           7     1.69     0.00058</t>
+  </si>
+  <si>
+    <t>23 GO:1902589      single-organism organelle organization      1087           6     2.61     0.00064</t>
+  </si>
+  <si>
+    <t>24 GO:0006626          protein targeting to mitochondrion        73           3     0.18     0.00075</t>
+  </si>
+  <si>
+    <t>25 GO:0034470                            ncRNA processing       415           7     1.00     0.00118</t>
+  </si>
+  <si>
+    <t>26 GO:0070585       protein localization to mitochondrion        73           3     0.18     0.00176</t>
+  </si>
+  <si>
+    <t>27 GO:0072655 establishment of protein localization to...        73           3     0.18     0.00204</t>
+  </si>
+  <si>
+    <t>28 GO:0065002 intracellular protein transmembrane tran...       169           3     0.41     0.00490</t>
+  </si>
+  <si>
+    <t>29 GO:1902578                single-organism localization       256           3     0.62     0.00492</t>
+  </si>
+  <si>
+    <t>30 GO:0071806             protein transmembrane transport       169           3     0.41     0.00599</t>
+  </si>
+  <si>
+    <t>31 GO:0072657            protein localization to membrane       168           3     0.40     0.00772</t>
+  </si>
+  <si>
+    <t>32 GO:0007005                  mitochondrion organization       148           3     0.36     0.00971</t>
+  </si>
+  <si>
+    <t>.------------------------- topGOdata object -------------------------</t>
+  </si>
+  <si>
+    <t>2748 GO terms scored: 8 terms with p &lt; 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Annotated genes: 56957 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Significant genes: 43 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nontrivial nodes: 289 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       GO.ID                                   Term Annotated Significant Expected parentchild</t>
+  </si>
+  <si>
+    <t>1 GO:0008152                      metabolic process     30488          34    23.02     0.00047</t>
+  </si>
+  <si>
+    <t>2 GO:0009247        glycolipid biosynthetic process        49           2     0.04     0.00137</t>
+  </si>
+  <si>
+    <t>3 GO:0006664           glycolipid metabolic process       101           2     0.08     0.00230</t>
+  </si>
+  <si>
+    <t>4 GO:0071496 cellular response to external stimulus       421           3     0.32     0.00259</t>
+  </si>
+  <si>
+    <t>5 GO:0044255       cellular lipid metabolic process      2038           7     1.54     0.00351</t>
+  </si>
+  <si>
+    <t>6 GO:0009991     response to extracellular stimulus       485           3     0.37     0.00397</t>
+  </si>
+  <si>
+    <t>7 GO:0046467    membrane lipid biosynthetic process       102           2     0.08     0.00524</t>
+  </si>
+  <si>
+    <t>8 GO:0006629                lipid metabolic process      3085           9     2.33     0.00576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 181  significant genes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 173  significant genes. </t>
+  </si>
+  <si>
+    <t>2748 GO terms scored: 29 terms with p &lt; 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Significant genes: 173 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nontrivial nodes: 747 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 212  significant genes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - 196  significant genes. </t>
+  </si>
+  <si>
+    <t>2748 GO terms scored: 13 terms with p &lt; 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Significant genes: 196 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nontrivial nodes: 830 </t>
+  </si>
+  <si>
+    <t>1  GO:0043412                  macromolecule modification      5387          33    18.54     4.1e-05</t>
+  </si>
+  <si>
+    <t>2  GO:0009690                 cytokinin metabolic process        47           3     0.16     0.00019</t>
+  </si>
+  <si>
+    <t>3  GO:0006464       cellular protein modification process      5082          32    17.49     0.00070</t>
+  </si>
+  <si>
+    <t>4  GO:0007165                         signal transduction      3110          20    10.70     0.00086</t>
+  </si>
+  <si>
+    <t>5  GO:0036211                protein modification process      5082          32    17.49     0.00089</t>
+  </si>
+  <si>
+    <t>6  GO:0034754          cellular hormone metabolic process        74           3     0.25     0.00171</t>
+  </si>
+  <si>
+    <t>7  GO:0009699        phenylpropanoid biosynthetic process       382           5     1.31     0.00171</t>
+  </si>
+  <si>
+    <t>8  GO:0015851                        nucleobase transport        19           2     0.07     0.00211</t>
+  </si>
+  <si>
+    <t>9  GO:0060548           negative regulation of cell death        78           3     0.27     0.00319</t>
+  </si>
+  <si>
+    <t>10 GO:0023052                                   signaling      3128          20    10.76     0.00586</t>
+  </si>
+  <si>
+    <t>11 GO:0032989            cellular component morphogenesis       904           7     3.11     0.00620</t>
+  </si>
+  <si>
+    <t>12 GO:0031537 regulation of anthocyanin metabolic proc...        45           2     0.15     0.00636</t>
+  </si>
+  <si>
+    <t>13 GO:0016137                 glycoside metabolic process        33           2     0.11     0.00818</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>1  GO:0009813              flavonoid biosynthetic process       336           7     1.02     7.8e-05</t>
+  </si>
+  <si>
+    <t>2  GO:0006508                                 proteolysis      2280          16     6.93     8.2e-05</t>
+  </si>
+  <si>
+    <t>3  GO:0009812                 flavonoid metabolic process       378           7     1.15     0.00018</t>
+  </si>
+  <si>
+    <t>4  GO:0019852           L-ascorbic acid metabolic process        37           3     0.11     0.00026</t>
+  </si>
+  <si>
+    <t>5  GO:0043086 negative regulation of catalytic activit...        39           4     0.12     0.00028</t>
+  </si>
+  <si>
+    <t>6  GO:0048468                            cell development       716           7     2.17     0.00036</t>
+  </si>
+  <si>
+    <t>7  GO:0019853        L-ascorbic acid biosynthetic process        37           3     0.11     0.00044</t>
+  </si>
+  <si>
+    <t>8  GO:2001289                   lipid X metabolic process        10           2     0.03     0.00048</t>
+  </si>
+  <si>
+    <t>9  GO:0006040               amino sugar metabolic process        37           3     0.11     0.00152</t>
+  </si>
+  <si>
+    <t>10 GO:0016051           carbohydrate biosynthetic process       727           8     2.21     0.00158</t>
+  </si>
+  <si>
+    <t>11 GO:0009110                vitamin biosynthetic process       199           4     0.60     0.00178</t>
+  </si>
+  <si>
+    <t>12 GO:0015980 energy derivation by oxidation of organi...       472           6     1.43     0.00227</t>
+  </si>
+  <si>
+    <t>13 GO:0050790            regulation of catalytic activity       389           5     1.18     0.00264</t>
+  </si>
+  <si>
+    <t>14 GO:0044257          cellular protein catabolic process      1125           8     3.42     0.00355</t>
+  </si>
+  <si>
+    <t>15 GO:0044092 negative regulation of molecular functio...        79           4     0.24     0.00382</t>
+  </si>
+  <si>
+    <t>16 GO:0006013                   mannose metabolic process        24           3     0.07     0.00477</t>
+  </si>
+  <si>
+    <t>17 GO:0065009            regulation of molecular function       451           5     1.37     0.00507</t>
+  </si>
+  <si>
+    <t>18 GO:0006766                   vitamin metabolic process       207           4     0.63     0.00642</t>
+  </si>
+  <si>
+    <t>19 GO:0021700                    developmental maturation       204           3     0.62     0.00667</t>
+  </si>
+  <si>
+    <t>20 GO:0009888                          tissue development      1146           7     3.48     0.00670</t>
+  </si>
+  <si>
+    <t>21 GO:0006083                   acetate metabolic process        58           2     0.18     0.00672</t>
+  </si>
+  <si>
+    <t>22 GO:0044723 single-organism carbohydrate metabolic p...      1665          11     5.06     0.00729</t>
+  </si>
+  <si>
+    <t>23 GO:0006015 5-phosphoribose 1-diphosphate biosynthet...        32           2     0.10     0.00741</t>
+  </si>
+  <si>
+    <t>24 GO:0015979                              photosynthesis      1874          12     5.69     0.00742</t>
+  </si>
+  <si>
+    <t>25 GO:0019307                mannose biosynthetic process        12           3     0.04     0.00752</t>
+  </si>
+  <si>
+    <t>26 GO:1901135 carbohydrate derivative metabolic proces...      1978          13     6.01     0.00775</t>
+  </si>
+  <si>
+    <t>27 GO:0006740                          NADPH regeneration        92           3     0.28     0.00825</t>
+  </si>
+  <si>
+    <t>28 GO:0046391 5-phosphoribose 1-diphosphate metabolic ...        32           2     0.10     0.00847</t>
+  </si>
+  <si>
+    <t>29 GO:0010876                          lipid localization       333           3     1.01     0.00872</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1261,13 +1674,34 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1282,10 +1716,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,7 +2030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:R25"/>
     </sheetView>
   </sheetViews>
@@ -2371,6 +2819,427 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="55.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="R1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="R3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I7" t="s">
+        <v>439</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="I9" t="s">
+        <v>440</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I10" t="s">
+        <v>441</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="I12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="R10" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="R11" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="R13" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="R14" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="R15" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="17" spans="18:18">
+      <c r="R17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="18:18">
+      <c r="R18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="18:18">
+      <c r="R19" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20" spans="18:18">
+      <c r="R20" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="18:18">
+      <c r="R22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R24"/>
   <sheetViews>
@@ -2562,7 +3431,431 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="55.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="57.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="7"/>
+      <c r="R15" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="8" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="17" spans="18:18">
+      <c r="R17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="18:18">
+      <c r="R18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="18:18">
+      <c r="R19" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20" spans="18:18">
+      <c r="R20" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="18:18">
+      <c r="R22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R237"/>
   <sheetViews>
@@ -3846,7 +5139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R24"/>
   <sheetViews>
@@ -4061,4 +5354,258 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B20:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2.4799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2.81E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2.9399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="5">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>3.5499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.8300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D10" s="5">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>4.82E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Restart pop modeling for Origin*Trt models after Darjeeling crash. Also start Origin*PC1 modeling... just in case.
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20520" windowHeight="7515" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20520" windowHeight="7515" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="intGOterms" sheetId="1" r:id="rId1"/>
@@ -1678,10 +1678,12 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3678,7 +3680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
@@ -5143,7 +5145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Comparing dr tmpt0 w/ dr tmpt2. what do the two ranges do in response to dr? Using strict > to compare pop and range mean values. Maybe use something for nearly equal?
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515" activeTab="2"/>
+    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryOrigin" sheetId="28" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5030" uniqueCount="2433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5182" uniqueCount="2441">
   <si>
     <t>GO:0006412</t>
   </si>
@@ -7341,6 +7341,30 @@
   </si>
   <si>
     <t>phosphoenolpyruvate transport</t>
+  </si>
+  <si>
+    <t>InvdrT2 rel to InvdrT0</t>
+  </si>
+  <si>
+    <t>NatdrT2 rel to NatdrT0</t>
+  </si>
+  <si>
+    <t>reasoning</t>
+  </si>
+  <si>
+    <t>direction in inv drought, tmpt2 rel to nat dr tmpt2</t>
+  </si>
+  <si>
+    <t>direction in inv control tmpt 2 rel to nat control tmpt 2</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>inv dr incr 80 genes over T0</t>
+  </si>
+  <si>
+    <t>nat dr incr 103 genes over T0</t>
   </si>
 </sst>
 </file>
@@ -7379,7 +7403,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7404,6 +7428,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -7417,7 +7459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7441,11 +7483,127 @@
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -7737,8 +7895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:H26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16960,10 +17118,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16971,9 +17132,11 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="59.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="13"/>
+    <col min="12" max="12" width="19.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>1934</v>
       </c>
@@ -16996,68 +17159,89 @@
         <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>952</v>
+        <v>2436</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>954</v>
       </c>
       <c r="J1" t="s">
-        <v>953</v>
+        <v>2437</v>
       </c>
       <c r="K1" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="13" t="s">
+        <v>2433</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2435</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>2434</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1933</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D2" s="13">
-        <v>2007</v>
+        <v>1397</v>
       </c>
       <c r="E2" s="13">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="F2" s="13">
-        <v>9.67</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>2</v>
+        <v>6.73</v>
+      </c>
+      <c r="G2" s="13">
+        <v>8.3400000000000002E-3</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>942</v>
       </c>
       <c r="J2" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B3" s="13" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="13">
-        <v>5027</v>
-      </c>
-      <c r="E3" s="13">
-        <v>85</v>
-      </c>
-      <c r="F3" s="13">
-        <v>24.21</v>
-      </c>
-      <c r="G3" s="14">
-        <v>2.0999999999999998E-15</v>
+      <c r="F3">
+        <v>0.17</v>
+      </c>
+      <c r="G3">
+        <v>6.6699999999999997E-3</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>933</v>
@@ -17065,28 +17249,34 @@
       <c r="J3" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>5</v>
+        <v>1931</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1912</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="13">
-        <v>5610</v>
-      </c>
-      <c r="E4" s="13">
-        <v>84</v>
-      </c>
-      <c r="F4" s="13">
-        <v>27.02</v>
-      </c>
-      <c r="G4" s="14">
-        <v>6.2999999999999998E-15</v>
+        <v>1913</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G4">
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>933</v>
@@ -17094,57 +17284,71 @@
       <c r="J4" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>1933</v>
+      <c r="L4" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="13" t="s">
+        <v>1932</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>1928</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>1929</v>
       </c>
       <c r="D5" s="13">
-        <v>7650</v>
+        <v>18</v>
       </c>
       <c r="E5" s="13">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="F5" s="13">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="G5" s="14">
-        <v>3.6999999999999999E-13</v>
-      </c>
-      <c r="H5" s="9" t="s">
+        <v>0.09</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="J5" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="K5" s="13"/>
+      <c r="L5" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>1933</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D6" s="13">
-        <v>6883</v>
+        <v>2007</v>
       </c>
       <c r="E6" s="13">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F6" s="13">
-        <v>33.15</v>
-      </c>
-      <c r="G6" s="14">
-        <v>8.9000000000000004E-13</v>
+        <v>9.67</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>933</v>
@@ -17152,28 +17356,37 @@
       <c r="J6" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>1933</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>948</v>
+        <v>10</v>
       </c>
       <c r="D7" s="13">
-        <v>5574</v>
+        <v>6883</v>
       </c>
       <c r="E7" s="13">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F7" s="13">
-        <v>26.85</v>
+        <v>33.15</v>
       </c>
       <c r="G7" s="14">
-        <v>3.2000000000000001E-12</v>
+        <v>8.9000000000000004E-13</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>933</v>
@@ -17181,28 +17394,34 @@
       <c r="J7" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>1933</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>13</v>
+        <v>937</v>
       </c>
       <c r="D8" s="13">
-        <v>590</v>
+        <v>11</v>
       </c>
       <c r="E8" s="13">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F8" s="13">
-        <v>2.84</v>
+        <v>0.05</v>
       </c>
       <c r="G8" s="14">
-        <v>7.5E-10</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>933</v>
@@ -17210,28 +17429,34 @@
       <c r="J8" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>1933</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>938</v>
       </c>
       <c r="D9" s="13">
-        <v>8498</v>
+        <v>16</v>
       </c>
       <c r="E9" s="13">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="F9" s="13">
-        <v>40.93</v>
+        <v>0.08</v>
       </c>
       <c r="G9" s="14">
-        <v>2.2999999999999999E-9</v>
+        <v>4.5000000000000003E-5</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>933</v>
@@ -17239,28 +17464,34 @@
       <c r="J9" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>1933</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D10" s="13">
-        <v>9084</v>
+        <v>15584</v>
       </c>
       <c r="E10" s="13">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="F10" s="13">
-        <v>43.75</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2.7999999999999998E-9</v>
+        <v>75.06</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>933</v>
@@ -17268,57 +17499,75 @@
       <c r="J10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>1933</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="13">
-        <v>20227</v>
+        <v>16705</v>
       </c>
       <c r="E11" s="13">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="F11" s="13">
-        <v>97.42</v>
-      </c>
-      <c r="G11" s="14">
-        <v>1.4E-8</v>
-      </c>
-      <c r="H11" s="10" t="s">
+        <v>80.459999999999994</v>
+      </c>
+      <c r="G11" s="13">
+        <v>4.13E-3</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>934</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>944</v>
+      </c>
+      <c r="J11" t="s">
         <v>931</v>
       </c>
-      <c r="J11" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>20</v>
+        <v>1932</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1920</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D12">
+        <v>1495</v>
+      </c>
+      <c r="E12">
         <v>21</v>
       </c>
-      <c r="D12" s="13">
-        <v>10620</v>
-      </c>
-      <c r="E12" s="13">
-        <v>104</v>
-      </c>
-      <c r="F12" s="13">
-        <v>51.15</v>
-      </c>
-      <c r="G12" s="14">
-        <v>5.1E-8</v>
+      <c r="F12">
+        <v>7.52</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.0000000000000005E-8</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>933</v>
@@ -17326,27 +17575,33 @@
       <c r="J12" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>22</v>
+        <v>1931</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1876</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>936</v>
-      </c>
-      <c r="D13" s="13">
-        <v>3882</v>
-      </c>
-      <c r="E13" s="13">
-        <v>43</v>
-      </c>
-      <c r="F13" s="13">
-        <v>18.7</v>
-      </c>
-      <c r="G13" s="14">
+        <v>1877</v>
+      </c>
+      <c r="D13">
+        <v>2318</v>
+      </c>
+      <c r="E13">
+        <v>33</v>
+      </c>
+      <c r="F13">
+        <v>12.17</v>
+      </c>
+      <c r="G13" s="1">
         <v>1.4000000000000001E-7</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -17355,86 +17610,110 @@
       <c r="J13" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>23</v>
+        <v>1931</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1880</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="13">
-        <v>8663</v>
-      </c>
-      <c r="E14" s="13">
-        <v>91</v>
-      </c>
-      <c r="F14" s="13">
-        <v>41.72</v>
-      </c>
-      <c r="G14" s="14">
-        <v>2.7000000000000001E-7</v>
+        <v>1881</v>
+      </c>
+      <c r="D14">
+        <v>1985</v>
+      </c>
+      <c r="E14">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>10.42</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6.4000000000000001E-7</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I14" s="13" t="s">
+        <v>1824</v>
+      </c>
       <c r="J14" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>25</v>
+        <v>1931</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1886</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="13">
-        <v>20735</v>
-      </c>
-      <c r="E15" s="13">
-        <v>132</v>
-      </c>
-      <c r="F15" s="13">
-        <v>99.87</v>
-      </c>
-      <c r="G15" s="14">
-        <v>5.6000000000000004E-7</v>
+        <v>1887</v>
+      </c>
+      <c r="D15">
+        <v>3056</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>16.04</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.1E-5</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I15" s="13" t="s">
+        <v>1823</v>
+      </c>
       <c r="J15" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>27</v>
+        <v>1931</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1892</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="13">
-        <v>16463</v>
-      </c>
-      <c r="E16" s="13">
-        <v>123</v>
-      </c>
-      <c r="F16" s="13">
-        <v>79.290000000000006</v>
-      </c>
-      <c r="G16" s="14">
-        <v>9.1999999999999998E-7</v>
+        <v>1893</v>
+      </c>
+      <c r="D16">
+        <v>3492</v>
+      </c>
+      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>933</v>
@@ -17442,28 +17721,34 @@
       <c r="J16" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" s="16" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>1933</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>937</v>
+        <v>4</v>
       </c>
       <c r="D17" s="13">
-        <v>11</v>
+        <v>5027</v>
       </c>
       <c r="E17" s="13">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="F17" s="13">
-        <v>0.05</v>
+        <v>24.21</v>
       </c>
       <c r="G17" s="14">
-        <v>1.0000000000000001E-5</v>
+        <v>2.0999999999999998E-15</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>933</v>
@@ -17471,28 +17756,34 @@
       <c r="J17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="L17" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>1933</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D18" s="13">
-        <v>11611</v>
+        <v>5610</v>
       </c>
       <c r="E18" s="13">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="F18" s="13">
-        <v>55.92</v>
+        <v>27.02</v>
       </c>
       <c r="G18" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>6.2999999999999998E-15</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>933</v>
@@ -17500,28 +17791,34 @@
       <c r="J18" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="L18" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>1933</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D19" s="13">
-        <v>1792</v>
+        <v>7650</v>
       </c>
       <c r="E19" s="13">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="F19" s="13">
-        <v>8.6300000000000008</v>
+        <v>36.840000000000003</v>
       </c>
       <c r="G19" s="14">
-        <v>4.0000000000000003E-5</v>
+        <v>3.6999999999999999E-13</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>933</v>
@@ -17529,28 +17826,34 @@
       <c r="J19" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="L19" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>1933</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>938</v>
+        <v>948</v>
       </c>
       <c r="D20" s="13">
-        <v>16</v>
+        <v>5574</v>
       </c>
       <c r="E20" s="13">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="F20" s="13">
-        <v>0.08</v>
+        <v>26.85</v>
       </c>
       <c r="G20" s="14">
-        <v>4.5000000000000003E-5</v>
+        <v>3.2000000000000001E-12</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>933</v>
@@ -17558,28 +17861,34 @@
       <c r="J20" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="L20" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>1933</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D21" s="13">
-        <v>18</v>
+        <v>590</v>
       </c>
       <c r="E21" s="13">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F21" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1.3999999999999999E-4</v>
+        <v>2.84</v>
+      </c>
+      <c r="G21" s="14">
+        <v>7.5E-10</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>933</v>
@@ -17587,28 +17896,34 @@
       <c r="J21" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="L21" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>1933</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D22" s="13">
-        <v>15584</v>
+        <v>8498</v>
       </c>
       <c r="E22" s="13">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F22" s="13">
-        <v>75.06</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1.4999999999999999E-4</v>
+        <v>40.93</v>
+      </c>
+      <c r="G22" s="14">
+        <v>2.2999999999999999E-9</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>933</v>
@@ -17616,28 +17931,34 @@
       <c r="J22" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>1933</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>286</v>
+        <v>9084</v>
       </c>
       <c r="E23" s="13">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="F23" s="13">
-        <v>1.38</v>
-      </c>
-      <c r="G23" s="13">
-        <v>5.0000000000000001E-4</v>
+        <v>43.75</v>
+      </c>
+      <c r="G23" s="14">
+        <v>2.7999999999999998E-9</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>933</v>
@@ -17645,28 +17966,34 @@
       <c r="J23" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="L23" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>1933</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D24" s="13">
-        <v>53</v>
+        <v>10620</v>
       </c>
       <c r="E24" s="13">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F24" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G24" s="13">
-        <v>9.3000000000000005E-4</v>
+        <v>51.15</v>
+      </c>
+      <c r="G24" s="14">
+        <v>5.1E-8</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>933</v>
@@ -17674,28 +18001,34 @@
       <c r="J24" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="L24" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>1933</v>
       </c>
       <c r="B25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>936</v>
+      </c>
+      <c r="D25" s="13">
+        <v>3882</v>
+      </c>
+      <c r="E25" s="13">
         <v>43</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="13">
-        <v>484</v>
-      </c>
-      <c r="E25" s="13">
-        <v>8</v>
-      </c>
       <c r="F25" s="13">
-        <v>2.33</v>
-      </c>
-      <c r="G25" s="13">
-        <v>1.48E-3</v>
+        <v>18.7</v>
+      </c>
+      <c r="G25" s="14">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>933</v>
@@ -17703,28 +18036,34 @@
       <c r="J25" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="L25" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>1933</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D26" s="13">
-        <v>53</v>
+        <v>8663</v>
       </c>
       <c r="E26" s="13">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="F26" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G26" s="13">
-        <v>2.16E-3</v>
+        <v>41.72</v>
+      </c>
+      <c r="G26" s="14">
+        <v>2.7000000000000001E-7</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>933</v>
@@ -17732,28 +18071,34 @@
       <c r="J26" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="L26" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>1933</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>939</v>
+        <v>26</v>
       </c>
       <c r="D27" s="13">
-        <v>53</v>
+        <v>20735</v>
       </c>
       <c r="E27" s="13">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="F27" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G27" s="13">
-        <v>2.5000000000000001E-3</v>
+        <v>99.87</v>
+      </c>
+      <c r="G27" s="14">
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>933</v>
@@ -17761,89 +18106,104 @@
       <c r="J27" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="L27" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>1933</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D28" s="13">
-        <v>16705</v>
+        <v>16463</v>
       </c>
       <c r="E28" s="13">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F28" s="13">
-        <v>80.459999999999994</v>
-      </c>
-      <c r="G28" s="13">
-        <v>4.13E-3</v>
+        <v>79.290000000000006</v>
+      </c>
+      <c r="G28" s="14">
+        <v>9.1999999999999998E-7</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="J28" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="L28" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>1933</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D29" s="13">
-        <v>33</v>
+        <v>11611</v>
       </c>
       <c r="E29" s="13">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="F29" s="13">
-        <v>0.16</v>
-      </c>
-      <c r="G29" s="13">
-        <v>4.3899999999999998E-3</v>
-      </c>
-      <c r="H29" s="10" t="s">
+        <v>55.92</v>
+      </c>
+      <c r="G29" s="14">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J29" t="s">
         <v>931</v>
       </c>
-      <c r="J29" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="L29" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>1933</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>949</v>
+        <v>36</v>
       </c>
       <c r="D30" s="13">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="E30" s="13">
         <v>3</v>
       </c>
       <c r="F30" s="13">
-        <v>0.56999999999999995</v>
+        <v>0.09</v>
       </c>
       <c r="G30" s="13">
-        <v>5.4999999999999997E-3</v>
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>933</v>
@@ -17851,28 +18211,34 @@
       <c r="J30" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="L30" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>1933</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D31" s="13">
-        <v>118</v>
+        <v>286</v>
       </c>
       <c r="E31" s="13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F31" s="13">
-        <v>0.56999999999999995</v>
+        <v>1.38</v>
       </c>
       <c r="G31" s="13">
-        <v>7.0499999999999998E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>933</v>
@@ -17880,121 +18246,139 @@
       <c r="J31" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="L31" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N31" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>1933</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>56</v>
+        <v>41</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D32" s="13">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E32" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="13">
-        <v>0.34</v>
+        <v>0.26</v>
       </c>
       <c r="G32" s="13">
-        <v>7.3400000000000002E-3</v>
-      </c>
-      <c r="H32" s="10" t="s">
+        <v>9.3000000000000005E-4</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J32" t="s">
         <v>931</v>
       </c>
-      <c r="J32" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="L32" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>1933</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D33" s="13">
-        <v>250</v>
+        <v>484</v>
       </c>
       <c r="E33" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F33" s="13">
-        <v>1.2</v>
+        <v>2.33</v>
       </c>
       <c r="G33" s="13">
-        <v>8.0599999999999995E-3</v>
+        <v>1.48E-3</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="J33" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="L33" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>1933</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D34" s="13">
-        <v>1397</v>
+        <v>53</v>
       </c>
       <c r="E34" s="13">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F34" s="13">
-        <v>6.73</v>
+        <v>0.26</v>
       </c>
       <c r="G34" s="13">
-        <v>8.3400000000000002E-3</v>
+        <v>2.16E-3</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="J34" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="L34" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1916</v>
+        <v>1933</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1917</v>
-      </c>
-      <c r="D35">
-        <v>1722</v>
-      </c>
-      <c r="E35">
-        <v>72</v>
-      </c>
-      <c r="F35">
-        <v>8.66</v>
-      </c>
-      <c r="G35" t="s">
-        <v>2</v>
+        <v>939</v>
+      </c>
+      <c r="D35" s="13">
+        <v>53</v>
+      </c>
+      <c r="E35" s="13">
+        <v>3</v>
+      </c>
+      <c r="F35" s="13">
+        <v>0.26</v>
+      </c>
+      <c r="G35" s="13">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>933</v>
@@ -18002,28 +18386,34 @@
       <c r="J35" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="L35" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B36" t="s">
-        <v>1918</v>
+        <v>1933</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1919</v>
-      </c>
-      <c r="D36">
-        <v>1357</v>
-      </c>
-      <c r="E36">
-        <v>72</v>
-      </c>
-      <c r="F36">
-        <v>6.82</v>
-      </c>
-      <c r="G36" s="1">
-        <v>2.4E-8</v>
+        <v>949</v>
+      </c>
+      <c r="D36" s="13">
+        <v>118</v>
+      </c>
+      <c r="E36" s="13">
+        <v>3</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G36" s="13">
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>933</v>
@@ -18031,28 +18421,34 @@
       <c r="J36" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="L36" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1920</v>
+        <v>1933</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1921</v>
-      </c>
-      <c r="D37">
-        <v>1495</v>
-      </c>
-      <c r="E37">
-        <v>21</v>
-      </c>
-      <c r="F37">
-        <v>7.52</v>
-      </c>
-      <c r="G37" s="1">
-        <v>7.0000000000000005E-8</v>
+        <v>54</v>
+      </c>
+      <c r="D37" s="13">
+        <v>118</v>
+      </c>
+      <c r="E37" s="13">
+        <v>3</v>
+      </c>
+      <c r="F37" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G37" s="13">
+        <v>7.0499999999999998E-3</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>933</v>
@@ -18060,57 +18456,72 @@
       <c r="J37" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="L37" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1922</v>
+        <v>1933</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1923</v>
-      </c>
-      <c r="D38">
-        <v>42</v>
-      </c>
-      <c r="E38">
+        <v>58</v>
+      </c>
+      <c r="D38" s="13">
+        <v>250</v>
+      </c>
+      <c r="E38" s="13">
         <v>4</v>
       </c>
-      <c r="F38">
-        <v>0.21</v>
-      </c>
-      <c r="G38" s="1">
-        <v>2.5999999999999998E-5</v>
+      <c r="F38" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="G38" s="13">
+        <v>8.0599999999999995E-3</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>943</v>
       </c>
       <c r="J38" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="L38" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N38" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>1932</v>
       </c>
       <c r="B39" t="s">
-        <v>1924</v>
+        <v>1916</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1925</v>
+        <v>1917</v>
       </c>
       <c r="D39">
-        <v>42</v>
+        <v>1722</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="F39">
-        <v>0.21</v>
-      </c>
-      <c r="G39" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>8.66</v>
+      </c>
+      <c r="G39" t="s">
+        <v>2</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>933</v>
@@ -18118,28 +18529,34 @@
       <c r="J39" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="L39" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>1932</v>
       </c>
       <c r="B40" t="s">
-        <v>1926</v>
+        <v>1918</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
       <c r="D40">
-        <v>42</v>
+        <v>1357</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="F40">
-        <v>0.21</v>
+        <v>6.82</v>
       </c>
       <c r="G40" s="1">
-        <v>4.3999999999999999E-5</v>
+        <v>2.4E-8</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>933</v>
@@ -18147,57 +18564,71 @@
       <c r="J40" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" s="13" customFormat="1">
-      <c r="A41" s="13" t="s">
+      <c r="L40" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="13" customFormat="1">
+      <c r="A41" t="s">
         <v>1932</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>1929</v>
-      </c>
-      <c r="D41" s="13">
-        <v>18</v>
-      </c>
-      <c r="E41" s="13">
-        <v>3</v>
-      </c>
-      <c r="F41" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="G41" s="13">
-        <v>2.3E-3</v>
-      </c>
-      <c r="H41" s="10" t="s">
+      <c r="B41" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D41">
+        <v>42</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>0.21</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2.5999999999999998E-5</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J41" t="s">
         <v>931</v>
       </c>
-      <c r="J41" s="13" t="s">
+      <c r="K41"/>
+      <c r="L41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="M41"/>
+      <c r="N41" s="15" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B42" t="s">
-        <v>1848</v>
+        <v>1924</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1849</v>
+        <v>1925</v>
       </c>
       <c r="D42">
-        <v>1151</v>
+        <v>42</v>
       </c>
       <c r="E42">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>6.04</v>
-      </c>
-      <c r="G42" t="s">
-        <v>2</v>
+        <v>0.21</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>933</v>
@@ -18205,28 +18636,34 @@
       <c r="J42" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="L42" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N42" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B43" t="s">
-        <v>1850</v>
+        <v>1926</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1851</v>
+        <v>1927</v>
       </c>
       <c r="D43">
-        <v>1066</v>
+        <v>42</v>
       </c>
       <c r="E43">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>5.6</v>
-      </c>
-      <c r="G43" t="s">
-        <v>2</v>
+        <v>0.21</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>933</v>
@@ -18234,25 +18671,31 @@
       <c r="J43" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="L43" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>1931</v>
       </c>
       <c r="B44" t="s">
-        <v>1852</v>
+        <v>1848</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1853</v>
+        <v>1849</v>
       </c>
       <c r="D44">
-        <v>1767</v>
+        <v>1151</v>
       </c>
       <c r="E44">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F44">
-        <v>9.2799999999999994</v>
+        <v>6.04</v>
       </c>
       <c r="G44" t="s">
         <v>2</v>
@@ -18263,25 +18706,31 @@
       <c r="J44" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="L44" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N44" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>1931</v>
       </c>
       <c r="B45" t="s">
-        <v>1854</v>
+        <v>1850</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1855</v>
+        <v>1851</v>
       </c>
       <c r="D45">
-        <v>1595</v>
+        <v>1066</v>
       </c>
       <c r="E45">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F45">
-        <v>8.3699999999999992</v>
+        <v>5.6</v>
       </c>
       <c r="G45" t="s">
         <v>2</v>
@@ -18292,28 +18741,34 @@
       <c r="J45" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="L45" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N45" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>1931</v>
       </c>
       <c r="B46" t="s">
-        <v>1856</v>
+        <v>1852</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1857</v>
+        <v>1853</v>
       </c>
       <c r="D46">
-        <v>3016</v>
+        <v>1767</v>
       </c>
       <c r="E46">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F46">
-        <v>15.83</v>
-      </c>
-      <c r="G46" s="1">
-        <v>3.4000000000000001E-28</v>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>933</v>
@@ -18321,28 +18776,34 @@
       <c r="J46" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="L46" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N46" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>1931</v>
       </c>
       <c r="B47" t="s">
-        <v>1858</v>
+        <v>1854</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1859</v>
+        <v>1855</v>
       </c>
       <c r="D47">
-        <v>3016</v>
+        <v>1595</v>
       </c>
       <c r="E47">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F47">
-        <v>15.83</v>
-      </c>
-      <c r="G47" s="1">
-        <v>3.5E-28</v>
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="G47" t="s">
+        <v>2</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>933</v>
@@ -18350,28 +18811,34 @@
       <c r="J47" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="L47" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N47" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>1931</v>
       </c>
       <c r="B48" t="s">
-        <v>1860</v>
+        <v>1856</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>1861</v>
+        <v>1857</v>
       </c>
       <c r="D48">
-        <v>5431</v>
+        <v>3016</v>
       </c>
       <c r="E48">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F48">
-        <v>28.51</v>
+        <v>15.83</v>
       </c>
       <c r="G48" s="1">
-        <v>5.5000000000000005E-26</v>
+        <v>3.4000000000000001E-28</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>933</v>
@@ -18379,28 +18846,34 @@
       <c r="J48" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="L48" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N48" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>1931</v>
       </c>
       <c r="B49" t="s">
-        <v>1862</v>
+        <v>1858</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1863</v>
+        <v>1859</v>
       </c>
       <c r="D49">
-        <v>10580</v>
+        <v>3016</v>
       </c>
       <c r="E49">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="F49">
-        <v>55.55</v>
+        <v>15.83</v>
       </c>
       <c r="G49" s="1">
-        <v>1.8000000000000001E-19</v>
+        <v>3.5E-28</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>933</v>
@@ -18408,28 +18881,34 @@
       <c r="J49" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="L49" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N49" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>1931</v>
       </c>
       <c r="B50" t="s">
-        <v>1864</v>
+        <v>1860</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1865</v>
+        <v>1861</v>
       </c>
       <c r="D50">
-        <v>5893</v>
+        <v>5431</v>
       </c>
       <c r="E50">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F50">
-        <v>30.94</v>
+        <v>28.51</v>
       </c>
       <c r="G50" s="1">
-        <v>6.4999999999999996E-13</v>
+        <v>5.5000000000000005E-26</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>933</v>
@@ -18437,28 +18916,34 @@
       <c r="J50" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="L50" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>1931</v>
       </c>
       <c r="B51" t="s">
-        <v>1866</v>
+        <v>1862</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1867</v>
+        <v>1863</v>
       </c>
       <c r="D51">
-        <v>20261</v>
+        <v>10580</v>
       </c>
       <c r="E51">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="F51">
-        <v>106.37</v>
+        <v>55.55</v>
       </c>
       <c r="G51" s="1">
-        <v>1.1E-12</v>
+        <v>1.8000000000000001E-19</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>933</v>
@@ -18466,28 +18951,34 @@
       <c r="J51" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="L51" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N51" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>1931</v>
       </c>
       <c r="B52" t="s">
-        <v>1868</v>
+        <v>1864</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>1869</v>
+        <v>1865</v>
       </c>
       <c r="D52">
-        <v>10569</v>
+        <v>5893</v>
       </c>
       <c r="E52">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="F52">
-        <v>55.49</v>
+        <v>30.94</v>
       </c>
       <c r="G52" s="1">
-        <v>1.3E-11</v>
+        <v>6.4999999999999996E-13</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>933</v>
@@ -18495,28 +18986,34 @@
       <c r="J52" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="L52" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N52" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>1870</v>
+        <v>1866</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1871</v>
+        <v>1867</v>
       </c>
       <c r="D53">
-        <v>1115</v>
+        <v>20261</v>
       </c>
       <c r="E53">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="F53">
-        <v>5.85</v>
+        <v>106.37</v>
       </c>
       <c r="G53" s="1">
-        <v>2.9000000000000002E-8</v>
+        <v>1.1E-12</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>933</v>
@@ -18524,28 +19021,34 @@
       <c r="J53" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="L53" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N53" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>1931</v>
       </c>
       <c r="B54" t="s">
-        <v>1872</v>
+        <v>1868</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>1873</v>
+        <v>1869</v>
       </c>
       <c r="D54">
-        <v>1411</v>
+        <v>10569</v>
       </c>
       <c r="E54">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="F54">
-        <v>7.41</v>
+        <v>55.49</v>
       </c>
       <c r="G54" s="1">
-        <v>1.1000000000000001E-7</v>
+        <v>1.3E-11</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>933</v>
@@ -18553,28 +19056,34 @@
       <c r="J54" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="L54" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>1931</v>
       </c>
       <c r="B55" t="s">
-        <v>1874</v>
+        <v>1870</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1875</v>
+        <v>1871</v>
       </c>
       <c r="D55">
-        <v>2318</v>
+        <v>1115</v>
       </c>
       <c r="E55">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="F55">
-        <v>12.17</v>
+        <v>5.85</v>
       </c>
       <c r="G55" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>2.9000000000000002E-8</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>933</v>
@@ -18582,28 +19091,34 @@
       <c r="J55" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="L55" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>1931</v>
       </c>
       <c r="B56" t="s">
-        <v>1876</v>
+        <v>1872</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>1877</v>
+        <v>1873</v>
       </c>
       <c r="D56">
-        <v>2318</v>
+        <v>1411</v>
       </c>
       <c r="E56">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F56">
-        <v>12.17</v>
+        <v>7.41</v>
       </c>
       <c r="G56" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>933</v>
@@ -18611,28 +19126,34 @@
       <c r="J56" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="L56" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>1931</v>
       </c>
       <c r="B57" t="s">
-        <v>1878</v>
+        <v>1874</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>1879</v>
+        <v>1875</v>
       </c>
       <c r="D57">
-        <v>23508</v>
+        <v>2318</v>
       </c>
       <c r="E57">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="F57">
-        <v>123.42</v>
+        <v>12.17</v>
       </c>
       <c r="G57" s="1">
-        <v>5.6000000000000004E-7</v>
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>933</v>
@@ -18640,40 +19161,49 @@
       <c r="J57" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="L57" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>1931</v>
       </c>
       <c r="B58" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="D58">
-        <v>1985</v>
+        <v>23508</v>
       </c>
       <c r="E58">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="F58">
-        <v>10.42</v>
+        <v>123.42</v>
       </c>
       <c r="G58" s="1">
-        <v>6.4000000000000001E-7</v>
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I58" s="13" t="s">
-        <v>1824</v>
-      </c>
       <c r="J58" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="L58" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N58" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>1931</v>
       </c>
@@ -18701,8 +19231,14 @@
       <c r="J59" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="L59" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N59" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>1931</v>
       </c>
@@ -18730,48 +19266,57 @@
       <c r="J60" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="L60" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>1931</v>
       </c>
       <c r="B61" t="s">
-        <v>1886</v>
+        <v>1888</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>1887</v>
+        <v>1889</v>
       </c>
       <c r="D61">
-        <v>3056</v>
+        <v>27911</v>
       </c>
       <c r="E61">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="F61">
-        <v>16.04</v>
+        <v>146.54</v>
       </c>
       <c r="G61" s="1">
-        <v>1.1E-5</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H61" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I61" s="13" t="s">
-        <v>1823</v>
-      </c>
       <c r="J61" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="L61" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>1931</v>
       </c>
       <c r="B62" t="s">
-        <v>1888</v>
+        <v>1890</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>1889</v>
+        <v>1891</v>
       </c>
       <c r="D62">
         <v>27911</v>
@@ -18791,28 +19336,34 @@
       <c r="J62" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="L62" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N62" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>1931</v>
       </c>
       <c r="B63" t="s">
-        <v>1890</v>
+        <v>1894</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>1891</v>
+        <v>1895</v>
       </c>
       <c r="D63">
-        <v>27911</v>
+        <v>720</v>
       </c>
       <c r="E63">
-        <v>166</v>
+        <v>11</v>
       </c>
       <c r="F63">
-        <v>146.54</v>
-      </c>
-      <c r="G63" s="1">
-        <v>1.8E-5</v>
+        <v>3.78</v>
+      </c>
+      <c r="G63">
+        <v>1.1E-4</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>933</v>
@@ -18820,57 +19371,72 @@
       <c r="J63" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="L63" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N63" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>1931</v>
       </c>
       <c r="B64" t="s">
-        <v>1892</v>
+        <v>1896</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>1893</v>
+        <v>1897</v>
       </c>
       <c r="D64">
-        <v>3492</v>
+        <v>1969</v>
       </c>
       <c r="E64">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F64">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="G64" s="1">
-        <v>4.8000000000000001E-5</v>
+        <v>10.34</v>
+      </c>
+      <c r="G64">
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="H64" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I64" s="13" t="s">
+        <v>1825</v>
+      </c>
       <c r="J64" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="L64" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N64" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>1931</v>
       </c>
       <c r="B65" t="s">
-        <v>1894</v>
+        <v>1898</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>1895</v>
+        <v>1899</v>
       </c>
       <c r="D65">
-        <v>720</v>
+        <v>1480</v>
       </c>
       <c r="E65">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F65">
-        <v>3.78</v>
+        <v>7.77</v>
       </c>
       <c r="G65">
-        <v>1.1E-4</v>
+        <v>1.65E-3</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>933</v>
@@ -18878,176 +19444,209 @@
       <c r="J65" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="L65" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>1931</v>
       </c>
       <c r="B66" t="s">
-        <v>1896</v>
+        <v>1900</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1897</v>
+        <v>1901</v>
       </c>
       <c r="D66">
-        <v>1969</v>
+        <v>20252</v>
       </c>
       <c r="E66">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="F66">
-        <v>10.34</v>
+        <v>106.33</v>
       </c>
       <c r="G66">
-        <v>1.7000000000000001E-4</v>
+        <v>1.7700000000000001E-3</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I66" s="13" t="s">
-        <v>1825</v>
-      </c>
       <c r="J66" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="L66" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>1931</v>
       </c>
       <c r="B67" t="s">
-        <v>1898</v>
+        <v>1902</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>1899</v>
+        <v>1903</v>
       </c>
       <c r="D67">
-        <v>1480</v>
+        <v>361</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F67">
-        <v>7.77</v>
+        <v>1.9</v>
       </c>
       <c r="G67">
-        <v>1.65E-3</v>
+        <v>3.8800000000000002E-3</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J67" t="s">
+        <v>1827</v>
+      </c>
+      <c r="L67" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="N67" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>1931</v>
       </c>
       <c r="B68" t="s">
-        <v>1900</v>
+        <v>1904</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1901</v>
+        <v>1905</v>
       </c>
       <c r="D68">
-        <v>20252</v>
+        <v>361</v>
       </c>
       <c r="E68">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="F68">
-        <v>106.33</v>
+        <v>1.9</v>
       </c>
       <c r="G68">
-        <v>1.7700000000000001E-3</v>
+        <v>4.13E-3</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J68" t="s">
+        <v>1826</v>
+      </c>
+      <c r="L68" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="N68" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
         <v>1931</v>
       </c>
       <c r="B69" t="s">
-        <v>1902</v>
+        <v>1906</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>1903</v>
+        <v>1907</v>
       </c>
       <c r="D69">
-        <v>361</v>
+        <v>32</v>
       </c>
       <c r="E69">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>1.9</v>
+        <v>0.17</v>
       </c>
       <c r="G69">
-        <v>3.8800000000000002E-3</v>
+        <v>4.8300000000000001E-3</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J69" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>931</v>
+      </c>
+      <c r="L69" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N69" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>1931</v>
       </c>
       <c r="B70" t="s">
-        <v>1904</v>
+        <v>1908</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1905</v>
+        <v>1909</v>
       </c>
       <c r="D70">
-        <v>361</v>
+        <v>20703</v>
       </c>
       <c r="E70">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="F70">
-        <v>1.9</v>
+        <v>108.69</v>
       </c>
       <c r="G70">
-        <v>4.13E-3</v>
+        <v>5.6499999999999996E-3</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J70" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>931</v>
+      </c>
+      <c r="L70" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N70" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
         <v>1931</v>
       </c>
       <c r="B71" t="s">
-        <v>1906</v>
+        <v>1914</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1907</v>
+        <v>1915</v>
       </c>
       <c r="D71">
-        <v>32</v>
+        <v>19850</v>
       </c>
       <c r="E71">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="F71">
-        <v>0.17</v>
+        <v>104.21</v>
       </c>
       <c r="G71">
-        <v>4.8300000000000001E-3</v>
+        <v>8.0300000000000007E-3</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>933</v>
@@ -19055,115 +19654,136 @@
       <c r="J71" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="L71" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1908</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>1909</v>
-      </c>
-      <c r="D72">
-        <v>20703</v>
-      </c>
-      <c r="E72">
-        <v>151</v>
-      </c>
-      <c r="F72">
-        <v>108.69</v>
-      </c>
-      <c r="G72">
-        <v>5.6499999999999996E-3</v>
-      </c>
-      <c r="H72" s="9" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="13">
+        <v>20227</v>
+      </c>
+      <c r="E72" s="13">
+        <v>134</v>
+      </c>
+      <c r="F72" s="13">
+        <v>97.42</v>
+      </c>
+      <c r="G72" s="14">
+        <v>1.4E-8</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J72" t="s">
+        <v>1008</v>
+      </c>
+      <c r="L72" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N72" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D73" s="13">
+        <v>33</v>
+      </c>
+      <c r="E73" s="13">
+        <v>2</v>
+      </c>
+      <c r="F73" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="G73" s="13">
+        <v>4.3899999999999998E-3</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J73" t="s">
         <v>933</v>
       </c>
-      <c r="J72" t="s">
+      <c r="L73" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1910</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>1911</v>
-      </c>
-      <c r="D73">
+      <c r="N73" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="13">
+        <v>70</v>
+      </c>
+      <c r="E74" s="13">
+        <v>2</v>
+      </c>
+      <c r="F74" s="13">
+        <v>0.34</v>
+      </c>
+      <c r="G74" s="13">
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J74" t="s">
+        <v>933</v>
+      </c>
+      <c r="L74" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B75" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E73">
-        <v>3</v>
-      </c>
-      <c r="F73">
-        <v>0.17</v>
-      </c>
-      <c r="G73">
-        <v>6.6699999999999997E-3</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>933</v>
-      </c>
-      <c r="J73" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1912</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>1913</v>
-      </c>
-      <c r="D74">
-        <v>53</v>
-      </c>
-      <c r="E74">
-        <v>3</v>
-      </c>
-      <c r="F74">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G74">
-        <v>6.7499999999999999E-3</v>
-      </c>
-      <c r="H74" s="9" t="s">
-        <v>933</v>
-      </c>
-      <c r="J74" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1914</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>1915</v>
-      </c>
-      <c r="D75">
-        <v>19850</v>
-      </c>
-      <c r="E75">
-        <v>146</v>
-      </c>
-      <c r="F75">
-        <v>104.21</v>
-      </c>
-      <c r="G75">
-        <v>8.0300000000000007E-3</v>
+        <v>33</v>
+      </c>
+      <c r="D75" s="13">
+        <v>1792</v>
+      </c>
+      <c r="E75" s="13">
+        <v>33</v>
+      </c>
+      <c r="F75" s="13">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="G75" s="14">
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>933</v>
@@ -19171,8 +19791,16 @@
       <c r="J75" t="s">
         <v>931</v>
       </c>
+      <c r="N75" s="17" t="s">
+        <v>931</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:N75">
+    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="5"/>
+    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -25516,7 +26144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R237"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
For sig int genes in drought treatment, Used nearly equal approach to on T2 inv vs. nat (yellow and blue in spreadsheet) as well as T2 vs T0. Looks like expression is reduced in most cases for both nat and inv, but inv doesn't reduce as much. Some terms did not turn up in topGO analysis of subset of genes.
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5182" uniqueCount="2441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5404" uniqueCount="2452">
   <si>
     <t>GO:0006412</t>
   </si>
@@ -7352,12 +7352,6 @@
     <t>reasoning</t>
   </si>
   <si>
-    <t>direction in inv drought, tmpt2 rel to nat dr tmpt2</t>
-  </si>
-  <si>
-    <t>direction in inv control tmpt 2 rel to nat control tmpt 2</t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
@@ -7365,6 +7359,45 @@
   </si>
   <si>
     <t>nat dr incr 103 genes over T0</t>
+  </si>
+  <si>
+    <t>Inv DefUp dr T2  rel to T0</t>
+  </si>
+  <si>
+    <t>Nat DefUp dr T2  rel to T0</t>
+  </si>
+  <si>
+    <t>pval=0.08136</t>
+  </si>
+  <si>
+    <t>pval=0.06264</t>
+  </si>
+  <si>
+    <t>pval=0.0869</t>
+  </si>
+  <si>
+    <t>inv dr, tmpt2 rel to nat dr tmpt2</t>
+  </si>
+  <si>
+    <t>inv control tmpt 2 rel to nat control tmpt 2</t>
+  </si>
+  <si>
+    <t>NEinv dr, tmpt2 rel to nat dr tmpt2</t>
+  </si>
+  <si>
+    <t>inv up</t>
+  </si>
+  <si>
+    <t>nat up</t>
+  </si>
+  <si>
+    <t>inv pval=0.07093; nat pval = 0.1609</t>
+  </si>
+  <si>
+    <t>subset pval</t>
+  </si>
+  <si>
+    <t>up pval=0.0882</t>
   </si>
 </sst>
 </file>
@@ -7490,7 +7523,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -7542,15 +7631,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD8D8D8"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
+          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -7574,7 +7655,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -7590,7 +7679,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -7598,7 +7687,39 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -7896,7 +8017,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17118,13 +17239,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:N75"/>
+      <selection pane="bottomRight" activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17136,7 +17257,7 @@
     <col min="14" max="14" width="20.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>1934</v>
       </c>
@@ -17159,13 +17280,13 @@
         <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>2436</v>
+        <v>2444</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>954</v>
       </c>
       <c r="J1" t="s">
-        <v>2437</v>
+        <v>2445</v>
       </c>
       <c r="K1" t="s">
         <v>955</v>
@@ -17182,101 +17303,137 @@
       <c r="O1" t="s">
         <v>2435</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="P1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>1933</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D2" s="13">
-        <v>1397</v>
+        <v>16705</v>
       </c>
       <c r="E2" s="13">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="F2" s="13">
-        <v>6.73</v>
+        <v>80.459999999999994</v>
       </c>
       <c r="G2" s="13">
-        <v>8.3400000000000002E-3</v>
+        <v>4.13E-3</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>934</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="J2" t="s">
         <v>931</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>933</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="P2" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="13" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D3" s="13">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="G3" s="13">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1910</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1911</v>
-      </c>
-      <c r="D3">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>0.17</v>
-      </c>
-      <c r="G3">
-        <v>6.6699999999999997E-3</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="J3" t="s">
-        <v>931</v>
-      </c>
+      <c r="K3" s="13"/>
       <c r="L3" s="15" t="s">
         <v>933</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="M3" s="13"/>
+      <c r="N3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1912</v>
+        <v>1933</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1913</v>
-      </c>
-      <c r="D4">
-        <v>53</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G4">
-        <v>6.7499999999999999E-3</v>
+        <v>38</v>
+      </c>
+      <c r="D4" s="13">
+        <v>15584</v>
+      </c>
+      <c r="E4" s="13">
+        <v>120</v>
+      </c>
+      <c r="F4" s="13">
+        <v>75.06</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>933</v>
@@ -17284,109 +17441,131 @@
       <c r="J4" t="s">
         <v>931</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T4" s="15" t="s">
         <v>933</v>
       </c>
-      <c r="N4" s="17" t="s">
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D5">
+        <v>1495</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>7.52</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7.0000000000000005E-8</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J5" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="13" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>1929</v>
-      </c>
-      <c r="D5" s="13">
-        <v>18</v>
-      </c>
-      <c r="E5" s="13">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="G5" s="13">
-        <v>2.3E-3</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>931</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>933</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="L5" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>1933</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="13">
-        <v>2007</v>
+        <v>20227</v>
       </c>
       <c r="E6" s="13">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="F6" s="13">
-        <v>9.67</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>933</v>
+        <v>97.42</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1.4E-8</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>931</v>
       </c>
       <c r="J6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>2438</v>
-      </c>
       <c r="N6" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>2439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>2436</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>1933</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D7" s="13">
-        <v>6883</v>
+        <v>5027</v>
       </c>
       <c r="E7" s="13">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F7" s="13">
-        <v>33.15</v>
+        <v>24.21</v>
       </c>
       <c r="G7" s="14">
-        <v>8.9000000000000004E-13</v>
+        <v>2.0999999999999998E-15</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>933</v>
@@ -17394,34 +17573,46 @@
       <c r="J7" t="s">
         <v>931</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="X7" s="13" t="s">
         <v>2438</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>1933</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>937</v>
+        <v>6</v>
       </c>
       <c r="D8" s="13">
-        <v>11</v>
+        <v>5610</v>
       </c>
       <c r="E8" s="13">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="F8" s="13">
-        <v>0.05</v>
+        <v>27.02</v>
       </c>
       <c r="G8" s="14">
-        <v>1.0000000000000001E-5</v>
+        <v>6.2999999999999998E-15</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>933</v>
@@ -17429,34 +17620,43 @@
       <c r="J8" t="s">
         <v>931</v>
       </c>
-      <c r="L8" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N8" s="17" t="s">
+      <c r="L8" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="N8" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>1933</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>938</v>
+        <v>8</v>
       </c>
       <c r="D9" s="13">
-        <v>16</v>
+        <v>7650</v>
       </c>
       <c r="E9" s="13">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F9" s="13">
-        <v>0.08</v>
+        <v>36.840000000000003</v>
       </c>
       <c r="G9" s="14">
-        <v>4.5000000000000003E-5</v>
+        <v>3.6999999999999999E-13</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>933</v>
@@ -17464,34 +17664,43 @@
       <c r="J9" t="s">
         <v>931</v>
       </c>
-      <c r="L9" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N9" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="N9" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R9" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>1933</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D10" s="13">
-        <v>15584</v>
+        <v>6883</v>
       </c>
       <c r="E10" s="13">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="F10" s="13">
-        <v>75.06</v>
-      </c>
-      <c r="G10" s="13">
-        <v>1.4999999999999999E-4</v>
+        <v>33.15</v>
+      </c>
+      <c r="G10" s="14">
+        <v>8.9000000000000004E-13</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>933</v>
@@ -17500,74 +17709,86 @@
         <v>931</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>2438</v>
+        <v>2436</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>2440</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>2436</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R10" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>1933</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>948</v>
       </c>
       <c r="D11" s="13">
-        <v>16705</v>
+        <v>5574</v>
       </c>
       <c r="E11" s="13">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="F11" s="13">
-        <v>80.459999999999994</v>
-      </c>
-      <c r="G11" s="13">
-        <v>4.13E-3</v>
+        <v>26.85</v>
+      </c>
+      <c r="G11" s="14">
+        <v>3.2000000000000001E-12</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="J11" t="s">
         <v>931</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="L11" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T11" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1920</v>
+        <v>1933</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1921</v>
-      </c>
-      <c r="D12">
-        <v>1495</v>
-      </c>
-      <c r="E12">
-        <v>21</v>
-      </c>
-      <c r="F12">
-        <v>7.52</v>
-      </c>
-      <c r="G12" s="1">
-        <v>7.0000000000000005E-8</v>
+        <v>13</v>
+      </c>
+      <c r="D12" s="13">
+        <v>590</v>
+      </c>
+      <c r="E12" s="13">
+        <v>28</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2.84</v>
+      </c>
+      <c r="G12" s="14">
+        <v>7.5E-10</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>933</v>
@@ -17575,34 +17796,43 @@
       <c r="J12" t="s">
         <v>931</v>
       </c>
-      <c r="L12" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="L12" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1876</v>
+        <v>1933</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D13">
-        <v>2318</v>
-      </c>
-      <c r="E13">
-        <v>33</v>
-      </c>
-      <c r="F13">
-        <v>12.17</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>15</v>
+      </c>
+      <c r="D13" s="13">
+        <v>8498</v>
+      </c>
+      <c r="E13" s="13">
+        <v>94</v>
+      </c>
+      <c r="F13" s="13">
+        <v>40.93</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2.2999999999999999E-9</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>933</v>
@@ -17610,110 +17840,131 @@
       <c r="J13" t="s">
         <v>931</v>
       </c>
-      <c r="L13" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="L13" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R13" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1880</v>
+        <v>1933</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1881</v>
-      </c>
-      <c r="D14">
-        <v>1985</v>
-      </c>
-      <c r="E14">
-        <v>35</v>
-      </c>
-      <c r="F14">
-        <v>10.42</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6.4000000000000001E-7</v>
+        <v>17</v>
+      </c>
+      <c r="D14" s="13">
+        <v>9084</v>
+      </c>
+      <c r="E14" s="13">
+        <v>94</v>
+      </c>
+      <c r="F14" s="13">
+        <v>43.75</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2.7999999999999998E-9</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>1824</v>
-      </c>
       <c r="J14" t="s">
         <v>931</v>
       </c>
-      <c r="L14" s="16" t="s">
-        <v>2438</v>
+      <c r="L14" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>2436</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T14" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1886</v>
+        <v>1933</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1887</v>
-      </c>
-      <c r="D15">
-        <v>3056</v>
-      </c>
-      <c r="E15">
-        <v>42</v>
-      </c>
-      <c r="F15">
-        <v>16.04</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1.1E-5</v>
+        <v>21</v>
+      </c>
+      <c r="D15" s="13">
+        <v>10620</v>
+      </c>
+      <c r="E15" s="13">
+        <v>104</v>
+      </c>
+      <c r="F15" s="13">
+        <v>51.15</v>
+      </c>
+      <c r="G15" s="14">
+        <v>5.1E-8</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>1823</v>
-      </c>
       <c r="J15" t="s">
         <v>931</v>
       </c>
-      <c r="L15" s="16" t="s">
-        <v>2438</v>
+      <c r="L15" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+        <v>2436</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R15" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T15" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1892</v>
+        <v>1933</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1893</v>
-      </c>
-      <c r="D16">
-        <v>3492</v>
-      </c>
-      <c r="E16">
-        <v>42</v>
-      </c>
-      <c r="F16">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4.8000000000000001E-5</v>
+        <v>936</v>
+      </c>
+      <c r="D16" s="13">
+        <v>3882</v>
+      </c>
+      <c r="E16" s="13">
+        <v>43</v>
+      </c>
+      <c r="F16" s="13">
+        <v>18.7</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>933</v>
@@ -17721,34 +17972,43 @@
       <c r="J16" t="s">
         <v>931</v>
       </c>
-      <c r="L16" s="16" t="s">
-        <v>2438</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="L16" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R16" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T16" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>1933</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D17" s="13">
-        <v>5027</v>
+        <v>8663</v>
       </c>
       <c r="E17" s="13">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F17" s="13">
-        <v>24.21</v>
+        <v>41.72</v>
       </c>
       <c r="G17" s="14">
-        <v>2.0999999999999998E-15</v>
+        <v>2.7000000000000001E-7</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>933</v>
@@ -17759,31 +18019,40 @@
       <c r="L17" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N17" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="N17" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T17" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>1933</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D18" s="13">
-        <v>5610</v>
+        <v>20735</v>
       </c>
       <c r="E18" s="13">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="F18" s="13">
-        <v>27.02</v>
+        <v>99.87</v>
       </c>
       <c r="G18" s="14">
-        <v>6.2999999999999998E-15</v>
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>933</v>
@@ -17795,30 +18064,39 @@
         <v>931</v>
       </c>
       <c r="N18" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R18" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T18" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>1933</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D19" s="13">
-        <v>7650</v>
+        <v>16463</v>
       </c>
       <c r="E19" s="13">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F19" s="13">
-        <v>36.840000000000003</v>
+        <v>79.290000000000006</v>
       </c>
       <c r="G19" s="14">
-        <v>3.6999999999999999E-13</v>
+        <v>9.1999999999999998E-7</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>933</v>
@@ -17830,30 +18108,39 @@
         <v>931</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R19" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>1933</v>
       </c>
       <c r="B20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="D20" s="13">
         <v>11</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>948</v>
-      </c>
-      <c r="D20" s="13">
-        <v>5574</v>
-      </c>
       <c r="E20" s="13">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="F20" s="13">
-        <v>26.85</v>
+        <v>0.05</v>
       </c>
       <c r="G20" s="14">
-        <v>3.2000000000000001E-12</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>933</v>
@@ -17861,34 +18148,43 @@
       <c r="J20" t="s">
         <v>931</v>
       </c>
-      <c r="L20" s="17" t="s">
+      <c r="L20" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N20" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N20" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="P20" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R20" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T20" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>1933</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D21" s="13">
-        <v>590</v>
+        <v>11611</v>
       </c>
       <c r="E21" s="13">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="F21" s="13">
-        <v>2.84</v>
+        <v>55.92</v>
       </c>
       <c r="G21" s="14">
-        <v>7.5E-10</v>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>933</v>
@@ -17902,28 +18198,37 @@
       <c r="N21" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="P21" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R21" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T21" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>1933</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D22" s="13">
-        <v>8498</v>
+        <v>1792</v>
       </c>
       <c r="E22" s="13">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="F22" s="13">
-        <v>40.93</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="G22" s="14">
-        <v>2.2999999999999999E-9</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>933</v>
@@ -17931,34 +18236,43 @@
       <c r="J22" t="s">
         <v>931</v>
       </c>
-      <c r="L22" s="17" t="s">
-        <v>931</v>
-      </c>
       <c r="N22" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="P22" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T22" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U22" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>1933</v>
       </c>
       <c r="B23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>938</v>
+      </c>
+      <c r="D23" s="13">
         <v>16</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="13">
-        <v>9084</v>
-      </c>
       <c r="E23" s="13">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="F23" s="13">
-        <v>43.75</v>
+        <v>0.08</v>
       </c>
       <c r="G23" s="14">
-        <v>2.7999999999999998E-9</v>
+        <v>4.5000000000000003E-5</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>933</v>
@@ -17966,34 +18280,43 @@
       <c r="J23" t="s">
         <v>931</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N23" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N23" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="P23" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T23" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>1933</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D24" s="13">
-        <v>10620</v>
+        <v>18</v>
       </c>
       <c r="E24" s="13">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="F24" s="13">
-        <v>51.15</v>
-      </c>
-      <c r="G24" s="14">
-        <v>5.1E-8</v>
+        <v>0.09</v>
+      </c>
+      <c r="G24" s="13">
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>933</v>
@@ -18004,31 +18327,40 @@
       <c r="L24" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N24" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="N24" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T24" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>1933</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>936</v>
+        <v>40</v>
       </c>
       <c r="D25" s="13">
-        <v>3882</v>
+        <v>286</v>
       </c>
       <c r="E25" s="13">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F25" s="13">
-        <v>18.7</v>
-      </c>
-      <c r="G25" s="14">
-        <v>1.4000000000000001E-7</v>
+        <v>1.38</v>
+      </c>
+      <c r="G25" s="13">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>933</v>
@@ -18039,31 +18371,43 @@
       <c r="L25" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N25" s="17" t="s">
+      <c r="N25" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R25" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="S25" t="s">
+        <v>2441</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>1933</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D26" s="13">
-        <v>8663</v>
+        <v>53</v>
       </c>
       <c r="E26" s="13">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="F26" s="13">
-        <v>41.72</v>
-      </c>
-      <c r="G26" s="14">
-        <v>2.7000000000000001E-7</v>
+        <v>0.26</v>
+      </c>
+      <c r="G26" s="13">
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>933</v>
@@ -18077,28 +18421,37 @@
       <c r="N26" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="P26" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T26" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>1933</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D27" s="13">
-        <v>20735</v>
+        <v>484</v>
       </c>
       <c r="E27" s="13">
-        <v>132</v>
+        <v>8</v>
       </c>
       <c r="F27" s="13">
-        <v>99.87</v>
-      </c>
-      <c r="G27" s="14">
-        <v>5.6000000000000004E-7</v>
+        <v>2.33</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1.48E-3</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>933</v>
@@ -18109,31 +18462,40 @@
       <c r="L27" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N27" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="N27" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T27" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>1933</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D28" s="13">
-        <v>16463</v>
+        <v>53</v>
       </c>
       <c r="E28" s="13">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="F28" s="13">
-        <v>79.290000000000006</v>
-      </c>
-      <c r="G28" s="14">
-        <v>9.1999999999999998E-7</v>
+        <v>0.26</v>
+      </c>
+      <c r="G28" s="13">
+        <v>2.16E-3</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>933</v>
@@ -18144,31 +18506,40 @@
       <c r="L28" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N28" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="N28" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T28" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>1933</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>31</v>
+        <v>939</v>
       </c>
       <c r="D29" s="13">
-        <v>11611</v>
+        <v>53</v>
       </c>
       <c r="E29" s="13">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="F29" s="13">
-        <v>55.92</v>
-      </c>
-      <c r="G29" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>0.26</v>
+      </c>
+      <c r="G29" s="13">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>933</v>
@@ -18182,28 +18553,37 @@
       <c r="N29" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="P29" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T29" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>1933</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>36</v>
+        <v>949</v>
       </c>
       <c r="D30" s="13">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="E30" s="13">
         <v>3</v>
       </c>
       <c r="F30" s="13">
-        <v>0.09</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G30" s="13">
-        <v>1.3999999999999999E-4</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>933</v>
@@ -18217,28 +18597,37 @@
       <c r="N30" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="P30" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R30" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T30" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>1933</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D31" s="13">
-        <v>286</v>
+        <v>118</v>
       </c>
       <c r="E31" s="13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F31" s="13">
-        <v>1.38</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G31" s="13">
-        <v>5.0000000000000001E-4</v>
+        <v>7.0499999999999998E-3</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>933</v>
@@ -18249,34 +18638,46 @@
       <c r="L31" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N31" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="N31" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T31" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>1933</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D32" s="13">
-        <v>53</v>
+        <v>250</v>
       </c>
       <c r="E32" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F32" s="13">
-        <v>0.26</v>
+        <v>1.2</v>
       </c>
       <c r="G32" s="13">
-        <v>9.3000000000000005E-4</v>
+        <v>8.0599999999999995E-3</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>943</v>
       </c>
       <c r="J32" t="s">
         <v>931</v>
@@ -18287,28 +18688,37 @@
       <c r="N32" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R32" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T32" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>1933</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D33" s="13">
-        <v>484</v>
+        <v>2007</v>
       </c>
       <c r="E33" s="13">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="F33" s="13">
-        <v>2.33</v>
-      </c>
-      <c r="G33" s="13">
-        <v>1.48E-3</v>
+        <v>9.67</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>933</v>
@@ -18316,34 +18726,43 @@
       <c r="J33" t="s">
         <v>931</v>
       </c>
-      <c r="L33" s="17" t="s">
+      <c r="L33" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N33" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R33" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N33" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="T33" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>45</v>
+        <v>1931</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1856</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="13">
-        <v>53</v>
-      </c>
-      <c r="E34" s="13">
-        <v>3</v>
-      </c>
-      <c r="F34" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G34" s="13">
-        <v>2.16E-3</v>
+        <v>1857</v>
+      </c>
+      <c r="D34">
+        <v>3016</v>
+      </c>
+      <c r="E34">
+        <v>80</v>
+      </c>
+      <c r="F34">
+        <v>15.83</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3.4000000000000001E-28</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>933</v>
@@ -18354,31 +18773,40 @@
       <c r="L34" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N34" s="17" t="s">
+      <c r="N34" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R34" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="T34" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>47</v>
+        <v>1931</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1858</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>939</v>
-      </c>
-      <c r="D35" s="13">
-        <v>53</v>
-      </c>
-      <c r="E35" s="13">
-        <v>3</v>
-      </c>
-      <c r="F35" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G35" s="13">
-        <v>2.5000000000000001E-3</v>
+        <v>1859</v>
+      </c>
+      <c r="D35">
+        <v>3016</v>
+      </c>
+      <c r="E35">
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <v>15.83</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3.5E-28</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>933</v>
@@ -18389,31 +18817,40 @@
       <c r="L35" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N35" s="17" t="s">
+      <c r="N35" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R35" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="T35" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>52</v>
+        <v>1931</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1860</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>949</v>
-      </c>
-      <c r="D36" s="13">
-        <v>118</v>
-      </c>
-      <c r="E36" s="13">
-        <v>3</v>
-      </c>
-      <c r="F36" s="13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G36" s="13">
-        <v>5.4999999999999997E-3</v>
+        <v>1861</v>
+      </c>
+      <c r="D36">
+        <v>5431</v>
+      </c>
+      <c r="E36">
+        <v>89</v>
+      </c>
+      <c r="F36">
+        <v>28.51</v>
+      </c>
+      <c r="G36" s="1">
+        <v>5.5000000000000005E-26</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>933</v>
@@ -18424,31 +18861,40 @@
       <c r="L36" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N36" s="17" t="s">
+      <c r="N36" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R36" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="T36" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>53</v>
+        <v>1931</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1862</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="13">
-        <v>118</v>
-      </c>
-      <c r="E37" s="13">
-        <v>3</v>
-      </c>
-      <c r="F37" s="13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G37" s="13">
-        <v>7.0499999999999998E-3</v>
+        <v>1863</v>
+      </c>
+      <c r="D37">
+        <v>10580</v>
+      </c>
+      <c r="E37">
+        <v>114</v>
+      </c>
+      <c r="F37">
+        <v>55.55</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1.8000000000000001E-19</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>933</v>
@@ -18459,37 +18905,43 @@
       <c r="L37" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N37" s="17" t="s">
+      <c r="N37" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R37" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="T37" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>57</v>
+        <v>1931</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1864</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="13">
-        <v>250</v>
-      </c>
-      <c r="E38" s="13">
-        <v>4</v>
-      </c>
-      <c r="F38" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="G38" s="13">
-        <v>8.0599999999999995E-3</v>
+        <v>1865</v>
+      </c>
+      <c r="D38">
+        <v>5893</v>
+      </c>
+      <c r="E38">
+        <v>85</v>
+      </c>
+      <c r="F38">
+        <v>30.94</v>
+      </c>
+      <c r="G38" s="1">
+        <v>6.4999999999999996E-13</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="J38" t="s">
         <v>931</v>
@@ -18497,31 +18949,40 @@
       <c r="L38" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N38" s="17" t="s">
+      <c r="N38" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P38" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R38" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="T38" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B39" t="s">
-        <v>1916</v>
+        <v>1866</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1917</v>
+        <v>1867</v>
       </c>
       <c r="D39">
-        <v>1722</v>
+        <v>20261</v>
       </c>
       <c r="E39">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="F39">
-        <v>8.66</v>
-      </c>
-      <c r="G39" t="s">
-        <v>2</v>
+        <v>106.37</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1.1E-12</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>933</v>
@@ -18533,30 +18994,39 @@
         <v>931</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P39" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R39" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T39" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B40" t="s">
-        <v>1918</v>
+        <v>1868</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1919</v>
+        <v>1869</v>
       </c>
       <c r="D40">
-        <v>1357</v>
+        <v>10569</v>
       </c>
       <c r="E40">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="F40">
-        <v>6.82</v>
+        <v>55.49</v>
       </c>
       <c r="G40" s="1">
-        <v>2.4E-8</v>
+        <v>1.3E-11</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>933</v>
@@ -18567,31 +19037,43 @@
       <c r="L40" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N40" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="13" customFormat="1">
+      <c r="N40" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="O40" s="13"/>
+      <c r="P40" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R40" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="S40" s="13"/>
+      <c r="T40" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U40" s="13"/>
+    </row>
+    <row r="41" spans="1:21" s="13" customFormat="1">
       <c r="A41" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B41" t="s">
-        <v>1922</v>
+        <v>1870</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1923</v>
+        <v>1871</v>
       </c>
       <c r="D41">
-        <v>42</v>
+        <v>1115</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F41">
-        <v>0.21</v>
+        <v>5.85</v>
       </c>
       <c r="G41" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>2.9000000000000002E-8</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>933</v>
@@ -18604,31 +19086,44 @@
         <v>931</v>
       </c>
       <c r="M41"/>
-      <c r="N41" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="N41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="O41"/>
+      <c r="P41" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="Q41"/>
+      <c r="R41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="S41"/>
+      <c r="T41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U41"/>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B42" t="s">
-        <v>1924</v>
+        <v>1872</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1925</v>
+        <v>1873</v>
       </c>
       <c r="D42">
-        <v>42</v>
+        <v>1411</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F42">
-        <v>0.21</v>
+        <v>7.41</v>
       </c>
       <c r="G42" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>933</v>
@@ -18639,31 +19134,40 @@
       <c r="L42" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N42" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="N42" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T42" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B43" t="s">
-        <v>1926</v>
+        <v>1876</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1927</v>
+        <v>1877</v>
       </c>
       <c r="D43">
-        <v>42</v>
+        <v>2318</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F43">
-        <v>0.21</v>
+        <v>12.17</v>
       </c>
       <c r="G43" s="1">
-        <v>4.3999999999999999E-5</v>
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>933</v>
@@ -18671,34 +19175,43 @@
       <c r="J43" t="s">
         <v>931</v>
       </c>
-      <c r="L43" s="17" t="s">
+      <c r="L43" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R43" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N43" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="T43" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>1931</v>
       </c>
       <c r="B44" t="s">
-        <v>1848</v>
+        <v>1874</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1849</v>
+        <v>1875</v>
       </c>
       <c r="D44">
-        <v>1151</v>
+        <v>2318</v>
       </c>
       <c r="E44">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="F44">
-        <v>6.04</v>
-      </c>
-      <c r="G44" t="s">
-        <v>2</v>
+        <v>12.17</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>933</v>
@@ -18710,30 +19223,39 @@
         <v>931</v>
       </c>
       <c r="N44" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P44" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R44" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T44" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>1931</v>
       </c>
       <c r="B45" t="s">
-        <v>1850</v>
+        <v>1878</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1851</v>
+        <v>1879</v>
       </c>
       <c r="D45">
-        <v>1066</v>
+        <v>23508</v>
       </c>
       <c r="E45">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="F45">
-        <v>5.6</v>
-      </c>
-      <c r="G45" t="s">
-        <v>2</v>
+        <v>123.42</v>
+      </c>
+      <c r="G45" s="1">
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>933</v>
@@ -18745,30 +19267,39 @@
         <v>931</v>
       </c>
       <c r="N45" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P45" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R45" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T45" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>1931</v>
       </c>
       <c r="B46" t="s">
-        <v>1852</v>
+        <v>1882</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1853</v>
+        <v>1883</v>
       </c>
       <c r="D46">
-        <v>1767</v>
+        <v>11959</v>
       </c>
       <c r="E46">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="F46">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="G46" t="s">
-        <v>2</v>
+        <v>62.79</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1.1999999999999999E-6</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>933</v>
@@ -18779,31 +19310,40 @@
       <c r="L46" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N46" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="N46" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P46" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R46" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T46" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>1931</v>
       </c>
       <c r="B47" t="s">
-        <v>1854</v>
+        <v>1884</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1855</v>
+        <v>1885</v>
       </c>
       <c r="D47">
-        <v>1595</v>
+        <v>23774</v>
       </c>
       <c r="E47">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="F47">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="G47" t="s">
-        <v>2</v>
+        <v>124.82</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2.3999999999999999E-6</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>933</v>
@@ -18815,30 +19355,39 @@
         <v>931</v>
       </c>
       <c r="N47" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R47" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T47" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>1931</v>
       </c>
       <c r="B48" t="s">
-        <v>1856</v>
+        <v>1888</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>1857</v>
+        <v>1889</v>
       </c>
       <c r="D48">
-        <v>3016</v>
+        <v>27911</v>
       </c>
       <c r="E48">
-        <v>80</v>
+        <v>166</v>
       </c>
       <c r="F48">
-        <v>15.83</v>
+        <v>146.54</v>
       </c>
       <c r="G48" s="1">
-        <v>3.4000000000000001E-28</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>933</v>
@@ -18850,30 +19399,39 @@
         <v>931</v>
       </c>
       <c r="N48" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P48" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R48" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T48" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>1931</v>
       </c>
       <c r="B49" t="s">
-        <v>1858</v>
+        <v>1890</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1859</v>
+        <v>1891</v>
       </c>
       <c r="D49">
-        <v>3016</v>
+        <v>27911</v>
       </c>
       <c r="E49">
-        <v>80</v>
+        <v>166</v>
       </c>
       <c r="F49">
-        <v>15.83</v>
+        <v>146.54</v>
       </c>
       <c r="G49" s="1">
-        <v>3.5E-28</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>933</v>
@@ -18885,100 +19443,127 @@
         <v>931</v>
       </c>
       <c r="N49" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P49" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R49" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>1931</v>
       </c>
       <c r="B50" t="s">
-        <v>1860</v>
+        <v>1902</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1861</v>
+        <v>1903</v>
       </c>
       <c r="D50">
-        <v>5431</v>
+        <v>361</v>
       </c>
       <c r="E50">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="F50">
-        <v>28.51</v>
-      </c>
-      <c r="G50" s="1">
-        <v>5.5000000000000005E-26</v>
+        <v>1.9</v>
+      </c>
+      <c r="G50">
+        <v>3.8800000000000002E-3</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J50" t="s">
-        <v>931</v>
+        <v>1827</v>
       </c>
       <c r="L50" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N50" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="N50" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P50" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R50" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T50" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" t="s">
         <v>1931</v>
       </c>
       <c r="B51" t="s">
-        <v>1862</v>
+        <v>1904</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1863</v>
+        <v>1905</v>
       </c>
       <c r="D51">
-        <v>10580</v>
+        <v>361</v>
       </c>
       <c r="E51">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="F51">
-        <v>55.55</v>
-      </c>
-      <c r="G51" s="1">
-        <v>1.8000000000000001E-19</v>
+        <v>1.9</v>
+      </c>
+      <c r="G51">
+        <v>4.13E-3</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J51" t="s">
-        <v>931</v>
+        <v>1826</v>
       </c>
       <c r="L51" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N51" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="N51" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P51" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R51" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T51" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
       <c r="A52" t="s">
         <v>1931</v>
       </c>
       <c r="B52" t="s">
-        <v>1864</v>
+        <v>1906</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>1865</v>
+        <v>1907</v>
       </c>
       <c r="D52">
-        <v>5893</v>
+        <v>32</v>
       </c>
       <c r="E52">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="F52">
-        <v>30.94</v>
-      </c>
-      <c r="G52" s="1">
-        <v>6.4999999999999996E-13</v>
+        <v>0.17</v>
+      </c>
+      <c r="G52">
+        <v>4.8300000000000001E-3</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>933</v>
@@ -18989,31 +19574,40 @@
       <c r="L52" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N52" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="N52" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P52" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R52" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T52" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>1866</v>
+        <v>1908</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1867</v>
+        <v>1909</v>
       </c>
       <c r="D53">
-        <v>20261</v>
+        <v>20703</v>
       </c>
       <c r="E53">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F53">
-        <v>106.37</v>
-      </c>
-      <c r="G53" s="1">
-        <v>1.1E-12</v>
+        <v>108.69</v>
+      </c>
+      <c r="G53">
+        <v>5.6499999999999996E-3</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>933</v>
@@ -19024,31 +19618,40 @@
       <c r="L53" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N53" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="N53" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P53" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R53" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54" t="s">
         <v>1931</v>
       </c>
       <c r="B54" t="s">
-        <v>1868</v>
+        <v>1910</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>1869</v>
+        <v>1911</v>
       </c>
       <c r="D54">
-        <v>10569</v>
+        <v>32</v>
       </c>
       <c r="E54">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="F54">
-        <v>55.49</v>
-      </c>
-      <c r="G54" s="1">
-        <v>1.3E-11</v>
+        <v>0.17</v>
+      </c>
+      <c r="G54">
+        <v>6.6699999999999997E-3</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>933</v>
@@ -19056,34 +19659,46 @@
       <c r="J54" t="s">
         <v>931</v>
       </c>
-      <c r="L54" s="17" t="s">
-        <v>931</v>
+      <c r="L54" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="N54" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="P54" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R54" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T54" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U54" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
       <c r="A55" t="s">
         <v>1931</v>
       </c>
       <c r="B55" t="s">
-        <v>1870</v>
+        <v>1848</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1871</v>
+        <v>1849</v>
       </c>
       <c r="D55">
-        <v>1115</v>
+        <v>1151</v>
       </c>
       <c r="E55">
         <v>69</v>
       </c>
       <c r="F55">
-        <v>5.85</v>
-      </c>
-      <c r="G55" s="1">
-        <v>2.9000000000000002E-8</v>
+        <v>6.04</v>
+      </c>
+      <c r="G55" t="s">
+        <v>2</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>933</v>
@@ -19094,31 +19709,40 @@
       <c r="L55" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N55" s="17" t="s">
+      <c r="N55" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P55" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R55" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="T55" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
       <c r="A56" t="s">
         <v>1931</v>
       </c>
       <c r="B56" t="s">
-        <v>1872</v>
+        <v>1850</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>1873</v>
+        <v>1851</v>
       </c>
       <c r="D56">
-        <v>1411</v>
+        <v>1066</v>
       </c>
       <c r="E56">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F56">
-        <v>7.41</v>
-      </c>
-      <c r="G56" s="1">
-        <v>1.1000000000000001E-7</v>
+        <v>5.6</v>
+      </c>
+      <c r="G56" t="s">
+        <v>2</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>933</v>
@@ -19129,31 +19753,40 @@
       <c r="L56" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N56" s="17" t="s">
+      <c r="N56" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P56" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R56" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="T56" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
       <c r="A57" t="s">
         <v>1931</v>
       </c>
       <c r="B57" t="s">
-        <v>1874</v>
+        <v>1852</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>1875</v>
+        <v>1853</v>
       </c>
       <c r="D57">
-        <v>2318</v>
+        <v>1767</v>
       </c>
       <c r="E57">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F57">
-        <v>12.17</v>
-      </c>
-      <c r="G57" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="G57" t="s">
+        <v>2</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>933</v>
@@ -19165,30 +19798,39 @@
         <v>931</v>
       </c>
       <c r="N57" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P57" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R57" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T57" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
       <c r="A58" t="s">
         <v>1931</v>
       </c>
       <c r="B58" t="s">
-        <v>1878</v>
+        <v>1854</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>1879</v>
+        <v>1855</v>
       </c>
       <c r="D58">
-        <v>23508</v>
+        <v>1595</v>
       </c>
       <c r="E58">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="F58">
-        <v>123.42</v>
-      </c>
-      <c r="G58" s="1">
-        <v>5.6000000000000004E-7</v>
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="G58" t="s">
+        <v>2</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>933</v>
@@ -19200,30 +19842,39 @@
         <v>931</v>
       </c>
       <c r="N58" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P58" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R58" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T58" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
       <c r="A59" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B59" t="s">
-        <v>1882</v>
+        <v>1918</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>1883</v>
+        <v>1919</v>
       </c>
       <c r="D59">
-        <v>11959</v>
+        <v>1357</v>
       </c>
       <c r="E59">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F59">
-        <v>62.79</v>
+        <v>6.82</v>
       </c>
       <c r="G59" s="1">
-        <v>1.1999999999999999E-6</v>
+        <v>2.4E-8</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>933</v>
@@ -19234,31 +19885,40 @@
       <c r="L59" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N59" s="17" t="s">
+      <c r="N59" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R59" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="T59" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
       <c r="A60" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B60" t="s">
-        <v>1884</v>
+        <v>1916</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>1885</v>
+        <v>1917</v>
       </c>
       <c r="D60">
-        <v>23774</v>
+        <v>1722</v>
       </c>
       <c r="E60">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="F60">
-        <v>124.82</v>
-      </c>
-      <c r="G60" s="1">
-        <v>2.3999999999999999E-6</v>
+        <v>8.66</v>
+      </c>
+      <c r="G60" t="s">
+        <v>2</v>
       </c>
       <c r="H60" s="9" t="s">
         <v>933</v>
@@ -19270,115 +19930,151 @@
         <v>931</v>
       </c>
       <c r="N60" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P60" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R60" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T60" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
       <c r="A61" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1888</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>1889</v>
-      </c>
-      <c r="D61">
-        <v>27911</v>
-      </c>
-      <c r="E61">
-        <v>166</v>
-      </c>
-      <c r="F61">
-        <v>146.54</v>
-      </c>
-      <c r="G61" s="1">
-        <v>1.8E-5</v>
-      </c>
-      <c r="H61" s="9" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="13">
+        <v>33</v>
+      </c>
+      <c r="E61" s="13">
+        <v>2</v>
+      </c>
+      <c r="F61" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="G61" s="13">
+        <v>4.3899999999999998E-3</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J61" t="s">
         <v>933</v>
-      </c>
-      <c r="J61" t="s">
-        <v>931</v>
       </c>
       <c r="L61" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N61" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="N61" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P61" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="R61" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T61" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
       <c r="A62" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1890</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>1891</v>
-      </c>
-      <c r="D62">
-        <v>27911</v>
-      </c>
-      <c r="E62">
-        <v>166</v>
-      </c>
-      <c r="F62">
-        <v>146.54</v>
-      </c>
-      <c r="G62" s="1">
-        <v>1.8E-5</v>
-      </c>
-      <c r="H62" s="9" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="13">
+        <v>70</v>
+      </c>
+      <c r="E62" s="13">
+        <v>2</v>
+      </c>
+      <c r="F62" s="13">
+        <v>0.34</v>
+      </c>
+      <c r="G62" s="13">
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J62" t="s">
         <v>933</v>
-      </c>
-      <c r="J62" t="s">
-        <v>931</v>
       </c>
       <c r="L62" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N62" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="P62" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="R62" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T62" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
       <c r="A63" t="s">
         <v>1931</v>
       </c>
       <c r="B63" t="s">
-        <v>1894</v>
+        <v>1886</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>1895</v>
+        <v>1887</v>
       </c>
       <c r="D63">
-        <v>720</v>
+        <v>3056</v>
       </c>
       <c r="E63">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F63">
-        <v>3.78</v>
-      </c>
-      <c r="G63">
-        <v>1.1E-4</v>
+        <v>16.04</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1.1E-5</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I63" s="13" t="s">
+        <v>1823</v>
+      </c>
       <c r="J63" t="s">
         <v>931</v>
       </c>
-      <c r="L63" s="17" t="s">
+      <c r="L63" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N63" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P63" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="R63" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N63" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="T63" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64" t="s">
         <v>1931</v>
       </c>
@@ -19413,65 +20109,86 @@
         <v>931</v>
       </c>
       <c r="N64" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>2436</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="R64" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T64" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>1931</v>
       </c>
       <c r="B65" t="s">
-        <v>1898</v>
+        <v>1880</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>1899</v>
+        <v>1881</v>
       </c>
       <c r="D65">
-        <v>1480</v>
+        <v>1985</v>
       </c>
       <c r="E65">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F65">
-        <v>7.77</v>
-      </c>
-      <c r="G65">
-        <v>1.65E-3</v>
+        <v>10.42</v>
+      </c>
+      <c r="G65" s="1">
+        <v>6.4000000000000001E-7</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I65" s="13" t="s">
+        <v>1824</v>
+      </c>
       <c r="J65" t="s">
         <v>931</v>
       </c>
-      <c r="L65" s="17" t="s">
+      <c r="L65" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N65" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P65" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="R65" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N65" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="T65" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>1931</v>
       </c>
       <c r="B66" t="s">
-        <v>1900</v>
+        <v>1892</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1901</v>
+        <v>1893</v>
       </c>
       <c r="D66">
-        <v>20252</v>
+        <v>3492</v>
       </c>
       <c r="E66">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="F66">
-        <v>106.33</v>
-      </c>
-      <c r="G66">
-        <v>1.7700000000000001E-3</v>
+        <v>18.329999999999998</v>
+      </c>
+      <c r="G66" s="1">
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>933</v>
@@ -19479,40 +20196,49 @@
       <c r="J66" t="s">
         <v>931</v>
       </c>
-      <c r="L66" s="17" t="s">
+      <c r="L66" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N66" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R66" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N66" s="17" t="s">
+      <c r="T66" s="17" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>1931</v>
       </c>
       <c r="B67" t="s">
-        <v>1902</v>
+        <v>1894</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>1903</v>
+        <v>1895</v>
       </c>
       <c r="D67">
-        <v>361</v>
+        <v>720</v>
       </c>
       <c r="E67">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F67">
-        <v>1.9</v>
+        <v>3.78</v>
       </c>
       <c r="G67">
-        <v>3.8800000000000002E-3</v>
+        <v>1.1E-4</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J67" t="s">
-        <v>1827</v>
+        <v>931</v>
       </c>
       <c r="L67" s="17" t="s">
         <v>931</v>
@@ -19520,34 +20246,46 @@
       <c r="N67" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="P67" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R67" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="S67" t="s">
+        <v>2442</v>
+      </c>
+      <c r="T67" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>1931</v>
       </c>
       <c r="B68" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1905</v>
+        <v>1899</v>
       </c>
       <c r="D68">
-        <v>361</v>
+        <v>1480</v>
       </c>
       <c r="E68">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F68">
-        <v>1.9</v>
+        <v>7.77</v>
       </c>
       <c r="G68">
-        <v>4.13E-3</v>
+        <v>1.65E-3</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J68" t="s">
-        <v>1826</v>
+        <v>931</v>
       </c>
       <c r="L68" s="17" t="s">
         <v>931</v>
@@ -19555,28 +20293,37 @@
       <c r="N68" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="P68" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R68" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T68" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>1931</v>
       </c>
       <c r="B69" t="s">
-        <v>1906</v>
+        <v>1900</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>1907</v>
+        <v>1901</v>
       </c>
       <c r="D69">
-        <v>32</v>
+        <v>20252</v>
       </c>
       <c r="E69">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="F69">
-        <v>0.17</v>
+        <v>106.33</v>
       </c>
       <c r="G69">
-        <v>4.8300000000000001E-3</v>
+        <v>1.7700000000000001E-3</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>933</v>
@@ -19590,28 +20337,37 @@
       <c r="N69" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="P69" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="R69" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T69" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>1931</v>
       </c>
       <c r="B70" t="s">
-        <v>1908</v>
+        <v>1914</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1909</v>
+        <v>1915</v>
       </c>
       <c r="D70">
-        <v>20703</v>
+        <v>19850</v>
       </c>
       <c r="E70">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F70">
-        <v>108.69</v>
+        <v>104.21</v>
       </c>
       <c r="G70">
-        <v>5.6499999999999996E-3</v>
+        <v>8.0300000000000007E-3</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>933</v>
@@ -19625,28 +20381,37 @@
       <c r="N70" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="P70" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R70" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T70" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>1931</v>
       </c>
       <c r="B71" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="D71">
-        <v>19850</v>
+        <v>53</v>
       </c>
       <c r="E71">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="F71">
-        <v>104.21</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G71">
-        <v>8.0300000000000007E-3</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>933</v>
@@ -19654,75 +20419,84 @@
       <c r="J71" t="s">
         <v>931</v>
       </c>
-      <c r="L71" s="17" t="s">
-        <v>931</v>
+      <c r="L71" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="N71" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="P71" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="T71" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D72" s="13">
-        <v>20227</v>
-      </c>
-      <c r="E72" s="13">
-        <v>134</v>
-      </c>
-      <c r="F72" s="13">
-        <v>97.42</v>
-      </c>
-      <c r="G72" s="14">
-        <v>1.4E-8</v>
-      </c>
-      <c r="H72" s="10" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D72">
+        <v>42</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72">
+        <v>0.21</v>
+      </c>
+      <c r="G72" s="1">
+        <v>2.5999999999999998E-5</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J72" t="s">
         <v>931</v>
-      </c>
-      <c r="J72" t="s">
-        <v>1008</v>
       </c>
       <c r="L72" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N72" s="16" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="N72" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P72" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D73" s="13">
-        <v>33</v>
-      </c>
-      <c r="E73" s="13">
-        <v>2</v>
-      </c>
-      <c r="F73" s="13">
-        <v>0.16</v>
-      </c>
-      <c r="G73" s="13">
-        <v>4.3899999999999998E-3</v>
-      </c>
-      <c r="H73" s="10" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D73">
+        <v>42</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
+      <c r="F73">
+        <v>0.21</v>
+      </c>
+      <c r="G73" s="1">
+        <v>2.5999999999999998E-5</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J73" t="s">
         <v>931</v>
-      </c>
-      <c r="J73" t="s">
-        <v>933</v>
       </c>
       <c r="L73" s="17" t="s">
         <v>931</v>
@@ -19730,76 +20504,99 @@
       <c r="N73" s="15" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="P73" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="13">
-        <v>70</v>
-      </c>
-      <c r="E74" s="13">
-        <v>2</v>
-      </c>
-      <c r="F74" s="13">
-        <v>0.34</v>
-      </c>
-      <c r="G74" s="13">
-        <v>7.3400000000000002E-3</v>
-      </c>
-      <c r="H74" s="10" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>1927</v>
+      </c>
+      <c r="D74">
+        <v>42</v>
+      </c>
+      <c r="E74">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <v>0.21</v>
+      </c>
+      <c r="G74" s="1">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J74" t="s">
         <v>931</v>
-      </c>
-      <c r="J74" t="s">
-        <v>933</v>
       </c>
       <c r="L74" s="17" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="N74" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P74" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>1933</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D75" s="13">
-        <v>1792</v>
+        <v>1397</v>
       </c>
       <c r="E75" s="13">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="F75" s="13">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="G75" s="14">
-        <v>4.0000000000000003E-5</v>
+        <v>6.73</v>
+      </c>
+      <c r="G75" s="13">
+        <v>8.3400000000000002E-3</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>942</v>
       </c>
       <c r="J75" t="s">
         <v>931</v>
       </c>
+      <c r="L75" s="15" t="s">
+        <v>933</v>
+      </c>
       <c r="N75" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="P75" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>2449</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N75">
-    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="5"/>
-    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="4"/>
-    <sortCondition sortBy="cellColor" ref="L2:L75" dxfId="3"/>
+  <sortState ref="A2:U75">
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="9"/>
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="8"/>
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="P2:P75" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="P2:P75" dxfId="5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working on nearly equal comparsions for origin sig genes.
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryOrigin" sheetId="28" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5404" uniqueCount="2452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2453">
   <si>
     <t>GO:0006412</t>
   </si>
@@ -7398,6 +7398,9 @@
   </si>
   <si>
     <t>up pval=0.0882</t>
+  </si>
+  <si>
+    <t>NE inv rel to nat, T0</t>
   </si>
 </sst>
 </file>
@@ -8014,10 +8017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8026,7 +8029,7 @@
     <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1930</v>
       </c>
@@ -8051,8 +8054,11 @@
       <c r="H1" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1933</v>
       </c>
@@ -8078,7 +8084,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1933</v>
       </c>
@@ -8104,7 +8110,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>1933</v>
       </c>
@@ -8130,7 +8136,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>1933</v>
       </c>
@@ -8156,7 +8162,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>1933</v>
       </c>
@@ -8182,7 +8188,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>1933</v>
       </c>
@@ -8208,7 +8214,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>1933</v>
       </c>
@@ -8234,7 +8240,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>1933</v>
       </c>
@@ -8260,7 +8266,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>1933</v>
       </c>
@@ -8286,7 +8292,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>1933</v>
       </c>
@@ -8312,7 +8318,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>1933</v>
       </c>
@@ -8338,7 +8344,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>1933</v>
       </c>
@@ -8364,7 +8370,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>1933</v>
       </c>
@@ -8390,7 +8396,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>1933</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>1933</v>
       </c>
@@ -17241,11 +17247,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U23" sqref="U23"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2:T75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17321,28 +17327,25 @@
         <v>1933</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="D2" s="13">
-        <v>16705</v>
+        <v>2007</v>
       </c>
       <c r="E2" s="13">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="F2" s="13">
-        <v>80.459999999999994</v>
-      </c>
-      <c r="G2" s="13">
-        <v>4.13E-3</v>
+        <v>9.67</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="J2" t="s">
         <v>931</v>
@@ -17350,67 +17353,61 @@
       <c r="L2" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>933</v>
+      <c r="N2" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13">
+        <v>5027</v>
+      </c>
+      <c r="E3" s="13">
+        <v>85</v>
+      </c>
+      <c r="F3" s="13">
+        <v>24.21</v>
+      </c>
+      <c r="G3" s="14">
+        <v>2.0999999999999998E-15</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="T2" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="13" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1929</v>
-      </c>
-      <c r="D3" s="13">
-        <v>18</v>
-      </c>
-      <c r="E3" s="13">
-        <v>3</v>
-      </c>
-      <c r="F3" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="G3" s="13">
-        <v>2.3E-3</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="J3" t="s">
         <v>931</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>933</v>
-      </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>2448</v>
-      </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>2437</v>
+      <c r="L3" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -17418,22 +17415,22 @@
         <v>1933</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D4" s="13">
-        <v>15584</v>
+        <v>5610</v>
       </c>
       <c r="E4" s="13">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="F4" s="13">
-        <v>75.06</v>
-      </c>
-      <c r="G4" s="13">
-        <v>1.4999999999999999E-4</v>
+        <v>27.02</v>
+      </c>
+      <c r="G4" s="14">
+        <v>6.2999999999999998E-15</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>933</v>
@@ -17441,8 +17438,8 @@
       <c r="J4" t="s">
         <v>931</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>2436</v>
+      <c r="L4" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N4" s="16" t="s">
         <v>2436</v>
@@ -17450,34 +17447,37 @@
       <c r="P4" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R4" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="T4" s="15" t="s">
-        <v>933</v>
+      <c r="R4" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>2437</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1920</v>
+        <v>1933</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1921</v>
-      </c>
-      <c r="D5">
-        <v>1495</v>
-      </c>
-      <c r="E5">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>7.52</v>
-      </c>
-      <c r="G5" s="1">
-        <v>7.0000000000000005E-8</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="13">
+        <v>7650</v>
+      </c>
+      <c r="E5" s="13">
+        <v>97</v>
+      </c>
+      <c r="F5" s="13">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3.6999999999999999E-13</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>933</v>
@@ -17485,8 +17485,8 @@
       <c r="J5" t="s">
         <v>931</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>2436</v>
+      <c r="L5" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2436</v>
@@ -17494,11 +17494,11 @@
       <c r="P5" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R5" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>2436</v>
+      <c r="R5" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -17506,43 +17506,43 @@
         <v>1933</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="13">
-        <v>20227</v>
+        <v>6883</v>
       </c>
       <c r="E6" s="13">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="F6" s="13">
-        <v>97.42</v>
+        <v>33.15</v>
       </c>
       <c r="G6" s="14">
-        <v>1.4E-8</v>
-      </c>
-      <c r="H6" s="10" t="s">
+        <v>8.9000000000000004E-13</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J6" t="s">
         <v>931</v>
       </c>
-      <c r="J6" t="s">
-        <v>1008</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>931</v>
+      <c r="L6" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P6" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="T6" s="16" t="s">
-        <v>2436</v>
+      <c r="P6" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -17550,22 +17550,22 @@
         <v>1933</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>4</v>
+        <v>948</v>
       </c>
       <c r="D7" s="13">
-        <v>5027</v>
+        <v>5574</v>
       </c>
       <c r="E7" s="13">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="13">
-        <v>24.21</v>
+        <v>26.85</v>
       </c>
       <c r="G7" s="14">
-        <v>2.0999999999999998E-15</v>
+        <v>3.2000000000000001E-12</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>933</v>
@@ -17587,9 +17587,6 @@
       </c>
       <c r="T7" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="X7" s="13" t="s">
-        <v>2438</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -17597,22 +17594,22 @@
         <v>1933</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D8" s="13">
-        <v>5610</v>
+        <v>590</v>
       </c>
       <c r="E8" s="13">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="F8" s="13">
-        <v>27.02</v>
+        <v>2.84</v>
       </c>
       <c r="G8" s="14">
-        <v>6.2999999999999998E-15</v>
+        <v>7.5E-10</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>933</v>
@@ -17623,8 +17620,8 @@
       <c r="L8" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N8" s="16" t="s">
-        <v>2436</v>
+      <c r="N8" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>2447</v>
@@ -17634,6 +17631,9 @@
       </c>
       <c r="T8" s="17" t="s">
         <v>931</v>
+      </c>
+      <c r="X8" s="13" t="s">
+        <v>2438</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -17641,22 +17641,22 @@
         <v>1933</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9" s="13">
-        <v>7650</v>
+        <v>8498</v>
       </c>
       <c r="E9" s="13">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F9" s="13">
-        <v>36.840000000000003</v>
+        <v>40.93</v>
       </c>
       <c r="G9" s="14">
-        <v>3.6999999999999999E-13</v>
+        <v>2.2999999999999999E-9</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>933</v>
@@ -17667,8 +17667,8 @@
       <c r="L9" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N9" s="16" t="s">
-        <v>2436</v>
+      <c r="N9" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>2447</v>
@@ -17685,22 +17685,22 @@
         <v>1933</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D10" s="13">
-        <v>6883</v>
+        <v>9084</v>
       </c>
       <c r="E10" s="13">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F10" s="13">
-        <v>33.15</v>
+        <v>43.75</v>
       </c>
       <c r="G10" s="14">
-        <v>8.9000000000000004E-13</v>
+        <v>2.7999999999999998E-9</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>933</v>
@@ -17708,8 +17708,8 @@
       <c r="J10" t="s">
         <v>931</v>
       </c>
-      <c r="L10" s="16" t="s">
-        <v>2436</v>
+      <c r="L10" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N10" s="16" t="s">
         <v>2436</v>
@@ -17729,28 +17729,28 @@
         <v>1933</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>948</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D11" s="13">
-        <v>5574</v>
+        <v>20227</v>
       </c>
       <c r="E11" s="13">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="F11" s="13">
-        <v>26.85</v>
+        <v>97.42</v>
       </c>
       <c r="G11" s="14">
-        <v>3.2000000000000001E-12</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>933</v>
+        <v>1.4E-8</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>931</v>
       </c>
       <c r="J11" t="s">
-        <v>931</v>
+        <v>1008</v>
       </c>
       <c r="L11" s="17" t="s">
         <v>931</v>
@@ -17758,14 +17758,14 @@
       <c r="N11" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P11" s="9" t="s">
-        <v>2447</v>
-      </c>
-      <c r="R11" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T11" s="17" t="s">
-        <v>931</v>
+      <c r="P11" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -17773,22 +17773,22 @@
         <v>1933</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D12" s="13">
-        <v>590</v>
+        <v>10620</v>
       </c>
       <c r="E12" s="13">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="F12" s="13">
-        <v>2.84</v>
+        <v>51.15</v>
       </c>
       <c r="G12" s="14">
-        <v>7.5E-10</v>
+        <v>5.1E-8</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>933</v>
@@ -17799,8 +17799,8 @@
       <c r="L12" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N12" s="17" t="s">
-        <v>931</v>
+      <c r="N12" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>2447</v>
@@ -17817,22 +17817,22 @@
         <v>1933</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>15</v>
+        <v>936</v>
       </c>
       <c r="D13" s="13">
-        <v>8498</v>
+        <v>3882</v>
       </c>
       <c r="E13" s="13">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="F13" s="13">
-        <v>40.93</v>
+        <v>18.7</v>
       </c>
       <c r="G13" s="14">
-        <v>2.2999999999999999E-9</v>
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>933</v>
@@ -17861,22 +17861,22 @@
         <v>1933</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D14" s="13">
-        <v>9084</v>
+        <v>8663</v>
       </c>
       <c r="E14" s="13">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F14" s="13">
-        <v>43.75</v>
+        <v>41.72</v>
       </c>
       <c r="G14" s="14">
-        <v>2.7999999999999998E-9</v>
+        <v>2.7000000000000001E-7</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>933</v>
@@ -17887,8 +17887,8 @@
       <c r="L14" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N14" s="16" t="s">
-        <v>2436</v>
+      <c r="N14" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>2447</v>
@@ -17905,22 +17905,22 @@
         <v>1933</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D15" s="13">
-        <v>10620</v>
+        <v>20735</v>
       </c>
       <c r="E15" s="13">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="F15" s="13">
-        <v>51.15</v>
+        <v>99.87</v>
       </c>
       <c r="G15" s="14">
-        <v>5.1E-8</v>
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>933</v>
@@ -17940,8 +17940,8 @@
       <c r="R15" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T15" s="17" t="s">
-        <v>931</v>
+      <c r="T15" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -17949,22 +17949,22 @@
         <v>1933</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>936</v>
+        <v>28</v>
       </c>
       <c r="D16" s="13">
-        <v>3882</v>
+        <v>16463</v>
       </c>
       <c r="E16" s="13">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="F16" s="13">
-        <v>18.7</v>
+        <v>79.290000000000006</v>
       </c>
       <c r="G16" s="14">
-        <v>1.4000000000000001E-7</v>
+        <v>9.1999999999999998E-7</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>933</v>
@@ -17975,8 +17975,8 @@
       <c r="L16" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>931</v>
+      <c r="N16" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>2447</v>
@@ -17984,8 +17984,8 @@
       <c r="R16" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T16" s="17" t="s">
-        <v>931</v>
+      <c r="T16" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -17993,22 +17993,22 @@
         <v>1933</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>24</v>
+        <v>937</v>
       </c>
       <c r="D17" s="13">
-        <v>8663</v>
+        <v>11</v>
       </c>
       <c r="E17" s="13">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="F17" s="13">
-        <v>41.72</v>
+        <v>0.05</v>
       </c>
       <c r="G17" s="14">
-        <v>2.7000000000000001E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>933</v>
@@ -18016,8 +18016,8 @@
       <c r="J17" t="s">
         <v>931</v>
       </c>
-      <c r="L17" s="17" t="s">
-        <v>931</v>
+      <c r="L17" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N17" s="17" t="s">
         <v>931</v>
@@ -18037,22 +18037,22 @@
         <v>1933</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D18" s="13">
-        <v>20735</v>
+        <v>11611</v>
       </c>
       <c r="E18" s="13">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="F18" s="13">
-        <v>99.87</v>
+        <v>55.92</v>
       </c>
       <c r="G18" s="14">
-        <v>5.6000000000000004E-7</v>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>933</v>
@@ -18063,8 +18063,8 @@
       <c r="L18" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N18" s="16" t="s">
-        <v>2436</v>
+      <c r="N18" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>2447</v>
@@ -18072,8 +18072,8 @@
       <c r="R18" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T18" s="16" t="s">
-        <v>2436</v>
+      <c r="T18" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -18081,22 +18081,22 @@
         <v>1933</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D19" s="13">
-        <v>16463</v>
+        <v>1792</v>
       </c>
       <c r="E19" s="13">
-        <v>123</v>
+        <v>33</v>
       </c>
       <c r="F19" s="13">
-        <v>79.290000000000006</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="G19" s="14">
-        <v>9.1999999999999998E-7</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>933</v>
@@ -18104,11 +18104,8 @@
       <c r="J19" t="s">
         <v>931</v>
       </c>
-      <c r="L19" s="17" t="s">
+      <c r="N19" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>2436</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>2447</v>
@@ -18116,8 +18113,11 @@
       <c r="R19" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T19" s="16" t="s">
-        <v>2436</v>
+      <c r="T19" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U19" t="s">
+        <v>2451</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -18125,22 +18125,22 @@
         <v>1933</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D20" s="13">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E20" s="13">
         <v>3</v>
       </c>
       <c r="F20" s="13">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="G20" s="14">
-        <v>1.0000000000000001E-5</v>
+        <v>4.5000000000000003E-5</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>933</v>
@@ -18169,22 +18169,22 @@
         <v>1933</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D21" s="13">
-        <v>11611</v>
+        <v>18</v>
       </c>
       <c r="E21" s="13">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="F21" s="13">
-        <v>55.92</v>
-      </c>
-      <c r="G21" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>0.09</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>933</v>
@@ -18213,22 +18213,22 @@
         <v>1933</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D22" s="13">
-        <v>1792</v>
+        <v>15584</v>
       </c>
       <c r="E22" s="13">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="F22" s="13">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="G22" s="14">
-        <v>4.0000000000000003E-5</v>
+        <v>75.06</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>933</v>
@@ -18236,20 +18236,20 @@
       <c r="J22" t="s">
         <v>931</v>
       </c>
-      <c r="N22" s="17" t="s">
-        <v>931</v>
+      <c r="L22" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R22" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T22" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="U22" t="s">
-        <v>2451</v>
+      <c r="R22" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -18257,22 +18257,22 @@
         <v>1933</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>938</v>
+        <v>40</v>
       </c>
       <c r="D23" s="13">
-        <v>16</v>
+        <v>286</v>
       </c>
       <c r="E23" s="13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F23" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="G23" s="14">
-        <v>4.5000000000000003E-5</v>
+        <v>1.38</v>
+      </c>
+      <c r="G23" s="13">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>933</v>
@@ -18280,11 +18280,11 @@
       <c r="J23" t="s">
         <v>931</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>2436</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>931</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>2447</v>
@@ -18292,8 +18292,11 @@
       <c r="R23" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T23" s="17" t="s">
-        <v>931</v>
+      <c r="S23" t="s">
+        <v>2441</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -18301,22 +18304,22 @@
         <v>1933</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D24" s="13">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="E24" s="13">
         <v>3</v>
       </c>
       <c r="F24" s="13">
-        <v>0.09</v>
+        <v>0.26</v>
       </c>
       <c r="G24" s="13">
-        <v>1.3999999999999999E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>933</v>
@@ -18345,22 +18348,22 @@
         <v>1933</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D25" s="13">
-        <v>286</v>
+        <v>484</v>
       </c>
       <c r="E25" s="13">
         <v>8</v>
       </c>
       <c r="F25" s="13">
-        <v>1.38</v>
+        <v>2.33</v>
       </c>
       <c r="G25" s="13">
-        <v>5.0000000000000001E-4</v>
+        <v>1.48E-3</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>933</v>
@@ -18371,8 +18374,8 @@
       <c r="L25" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N25" s="16" t="s">
-        <v>2436</v>
+      <c r="N25" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>2447</v>
@@ -18380,11 +18383,8 @@
       <c r="R25" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="S25" t="s">
-        <v>2441</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>2436</v>
+      <c r="T25" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -18392,10 +18392,10 @@
         <v>1933</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D26" s="13">
         <v>53</v>
@@ -18407,7 +18407,7 @@
         <v>0.26</v>
       </c>
       <c r="G26" s="13">
-        <v>9.3000000000000005E-4</v>
+        <v>2.16E-3</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>933</v>
@@ -18436,22 +18436,22 @@
         <v>1933</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>44</v>
+        <v>939</v>
       </c>
       <c r="D27" s="13">
-        <v>484</v>
+        <v>53</v>
       </c>
       <c r="E27" s="13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F27" s="13">
-        <v>2.33</v>
+        <v>0.26</v>
       </c>
       <c r="G27" s="13">
-        <v>1.48E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>933</v>
@@ -18480,43 +18480,46 @@
         <v>1933</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D28" s="13">
-        <v>53</v>
+        <v>16705</v>
       </c>
       <c r="E28" s="13">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="F28" s="13">
-        <v>0.26</v>
+        <v>80.459999999999994</v>
       </c>
       <c r="G28" s="13">
-        <v>2.16E-3</v>
+        <v>4.13E-3</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>944</v>
       </c>
       <c r="J28" t="s">
         <v>931</v>
       </c>
-      <c r="L28" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="N28" s="17" t="s">
-        <v>931</v>
+      <c r="L28" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R28" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T28" s="17" t="s">
-        <v>931</v>
+      <c r="R28" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T28" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -18524,43 +18527,43 @@
         <v>1933</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>939</v>
+        <v>50</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D29" s="13">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E29" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" s="13">
-        <v>0.26</v>
+        <v>0.16</v>
       </c>
       <c r="G29" s="13">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="H29" s="9" t="s">
+        <v>4.3899999999999998E-3</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J29" t="s">
         <v>933</v>
-      </c>
-      <c r="J29" t="s">
-        <v>931</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N29" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="P29" s="9" t="s">
-        <v>2447</v>
+      <c r="N29" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R29" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T29" s="17" t="s">
-        <v>931</v>
+      <c r="T29" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -18656,46 +18659,40 @@
         <v>1933</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="D32" s="13">
-        <v>250</v>
+        <v>70</v>
       </c>
       <c r="E32" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" s="13">
-        <v>1.2</v>
+        <v>0.34</v>
       </c>
       <c r="G32" s="13">
-        <v>8.0599999999999995E-3</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>943</v>
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>931</v>
       </c>
       <c r="J32" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N32" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="P32" s="9" t="s">
-        <v>2447</v>
+      <c r="P32" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R32" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T32" s="17" t="s">
-        <v>931</v>
+      <c r="T32" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -18703,34 +18700,37 @@
         <v>1933</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="D33" s="13">
-        <v>2007</v>
+        <v>250</v>
       </c>
       <c r="E33" s="13">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="F33" s="13">
-        <v>9.67</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>2</v>
+        <v>1.2</v>
+      </c>
+      <c r="G33" s="13">
+        <v>8.0599999999999995E-3</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>943</v>
       </c>
       <c r="J33" t="s">
         <v>931</v>
       </c>
-      <c r="L33" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="N33" s="16" t="s">
-        <v>2436</v>
+      <c r="L33" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>2447</v>
@@ -18738,75 +18738,75 @@
       <c r="R33" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T33" s="16" t="s">
-        <v>2436</v>
+      <c r="T33" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1856</v>
+        <v>1933</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1857</v>
-      </c>
-      <c r="D34">
-        <v>3016</v>
-      </c>
-      <c r="E34">
-        <v>80</v>
-      </c>
-      <c r="F34">
-        <v>15.83</v>
-      </c>
-      <c r="G34" s="1">
-        <v>3.4000000000000001E-28</v>
+        <v>60</v>
+      </c>
+      <c r="D34" s="13">
+        <v>1397</v>
+      </c>
+      <c r="E34" s="13">
+        <v>11</v>
+      </c>
+      <c r="F34" s="13">
+        <v>6.73</v>
+      </c>
+      <c r="G34" s="13">
+        <v>8.3400000000000002E-3</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>942</v>
       </c>
       <c r="J34" t="s">
         <v>931</v>
       </c>
-      <c r="L34" s="17" t="s">
+      <c r="L34" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N34" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N34" s="16" t="s">
-        <v>2436</v>
       </c>
       <c r="P34" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R34" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T34" s="16" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="Q34" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="13" customFormat="1">
       <c r="A35" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B35" t="s">
-        <v>1858</v>
+        <v>1916</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1859</v>
+        <v>1917</v>
       </c>
       <c r="D35">
-        <v>3016</v>
+        <v>1722</v>
       </c>
       <c r="E35">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F35">
-        <v>15.83</v>
-      </c>
-      <c r="G35" s="1">
-        <v>3.5E-28</v>
+        <v>8.66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>933</v>
@@ -18814,43 +18814,49 @@
       <c r="J35" t="s">
         <v>931</v>
       </c>
+      <c r="K35"/>
       <c r="L35" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="M35"/>
       <c r="N35" s="16" t="s">
         <v>2436</v>
       </c>
+      <c r="O35"/>
       <c r="P35" s="9" t="s">
         <v>2447</v>
       </c>
+      <c r="Q35"/>
       <c r="R35" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="S35"/>
       <c r="T35" s="16" t="s">
         <v>2436</v>
       </c>
+      <c r="U35"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B36" t="s">
-        <v>1860</v>
+        <v>1918</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1861</v>
+        <v>1919</v>
       </c>
       <c r="D36">
-        <v>5431</v>
+        <v>1357</v>
       </c>
       <c r="E36">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F36">
-        <v>28.51</v>
+        <v>6.82</v>
       </c>
       <c r="G36" s="1">
-        <v>5.5000000000000005E-26</v>
+        <v>2.4E-8</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>933</v>
@@ -18870,31 +18876,31 @@
       <c r="R36" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T36" s="16" t="s">
-        <v>2436</v>
+      <c r="T36" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B37" t="s">
-        <v>1862</v>
+        <v>1920</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1863</v>
+        <v>1921</v>
       </c>
       <c r="D37">
-        <v>10580</v>
+        <v>1495</v>
       </c>
       <c r="E37">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="F37">
-        <v>55.55</v>
+        <v>7.52</v>
       </c>
       <c r="G37" s="1">
-        <v>1.8000000000000001E-19</v>
+        <v>7.0000000000000005E-8</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>933</v>
@@ -18902,8 +18908,8 @@
       <c r="J37" t="s">
         <v>931</v>
       </c>
-      <c r="L37" s="17" t="s">
-        <v>931</v>
+      <c r="L37" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N37" s="16" t="s">
         <v>2436</v>
@@ -18911,34 +18917,34 @@
       <c r="P37" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R37" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T37" s="17" t="s">
-        <v>931</v>
+      <c r="R37" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T37" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B38" t="s">
-        <v>1864</v>
+        <v>1922</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1865</v>
+        <v>1923</v>
       </c>
       <c r="D38">
-        <v>5893</v>
+        <v>42</v>
       </c>
       <c r="E38">
-        <v>85</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>30.94</v>
+        <v>0.21</v>
       </c>
       <c r="G38" s="1">
-        <v>6.4999999999999996E-13</v>
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>933</v>
@@ -18949,40 +18955,34 @@
       <c r="L38" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N38" s="16" t="s">
-        <v>2436</v>
+      <c r="N38" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="P38" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R38" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T38" s="16" t="s">
-        <v>2436</v>
-      </c>
     </row>
     <row r="39" spans="1:21">
       <c r="A39" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B39" t="s">
-        <v>1866</v>
+        <v>1924</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1867</v>
+        <v>1925</v>
       </c>
       <c r="D39">
-        <v>20261</v>
+        <v>42</v>
       </c>
       <c r="E39">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="F39">
-        <v>106.37</v>
+        <v>0.21</v>
       </c>
       <c r="G39" s="1">
-        <v>1.1E-12</v>
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>933</v>
@@ -18993,40 +18993,34 @@
       <c r="L39" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N39" s="16" t="s">
-        <v>2436</v>
+      <c r="N39" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="P39" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R39" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T39" s="16" t="s">
-        <v>2436</v>
-      </c>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B40" t="s">
-        <v>1868</v>
+        <v>1926</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1869</v>
+        <v>1927</v>
       </c>
       <c r="D40">
-        <v>10569</v>
+        <v>42</v>
       </c>
       <c r="E40">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>55.49</v>
+        <v>0.21</v>
       </c>
       <c r="G40" s="1">
-        <v>1.3E-11</v>
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>933</v>
@@ -19037,93 +19031,81 @@
       <c r="L40" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N40" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="O40" s="13"/>
+      <c r="N40" s="15" t="s">
+        <v>933</v>
+      </c>
       <c r="P40" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R40" s="17" t="s">
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="13" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D41" s="13">
+        <v>18</v>
+      </c>
+      <c r="E41" s="13">
+        <v>3</v>
+      </c>
+      <c r="F41" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="G41" s="13">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>931</v>
       </c>
-      <c r="S40" s="13"/>
-      <c r="T40" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="U40" s="13"/>
-    </row>
-    <row r="41" spans="1:21" s="13" customFormat="1">
-      <c r="A41" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1870</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>1871</v>
-      </c>
-      <c r="D41">
-        <v>1115</v>
-      </c>
-      <c r="E41">
-        <v>69</v>
-      </c>
-      <c r="F41">
-        <v>5.85</v>
-      </c>
-      <c r="G41" s="1">
-        <v>2.9000000000000002E-8</v>
-      </c>
-      <c r="H41" s="9" t="s">
+      <c r="J41" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="J41" t="s">
-        <v>931</v>
-      </c>
-      <c r="K41"/>
-      <c r="L41" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="M41"/>
-      <c r="N41" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="O41"/>
-      <c r="P41" s="9" t="s">
-        <v>2447</v>
-      </c>
-      <c r="Q41"/>
-      <c r="R41" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="S41"/>
-      <c r="T41" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="U41"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="M41" s="13"/>
+      <c r="N41" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P41" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T41" s="15" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>1931</v>
       </c>
       <c r="B42" t="s">
-        <v>1872</v>
+        <v>1848</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1873</v>
+        <v>1849</v>
       </c>
       <c r="D42">
-        <v>1411</v>
+        <v>1151</v>
       </c>
       <c r="E42">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="F42">
-        <v>7.41</v>
-      </c>
-      <c r="G42" s="1">
-        <v>1.1000000000000001E-7</v>
+        <v>6.04</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>933</v>
@@ -19134,8 +19116,8 @@
       <c r="L42" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N42" s="17" t="s">
-        <v>931</v>
+      <c r="N42" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P42" s="9" t="s">
         <v>2447</v>
@@ -19143,8 +19125,8 @@
       <c r="R42" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T42" s="17" t="s">
-        <v>931</v>
+      <c r="T42" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -19152,22 +19134,22 @@
         <v>1931</v>
       </c>
       <c r="B43" t="s">
-        <v>1876</v>
+        <v>1850</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1877</v>
+        <v>1851</v>
       </c>
       <c r="D43">
-        <v>2318</v>
+        <v>1066</v>
       </c>
       <c r="E43">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="F43">
-        <v>12.17</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>5.6</v>
+      </c>
+      <c r="G43" t="s">
+        <v>2</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>933</v>
@@ -19175,8 +19157,8 @@
       <c r="J43" t="s">
         <v>931</v>
       </c>
-      <c r="L43" s="16" t="s">
-        <v>2436</v>
+      <c r="L43" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N43" s="16" t="s">
         <v>2436</v>
@@ -19196,22 +19178,22 @@
         <v>1931</v>
       </c>
       <c r="B44" t="s">
-        <v>1874</v>
+        <v>1852</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1875</v>
+        <v>1853</v>
       </c>
       <c r="D44">
-        <v>2318</v>
+        <v>1767</v>
       </c>
       <c r="E44">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F44">
-        <v>12.17</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="G44" t="s">
+        <v>2</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>933</v>
@@ -19231,8 +19213,8 @@
       <c r="R44" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T44" s="17" t="s">
-        <v>931</v>
+      <c r="T44" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -19240,22 +19222,22 @@
         <v>1931</v>
       </c>
       <c r="B45" t="s">
-        <v>1878</v>
+        <v>1854</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1879</v>
+        <v>1855</v>
       </c>
       <c r="D45">
-        <v>23508</v>
+        <v>1595</v>
       </c>
       <c r="E45">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="F45">
-        <v>123.42</v>
-      </c>
-      <c r="G45" s="1">
-        <v>5.6000000000000004E-7</v>
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="G45" t="s">
+        <v>2</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>933</v>
@@ -19275,8 +19257,8 @@
       <c r="R45" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T45" s="17" t="s">
-        <v>931</v>
+      <c r="T45" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -19284,22 +19266,22 @@
         <v>1931</v>
       </c>
       <c r="B46" t="s">
-        <v>1882</v>
+        <v>1856</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1883</v>
+        <v>1857</v>
       </c>
       <c r="D46">
-        <v>11959</v>
+        <v>3016</v>
       </c>
       <c r="E46">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F46">
-        <v>62.79</v>
+        <v>15.83</v>
       </c>
       <c r="G46" s="1">
-        <v>1.1999999999999999E-6</v>
+        <v>3.4000000000000001E-28</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>933</v>
@@ -19310,8 +19292,8 @@
       <c r="L46" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N46" s="17" t="s">
-        <v>931</v>
+      <c r="N46" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P46" s="9" t="s">
         <v>2447</v>
@@ -19319,8 +19301,8 @@
       <c r="R46" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T46" s="17" t="s">
-        <v>931</v>
+      <c r="T46" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -19328,22 +19310,22 @@
         <v>1931</v>
       </c>
       <c r="B47" t="s">
-        <v>1884</v>
+        <v>1858</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1885</v>
+        <v>1859</v>
       </c>
       <c r="D47">
-        <v>23774</v>
+        <v>3016</v>
       </c>
       <c r="E47">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="F47">
-        <v>124.82</v>
+        <v>15.83</v>
       </c>
       <c r="G47" s="1">
-        <v>2.3999999999999999E-6</v>
+        <v>3.5E-28</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>933</v>
@@ -19363,8 +19345,8 @@
       <c r="R47" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T47" s="17" t="s">
-        <v>931</v>
+      <c r="T47" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -19372,22 +19354,22 @@
         <v>1931</v>
       </c>
       <c r="B48" t="s">
-        <v>1888</v>
+        <v>1860</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>1889</v>
+        <v>1861</v>
       </c>
       <c r="D48">
-        <v>27911</v>
+        <v>5431</v>
       </c>
       <c r="E48">
-        <v>166</v>
+        <v>89</v>
       </c>
       <c r="F48">
-        <v>146.54</v>
+        <v>28.51</v>
       </c>
       <c r="G48" s="1">
-        <v>1.8E-5</v>
+        <v>5.5000000000000005E-26</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>933</v>
@@ -19407,8 +19389,8 @@
       <c r="R48" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T48" s="17" t="s">
-        <v>931</v>
+      <c r="T48" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -19416,22 +19398,22 @@
         <v>1931</v>
       </c>
       <c r="B49" t="s">
-        <v>1890</v>
+        <v>1862</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1891</v>
+        <v>1863</v>
       </c>
       <c r="D49">
-        <v>27911</v>
+        <v>10580</v>
       </c>
       <c r="E49">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="F49">
-        <v>146.54</v>
+        <v>55.55</v>
       </c>
       <c r="G49" s="1">
-        <v>1.8E-5</v>
+        <v>1.8000000000000001E-19</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>933</v>
@@ -19460,34 +19442,34 @@
         <v>1931</v>
       </c>
       <c r="B50" t="s">
-        <v>1902</v>
+        <v>1864</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1903</v>
+        <v>1865</v>
       </c>
       <c r="D50">
-        <v>361</v>
+        <v>5893</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="F50">
-        <v>1.9</v>
-      </c>
-      <c r="G50">
-        <v>3.8800000000000002E-3</v>
+        <v>30.94</v>
+      </c>
+      <c r="G50" s="1">
+        <v>6.4999999999999996E-13</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J50" t="s">
-        <v>1827</v>
+        <v>931</v>
       </c>
       <c r="L50" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N50" s="17" t="s">
-        <v>931</v>
+      <c r="N50" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P50" s="9" t="s">
         <v>2447</v>
@@ -19495,8 +19477,8 @@
       <c r="R50" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T50" s="17" t="s">
-        <v>931</v>
+      <c r="T50" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -19504,34 +19486,34 @@
         <v>1931</v>
       </c>
       <c r="B51" t="s">
-        <v>1904</v>
+        <v>1866</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1905</v>
+        <v>1867</v>
       </c>
       <c r="D51">
-        <v>361</v>
+        <v>20261</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="F51">
-        <v>1.9</v>
-      </c>
-      <c r="G51">
-        <v>4.13E-3</v>
+        <v>106.37</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1.1E-12</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J51" t="s">
-        <v>1826</v>
+        <v>931</v>
       </c>
       <c r="L51" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N51" s="17" t="s">
-        <v>931</v>
+      <c r="N51" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P51" s="9" t="s">
         <v>2447</v>
@@ -19539,8 +19521,8 @@
       <c r="R51" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T51" s="17" t="s">
-        <v>931</v>
+      <c r="T51" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -19548,22 +19530,22 @@
         <v>1931</v>
       </c>
       <c r="B52" t="s">
-        <v>1906</v>
+        <v>1868</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>1907</v>
+        <v>1869</v>
       </c>
       <c r="D52">
-        <v>32</v>
+        <v>10569</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F52">
-        <v>0.17</v>
-      </c>
-      <c r="G52">
-        <v>4.8300000000000001E-3</v>
+        <v>55.49</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1.3E-11</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>933</v>
@@ -19577,37 +19559,40 @@
       <c r="N52" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="O52" s="13"/>
       <c r="P52" s="9" t="s">
         <v>2447</v>
       </c>
       <c r="R52" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="S52" s="13"/>
       <c r="T52" s="17" t="s">
         <v>931</v>
       </c>
+      <c r="U52" s="13"/>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>1908</v>
+        <v>1870</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1909</v>
+        <v>1871</v>
       </c>
       <c r="D53">
-        <v>20703</v>
+        <v>1115</v>
       </c>
       <c r="E53">
-        <v>151</v>
+        <v>69</v>
       </c>
       <c r="F53">
-        <v>108.69</v>
-      </c>
-      <c r="G53">
-        <v>5.6499999999999996E-3</v>
+        <v>5.85</v>
+      </c>
+      <c r="G53" s="1">
+        <v>2.9000000000000002E-8</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>933</v>
@@ -19636,22 +19621,22 @@
         <v>1931</v>
       </c>
       <c r="B54" t="s">
-        <v>1910</v>
+        <v>1872</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>1911</v>
+        <v>1873</v>
       </c>
       <c r="D54">
-        <v>32</v>
+        <v>1411</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F54">
-        <v>0.17</v>
-      </c>
-      <c r="G54">
-        <v>6.6699999999999997E-3</v>
+        <v>7.41</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>933</v>
@@ -19659,8 +19644,8 @@
       <c r="J54" t="s">
         <v>931</v>
       </c>
-      <c r="L54" s="15" t="s">
-        <v>933</v>
+      <c r="L54" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N54" s="17" t="s">
         <v>931</v>
@@ -19673,9 +19658,6 @@
       </c>
       <c r="T54" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="U54" t="s">
-        <v>2443</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -19683,22 +19665,22 @@
         <v>1931</v>
       </c>
       <c r="B55" t="s">
-        <v>1848</v>
+        <v>1876</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1849</v>
+        <v>1877</v>
       </c>
       <c r="D55">
-        <v>1151</v>
+        <v>2318</v>
       </c>
       <c r="E55">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="F55">
-        <v>6.04</v>
-      </c>
-      <c r="G55" t="s">
-        <v>2</v>
+        <v>12.17</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>933</v>
@@ -19706,8 +19688,8 @@
       <c r="J55" t="s">
         <v>931</v>
       </c>
-      <c r="L55" s="17" t="s">
-        <v>931</v>
+      <c r="L55" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N55" s="16" t="s">
         <v>2436</v>
@@ -19718,8 +19700,8 @@
       <c r="R55" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T55" s="16" t="s">
-        <v>2436</v>
+      <c r="T55" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -19727,22 +19709,22 @@
         <v>1931</v>
       </c>
       <c r="B56" t="s">
-        <v>1850</v>
+        <v>1874</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>1851</v>
+        <v>1875</v>
       </c>
       <c r="D56">
-        <v>1066</v>
+        <v>2318</v>
       </c>
       <c r="E56">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F56">
-        <v>5.6</v>
-      </c>
-      <c r="G56" t="s">
-        <v>2</v>
+        <v>12.17</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>933</v>
@@ -19771,22 +19753,22 @@
         <v>1931</v>
       </c>
       <c r="B57" t="s">
-        <v>1852</v>
+        <v>1878</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>1853</v>
+        <v>1879</v>
       </c>
       <c r="D57">
-        <v>1767</v>
+        <v>23508</v>
       </c>
       <c r="E57">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="F57">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="G57" t="s">
-        <v>2</v>
+        <v>123.42</v>
+      </c>
+      <c r="G57" s="1">
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>933</v>
@@ -19806,8 +19788,8 @@
       <c r="R57" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T57" s="16" t="s">
-        <v>2436</v>
+      <c r="T57" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -19815,66 +19797,69 @@
         <v>1931</v>
       </c>
       <c r="B58" t="s">
-        <v>1854</v>
+        <v>1880</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>1855</v>
+        <v>1881</v>
       </c>
       <c r="D58">
-        <v>1595</v>
+        <v>1985</v>
       </c>
       <c r="E58">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="F58">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="G58" t="s">
-        <v>2</v>
+        <v>10.42</v>
+      </c>
+      <c r="G58" s="1">
+        <v>6.4000000000000001E-7</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I58" s="13" t="s">
+        <v>1824</v>
+      </c>
       <c r="J58" t="s">
         <v>931</v>
       </c>
-      <c r="L58" s="17" t="s">
-        <v>931</v>
+      <c r="L58" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N58" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P58" s="9" t="s">
-        <v>2447</v>
+      <c r="P58" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="R58" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T58" s="16" t="s">
-        <v>2436</v>
+      <c r="T58" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="59" spans="1:21">
       <c r="A59" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B59" t="s">
-        <v>1918</v>
+        <v>1882</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>1919</v>
+        <v>1883</v>
       </c>
       <c r="D59">
-        <v>1357</v>
+        <v>11959</v>
       </c>
       <c r="E59">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F59">
-        <v>6.82</v>
+        <v>62.79</v>
       </c>
       <c r="G59" s="1">
-        <v>2.4E-8</v>
+        <v>1.1999999999999999E-6</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>933</v>
@@ -19885,8 +19870,8 @@
       <c r="L59" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N59" s="16" t="s">
-        <v>2436</v>
+      <c r="N59" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P59" s="9" t="s">
         <v>2447</v>
@@ -19900,25 +19885,25 @@
     </row>
     <row r="60" spans="1:21">
       <c r="A60" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B60" t="s">
-        <v>1916</v>
+        <v>1884</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>1917</v>
+        <v>1885</v>
       </c>
       <c r="D60">
-        <v>1722</v>
+        <v>23774</v>
       </c>
       <c r="E60">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="F60">
-        <v>8.66</v>
-      </c>
-      <c r="G60" t="s">
-        <v>2</v>
+        <v>124.82</v>
+      </c>
+      <c r="G60" s="1">
+        <v>2.3999999999999999E-6</v>
       </c>
       <c r="H60" s="9" t="s">
         <v>933</v>
@@ -19938,43 +19923,46 @@
       <c r="R60" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T60" s="16" t="s">
-        <v>2436</v>
+      <c r="T60" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="61" spans="1:21">
       <c r="A61" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D61" s="13">
-        <v>33</v>
-      </c>
-      <c r="E61" s="13">
-        <v>2</v>
-      </c>
-      <c r="F61" s="13">
-        <v>0.16</v>
-      </c>
-      <c r="G61" s="13">
-        <v>4.3899999999999998E-3</v>
-      </c>
-      <c r="H61" s="10" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D61">
+        <v>3056</v>
+      </c>
+      <c r="E61">
+        <v>42</v>
+      </c>
+      <c r="F61">
+        <v>16.04</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>1823</v>
+      </c>
+      <c r="J61" t="s">
         <v>931</v>
       </c>
-      <c r="J61" t="s">
-        <v>933</v>
-      </c>
-      <c r="L61" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="N61" s="15" t="s">
-        <v>933</v>
+      <c r="L61" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P61" s="10" t="s">
         <v>2448</v>
@@ -19982,49 +19970,52 @@
       <c r="R61" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T61" s="16" t="s">
-        <v>2436</v>
+      <c r="T61" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="62" spans="1:21">
       <c r="A62" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D62" s="13">
-        <v>70</v>
-      </c>
-      <c r="E62" s="13">
-        <v>2</v>
-      </c>
-      <c r="F62" s="13">
-        <v>0.34</v>
-      </c>
-      <c r="G62" s="13">
-        <v>7.3400000000000002E-3</v>
-      </c>
-      <c r="H62" s="10" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>1889</v>
+      </c>
+      <c r="D62">
+        <v>27911</v>
+      </c>
+      <c r="E62">
+        <v>166</v>
+      </c>
+      <c r="F62">
+        <v>146.54</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1.8E-5</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J62" t="s">
         <v>931</v>
-      </c>
-      <c r="J62" t="s">
-        <v>933</v>
       </c>
       <c r="L62" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="P62" s="10" t="s">
-        <v>2448</v>
+      <c r="N62" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P62" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R62" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T62" s="16" t="s">
-        <v>2436</v>
+      <c r="T62" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -20032,46 +20023,43 @@
         <v>1931</v>
       </c>
       <c r="B63" t="s">
-        <v>1886</v>
+        <v>1890</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>1887</v>
+        <v>1891</v>
       </c>
       <c r="D63">
-        <v>3056</v>
+        <v>27911</v>
       </c>
       <c r="E63">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="F63">
-        <v>16.04</v>
+        <v>146.54</v>
       </c>
       <c r="G63" s="1">
-        <v>1.1E-5</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I63" s="13" t="s">
-        <v>1823</v>
-      </c>
       <c r="J63" t="s">
         <v>931</v>
       </c>
-      <c r="L63" s="16" t="s">
-        <v>2436</v>
+      <c r="L63" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P63" s="10" t="s">
-        <v>2448</v>
+      <c r="P63" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R63" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T63" s="15" t="s">
-        <v>933</v>
+      <c r="T63" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -20079,160 +20067,160 @@
         <v>1931</v>
       </c>
       <c r="B64" t="s">
-        <v>1896</v>
+        <v>1892</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>1897</v>
+        <v>1893</v>
       </c>
       <c r="D64">
-        <v>1969</v>
+        <v>3492</v>
       </c>
       <c r="E64">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F64">
-        <v>10.34</v>
-      </c>
-      <c r="G64">
-        <v>1.7000000000000001E-4</v>
+        <v>18.329999999999998</v>
+      </c>
+      <c r="G64" s="1">
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="H64" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I64" s="13" t="s">
-        <v>1825</v>
-      </c>
       <c r="J64" t="s">
         <v>931</v>
       </c>
-      <c r="L64" s="17" t="s">
-        <v>931</v>
+      <c r="L64" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P64" s="10" t="s">
-        <v>2448</v>
+      <c r="P64" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R64" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T64" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20">
+      <c r="T64" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21">
       <c r="A65" t="s">
         <v>1931</v>
       </c>
       <c r="B65" t="s">
-        <v>1880</v>
+        <v>1894</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>1881</v>
+        <v>1895</v>
       </c>
       <c r="D65">
-        <v>1985</v>
+        <v>720</v>
       </c>
       <c r="E65">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F65">
-        <v>10.42</v>
-      </c>
-      <c r="G65" s="1">
-        <v>6.4000000000000001E-7</v>
+        <v>3.78</v>
+      </c>
+      <c r="G65">
+        <v>1.1E-4</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I65" s="13" t="s">
-        <v>1824</v>
-      </c>
       <c r="J65" t="s">
         <v>931</v>
       </c>
-      <c r="L65" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="N65" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P65" s="16" t="s">
-        <v>2436</v>
+      <c r="L65" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R65" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T65" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20">
+      <c r="S65" t="s">
+        <v>2442</v>
+      </c>
+      <c r="T65" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21">
       <c r="A66" t="s">
         <v>1931</v>
       </c>
       <c r="B66" t="s">
-        <v>1892</v>
+        <v>1896</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1893</v>
+        <v>1897</v>
       </c>
       <c r="D66">
-        <v>3492</v>
+        <v>1969</v>
       </c>
       <c r="E66">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F66">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="G66" s="1">
-        <v>4.8000000000000001E-5</v>
+        <v>10.34</v>
+      </c>
+      <c r="G66">
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I66" s="13" t="s">
+        <v>1825</v>
+      </c>
       <c r="J66" t="s">
         <v>931</v>
       </c>
-      <c r="L66" s="16" t="s">
-        <v>2436</v>
+      <c r="L66" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N66" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P66" s="9" t="s">
-        <v>2447</v>
+      <c r="P66" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R66" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T66" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20">
+      <c r="T66" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21">
       <c r="A67" t="s">
         <v>1931</v>
       </c>
       <c r="B67" t="s">
-        <v>1894</v>
+        <v>1898</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>1895</v>
+        <v>1899</v>
       </c>
       <c r="D67">
-        <v>720</v>
+        <v>1480</v>
       </c>
       <c r="E67">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F67">
-        <v>3.78</v>
+        <v>7.77</v>
       </c>
       <c r="G67">
-        <v>1.1E-4</v>
+        <v>1.65E-3</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>933</v>
@@ -20252,34 +20240,31 @@
       <c r="R67" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="S67" t="s">
-        <v>2442</v>
-      </c>
       <c r="T67" s="17" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:21">
       <c r="A68" t="s">
         <v>1931</v>
       </c>
       <c r="B68" t="s">
-        <v>1898</v>
+        <v>1900</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1899</v>
+        <v>1901</v>
       </c>
       <c r="D68">
-        <v>1480</v>
+        <v>20252</v>
       </c>
       <c r="E68">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="F68">
-        <v>7.77</v>
+        <v>106.33</v>
       </c>
       <c r="G68">
-        <v>1.65E-3</v>
+        <v>1.7700000000000001E-3</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>933</v>
@@ -20293,8 +20278,8 @@
       <c r="N68" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="P68" s="9" t="s">
-        <v>2447</v>
+      <c r="P68" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="R68" s="17" t="s">
         <v>931</v>
@@ -20303,33 +20288,33 @@
         <v>931</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:21">
       <c r="A69" t="s">
         <v>1931</v>
       </c>
       <c r="B69" t="s">
-        <v>1900</v>
+        <v>1902</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>1901</v>
+        <v>1903</v>
       </c>
       <c r="D69">
-        <v>20252</v>
+        <v>361</v>
       </c>
       <c r="E69">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="F69">
-        <v>106.33</v>
+        <v>1.9</v>
       </c>
       <c r="G69">
-        <v>1.7700000000000001E-3</v>
+        <v>3.8800000000000002E-3</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J69" t="s">
-        <v>931</v>
+        <v>1827</v>
       </c>
       <c r="L69" s="17" t="s">
         <v>931</v>
@@ -20337,8 +20322,8 @@
       <c r="N69" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="P69" s="16" t="s">
-        <v>2436</v>
+      <c r="P69" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R69" s="17" t="s">
         <v>931</v>
@@ -20347,33 +20332,33 @@
         <v>931</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:21">
       <c r="A70" t="s">
         <v>1931</v>
       </c>
       <c r="B70" t="s">
-        <v>1914</v>
+        <v>1904</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1915</v>
+        <v>1905</v>
       </c>
       <c r="D70">
-        <v>19850</v>
+        <v>361</v>
       </c>
       <c r="E70">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="F70">
-        <v>104.21</v>
+        <v>1.9</v>
       </c>
       <c r="G70">
-        <v>8.0300000000000007E-3</v>
+        <v>4.13E-3</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J70" t="s">
-        <v>931</v>
+        <v>1826</v>
       </c>
       <c r="L70" s="17" t="s">
         <v>931</v>
@@ -20391,27 +20376,27 @@
         <v>931</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:21">
       <c r="A71" t="s">
         <v>1931</v>
       </c>
       <c r="B71" t="s">
-        <v>1912</v>
+        <v>1906</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1913</v>
+        <v>1907</v>
       </c>
       <c r="D71">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E71">
         <v>3</v>
       </c>
       <c r="F71">
-        <v>0.28000000000000003</v>
+        <v>0.17</v>
       </c>
       <c r="G71">
-        <v>6.7499999999999999E-3</v>
+        <v>4.8300000000000001E-3</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>933</v>
@@ -20419,8 +20404,8 @@
       <c r="J71" t="s">
         <v>931</v>
       </c>
-      <c r="L71" s="15" t="s">
-        <v>933</v>
+      <c r="L71" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N71" s="17" t="s">
         <v>931</v>
@@ -20428,31 +20413,34 @@
       <c r="P71" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="T71" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20">
+      <c r="R71" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T71" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21">
       <c r="A72" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B72" t="s">
-        <v>1922</v>
+        <v>1908</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>1923</v>
+        <v>1909</v>
       </c>
       <c r="D72">
-        <v>42</v>
+        <v>20703</v>
       </c>
       <c r="E72">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="F72">
-        <v>0.21</v>
-      </c>
-      <c r="G72" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>108.69</v>
+      </c>
+      <c r="G72">
+        <v>5.6499999999999996E-3</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>933</v>
@@ -20463,34 +20451,40 @@
       <c r="L72" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N72" s="15" t="s">
-        <v>933</v>
+      <c r="N72" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P72" s="9" t="s">
         <v>2447</v>
       </c>
-    </row>
-    <row r="73" spans="1:20">
+      <c r="R72" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T72" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21">
       <c r="A73" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B73" t="s">
-        <v>1924</v>
+        <v>1910</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>1925</v>
+        <v>1911</v>
       </c>
       <c r="D73">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73">
-        <v>0.21</v>
-      </c>
-      <c r="G73" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>0.17</v>
+      </c>
+      <c r="G73">
+        <v>6.6699999999999997E-3</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>933</v>
@@ -20498,37 +20492,46 @@
       <c r="J73" t="s">
         <v>931</v>
       </c>
-      <c r="L73" s="17" t="s">
+      <c r="L73" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N73" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N73" s="15" t="s">
-        <v>933</v>
       </c>
       <c r="P73" s="9" t="s">
         <v>2447</v>
       </c>
-    </row>
-    <row r="74" spans="1:20">
+      <c r="R73" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T73" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U73" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21">
       <c r="A74" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B74" t="s">
-        <v>1926</v>
+        <v>1912</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>1927</v>
+        <v>1913</v>
       </c>
       <c r="D74">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74">
-        <v>0.21</v>
-      </c>
-      <c r="G74" s="1">
-        <v>4.3999999999999999E-5</v>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G74">
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>933</v>
@@ -20536,49 +20539,49 @@
       <c r="J74" t="s">
         <v>931</v>
       </c>
-      <c r="L74" s="17" t="s">
+      <c r="L74" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="N74" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N74" s="15" t="s">
-        <v>933</v>
       </c>
       <c r="P74" s="9" t="s">
         <v>2447</v>
       </c>
-    </row>
-    <row r="75" spans="1:20">
+      <c r="T74" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21">
       <c r="A75" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>59</v>
+        <v>1931</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1914</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D75" s="13">
-        <v>1397</v>
-      </c>
-      <c r="E75" s="13">
-        <v>11</v>
-      </c>
-      <c r="F75" s="13">
-        <v>6.73</v>
-      </c>
-      <c r="G75" s="13">
-        <v>8.3400000000000002E-3</v>
+        <v>1915</v>
+      </c>
+      <c r="D75">
+        <v>19850</v>
+      </c>
+      <c r="E75">
+        <v>146</v>
+      </c>
+      <c r="F75">
+        <v>104.21</v>
+      </c>
+      <c r="G75">
+        <v>8.0300000000000007E-3</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="J75" t="s">
         <v>931</v>
       </c>
-      <c r="L75" s="15" t="s">
-        <v>933</v>
+      <c r="L75" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N75" s="17" t="s">
         <v>931</v>
@@ -20586,17 +20589,17 @@
       <c r="P75" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="Q75" t="s">
-        <v>2449</v>
+      <c r="R75" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T75" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:U75">
-    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="9"/>
-    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="8"/>
-    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="7"/>
-    <sortCondition sortBy="cellColor" ref="P2:P75" dxfId="6"/>
-    <sortCondition sortBy="cellColor" ref="P2:P75" dxfId="5"/>
+    <sortCondition ref="A2:A75" customList="BP,MF,CC"/>
+    <sortCondition ref="G2:G75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
write some Go Term tables and genes up or down tables!
</commit_message>
<xml_diff>
--- a/GOtermEnrichment.xlsx
+++ b/GOtermEnrichment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515"/>
+    <workbookView xWindow="270" yWindow="840" windowWidth="20520" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryOrigin" sheetId="28" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5434" uniqueCount="2457">
   <si>
     <t>GO:0006412</t>
   </si>
@@ -7401,6 +7401,18 @@
   </si>
   <si>
     <t>NE inv rel to nat, T0</t>
+  </si>
+  <si>
+    <t>inv pval = 0.071</t>
+  </si>
+  <si>
+    <t>nat pval = 0.04124</t>
+  </si>
+  <si>
+    <t>nat pval = 0.06344</t>
+  </si>
+  <si>
+    <t>nat pval = 0.0187, inv pval = 0.00376</t>
   </si>
 </sst>
 </file>
@@ -7526,7 +7538,135 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -8017,10 +8157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8029,7 +8169,7 @@
     <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>1930</v>
       </c>
@@ -8058,7 +8198,7 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1933</v>
       </c>
@@ -8083,8 +8223,14 @@
       <c r="H2" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1933</v>
       </c>
@@ -8109,8 +8255,14 @@
       <c r="H3" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1933</v>
       </c>
@@ -8135,8 +8287,11 @@
       <c r="H4" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1933</v>
       </c>
@@ -8161,8 +8316,11 @@
       <c r="H5" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>1933</v>
       </c>
@@ -8187,8 +8345,11 @@
       <c r="H6" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>1933</v>
       </c>
@@ -8213,8 +8374,11 @@
       <c r="H7" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1933</v>
       </c>
@@ -8239,8 +8403,11 @@
       <c r="H8" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1933</v>
       </c>
@@ -8265,8 +8432,11 @@
       <c r="H9" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>1933</v>
       </c>
@@ -8291,8 +8461,11 @@
       <c r="H10" s="10" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1933</v>
       </c>
@@ -8317,8 +8490,11 @@
       <c r="H11" s="10" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>1933</v>
       </c>
@@ -8343,8 +8519,11 @@
       <c r="H12" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1933</v>
       </c>
@@ -8369,8 +8548,11 @@
       <c r="H13" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>1933</v>
       </c>
@@ -8395,8 +8577,14 @@
       <c r="H14" s="9" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="J14" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="K14" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>1933</v>
       </c>
@@ -8421,8 +8609,11 @@
       <c r="H15" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>1933</v>
       </c>
@@ -8447,8 +8638,11 @@
       <c r="H16" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>1932</v>
       </c>
@@ -8473,8 +8667,14 @@
       <c r="H17" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="J17" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>1932</v>
       </c>
@@ -8499,8 +8699,11 @@
       <c r="H18" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="J18" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>1932</v>
       </c>
@@ -8525,8 +8728,11 @@
       <c r="H19" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="J19" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>1932</v>
       </c>
@@ -8551,8 +8757,11 @@
       <c r="H20" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="J20" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>1932</v>
       </c>
@@ -8577,8 +8786,11 @@
       <c r="H21" s="10" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="J21" s="10" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>1931</v>
       </c>
@@ -8603,8 +8815,11 @@
       <c r="H22" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="J22" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>1931</v>
       </c>
@@ -8629,8 +8844,11 @@
       <c r="H23" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="J23" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>1931</v>
       </c>
@@ -8655,8 +8873,11 @@
       <c r="H24" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="J24" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>1931</v>
       </c>
@@ -8681,8 +8902,11 @@
       <c r="H25" s="9" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="J25" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>1931</v>
       </c>
@@ -8706,6 +8930,9 @@
       </c>
       <c r="H26" s="9" t="s">
         <v>933</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>2447</v>
       </c>
     </row>
   </sheetData>
@@ -17247,11 +17474,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2:T75"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17327,25 +17554,28 @@
         <v>1933</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D2" s="13">
-        <v>2007</v>
+        <v>16705</v>
       </c>
       <c r="E2" s="13">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="F2" s="13">
-        <v>9.67</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>2</v>
+        <v>80.459999999999994</v>
+      </c>
+      <c r="G2" s="13">
+        <v>4.13E-3</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>944</v>
       </c>
       <c r="J2" t="s">
         <v>931</v>
@@ -17353,61 +17583,64 @@
       <c r="L2" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>2436</v>
+      <c r="N2" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="13" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D3" s="13">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="G3" s="13">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>931</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="13">
-        <v>5027</v>
-      </c>
-      <c r="E3" s="13">
-        <v>85</v>
-      </c>
-      <c r="F3" s="13">
-        <v>24.21</v>
-      </c>
-      <c r="G3" s="14">
-        <v>2.0999999999999998E-15</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="J3" t="s">
-        <v>931</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>2447</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>931</v>
+      <c r="K3" s="13"/>
+      <c r="L3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -17415,28 +17648,28 @@
         <v>1933</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="13">
-        <v>5610</v>
+        <v>20227</v>
       </c>
       <c r="E4" s="13">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="F4" s="13">
-        <v>27.02</v>
+        <v>97.42</v>
       </c>
       <c r="G4" s="14">
-        <v>6.2999999999999998E-15</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>933</v>
+        <v>1.4E-8</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>931</v>
       </c>
       <c r="J4" t="s">
-        <v>931</v>
+        <v>1008</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>931</v>
@@ -17444,14 +17677,14 @@
       <c r="N4" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>2447</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>931</v>
+      <c r="P4" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>2437</v>
@@ -17459,25 +17692,25 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
+        <v>1932</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1920</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13">
-        <v>7650</v>
-      </c>
-      <c r="E5" s="13">
-        <v>97</v>
-      </c>
-      <c r="F5" s="13">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="G5" s="14">
-        <v>3.6999999999999999E-13</v>
+        <v>1921</v>
+      </c>
+      <c r="D5">
+        <v>1495</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>7.52</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7.0000000000000005E-8</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>933</v>
@@ -17485,8 +17718,8 @@
       <c r="J5" t="s">
         <v>931</v>
       </c>
-      <c r="L5" s="17" t="s">
-        <v>931</v>
+      <c r="L5" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2436</v>
@@ -17494,11 +17727,11 @@
       <c r="P5" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R5" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T5" s="17" t="s">
-        <v>931</v>
+      <c r="R5" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -17506,22 +17739,22 @@
         <v>1933</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D6" s="13">
-        <v>6883</v>
+        <v>15584</v>
       </c>
       <c r="E6" s="13">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="F6" s="13">
-        <v>33.15</v>
-      </c>
-      <c r="G6" s="14">
-        <v>8.9000000000000004E-13</v>
+        <v>75.06</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>933</v>
@@ -17538,11 +17771,11 @@
       <c r="P6" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R6" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T6" s="17" t="s">
-        <v>931</v>
+      <c r="R6" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -17550,22 +17783,22 @@
         <v>1933</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>948</v>
+        <v>1</v>
       </c>
       <c r="D7" s="13">
-        <v>5574</v>
+        <v>2007</v>
       </c>
       <c r="E7" s="13">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F7" s="13">
-        <v>26.85</v>
-      </c>
-      <c r="G7" s="14">
-        <v>3.2000000000000001E-12</v>
+        <v>9.67</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>933</v>
@@ -17573,8 +17806,8 @@
       <c r="J7" t="s">
         <v>931</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>931</v>
+      <c r="L7" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N7" s="16" t="s">
         <v>2436</v>
@@ -17585,8 +17818,8 @@
       <c r="R7" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T7" s="17" t="s">
-        <v>931</v>
+      <c r="T7" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -17594,22 +17827,22 @@
         <v>1933</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13">
-        <v>590</v>
+        <v>20735</v>
       </c>
       <c r="E8" s="13">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="F8" s="13">
-        <v>2.84</v>
+        <v>99.87</v>
       </c>
       <c r="G8" s="14">
-        <v>7.5E-10</v>
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>933</v>
@@ -17620,8 +17853,8 @@
       <c r="L8" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>931</v>
+      <c r="N8" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>2447</v>
@@ -17629,8 +17862,8 @@
       <c r="R8" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T8" s="17" t="s">
-        <v>931</v>
+      <c r="T8" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>2438</v>
@@ -17641,22 +17874,22 @@
         <v>1933</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D9" s="13">
-        <v>8498</v>
+        <v>16463</v>
       </c>
       <c r="E9" s="13">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="F9" s="13">
-        <v>40.93</v>
+        <v>79.290000000000006</v>
       </c>
       <c r="G9" s="14">
-        <v>2.2999999999999999E-9</v>
+        <v>9.1999999999999998E-7</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>933</v>
@@ -17667,8 +17900,8 @@
       <c r="L9" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>931</v>
+      <c r="N9" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>2447</v>
@@ -17676,8 +17909,8 @@
       <c r="R9" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T9" s="17" t="s">
-        <v>931</v>
+      <c r="T9" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -17685,22 +17918,22 @@
         <v>1933</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D10" s="13">
-        <v>9084</v>
+        <v>286</v>
       </c>
       <c r="E10" s="13">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="F10" s="13">
-        <v>43.75</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2.7999999999999998E-9</v>
+        <v>1.38</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>933</v>
@@ -17720,8 +17953,11 @@
       <c r="R10" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T10" s="17" t="s">
-        <v>931</v>
+      <c r="S10" t="s">
+        <v>2441</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -17729,40 +17965,40 @@
         <v>1933</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D11" s="13">
-        <v>20227</v>
+        <v>33</v>
       </c>
       <c r="E11" s="13">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="F11" s="13">
-        <v>97.42</v>
-      </c>
-      <c r="G11" s="14">
-        <v>1.4E-8</v>
+        <v>0.16</v>
+      </c>
+      <c r="G11" s="13">
+        <v>4.3899999999999998E-3</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>931</v>
       </c>
       <c r="J11" t="s">
-        <v>1008</v>
+        <v>933</v>
       </c>
       <c r="L11" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N11" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>2436</v>
+      <c r="N11" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="T11" s="16" t="s">
         <v>2436</v>
@@ -17773,66 +18009,63 @@
         <v>1933</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>21</v>
+        <v>55</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="D12" s="13">
-        <v>10620</v>
+        <v>70</v>
       </c>
       <c r="E12" s="13">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="F12" s="13">
-        <v>51.15</v>
-      </c>
-      <c r="G12" s="14">
-        <v>5.1E-8</v>
-      </c>
-      <c r="H12" s="9" t="s">
+        <v>0.34</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="J12" t="s">
         <v>933</v>
-      </c>
-      <c r="J12" t="s">
-        <v>931</v>
       </c>
       <c r="L12" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N12" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>2447</v>
+      <c r="P12" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R12" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T12" s="17" t="s">
-        <v>931</v>
+      <c r="T12" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>22</v>
+        <v>1932</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1916</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>936</v>
-      </c>
-      <c r="D13" s="13">
-        <v>3882</v>
-      </c>
-      <c r="E13" s="13">
-        <v>43</v>
-      </c>
-      <c r="F13" s="13">
-        <v>18.7</v>
-      </c>
-      <c r="G13" s="14">
-        <v>1.4000000000000001E-7</v>
+        <v>1917</v>
+      </c>
+      <c r="D13">
+        <v>1722</v>
+      </c>
+      <c r="E13">
+        <v>72</v>
+      </c>
+      <c r="F13">
+        <v>8.66</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>933</v>
@@ -17843,8 +18076,8 @@
       <c r="L13" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N13" s="17" t="s">
-        <v>931</v>
+      <c r="N13" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>2447</v>
@@ -17852,31 +18085,31 @@
       <c r="R13" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T13" s="17" t="s">
-        <v>931</v>
+      <c r="T13" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>23</v>
+        <v>1931</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1848</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="13">
-        <v>8663</v>
-      </c>
-      <c r="E14" s="13">
-        <v>91</v>
-      </c>
-      <c r="F14" s="13">
-        <v>41.72</v>
-      </c>
-      <c r="G14" s="14">
-        <v>2.7000000000000001E-7</v>
+        <v>1849</v>
+      </c>
+      <c r="D14">
+        <v>1151</v>
+      </c>
+      <c r="E14">
+        <v>69</v>
+      </c>
+      <c r="F14">
+        <v>6.04</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>933</v>
@@ -17887,8 +18120,8 @@
       <c r="L14" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N14" s="17" t="s">
-        <v>931</v>
+      <c r="N14" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>2447</v>
@@ -17896,31 +18129,31 @@
       <c r="R14" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T14" s="17" t="s">
-        <v>931</v>
+      <c r="T14" s="16" t="s">
+        <v>2436</v>
       </c>
     </row>
     <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>25</v>
+        <v>1931</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1852</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="13">
-        <v>20735</v>
-      </c>
-      <c r="E15" s="13">
-        <v>132</v>
-      </c>
-      <c r="F15" s="13">
-        <v>99.87</v>
-      </c>
-      <c r="G15" s="14">
-        <v>5.6000000000000004E-7</v>
+        <v>1853</v>
+      </c>
+      <c r="D15">
+        <v>1767</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+      <c r="F15">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>933</v>
@@ -17946,25 +18179,25 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>27</v>
+        <v>1931</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1854</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="13">
-        <v>16463</v>
-      </c>
-      <c r="E16" s="13">
-        <v>123</v>
-      </c>
-      <c r="F16" s="13">
-        <v>79.290000000000006</v>
-      </c>
-      <c r="G16" s="14">
-        <v>9.1999999999999998E-7</v>
+        <v>1855</v>
+      </c>
+      <c r="D16">
+        <v>1595</v>
+      </c>
+      <c r="E16">
+        <v>73</v>
+      </c>
+      <c r="F16">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>933</v>
@@ -17988,27 +18221,27 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>29</v>
+        <v>1931</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1856</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>937</v>
-      </c>
-      <c r="D17" s="13">
-        <v>11</v>
-      </c>
-      <c r="E17" s="13">
-        <v>3</v>
-      </c>
-      <c r="F17" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="G17" s="14">
-        <v>1.0000000000000001E-5</v>
+        <v>1857</v>
+      </c>
+      <c r="D17">
+        <v>3016</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17">
+        <v>15.83</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.4000000000000001E-28</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>933</v>
@@ -18016,11 +18249,11 @@
       <c r="J17" t="s">
         <v>931</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N17" s="16" t="s">
         <v>2436</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>931</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>2447</v>
@@ -18028,31 +18261,31 @@
       <c r="R17" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T17" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="T17" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>30</v>
+        <v>1931</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1858</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="13">
-        <v>11611</v>
-      </c>
-      <c r="E18" s="13">
-        <v>105</v>
-      </c>
-      <c r="F18" s="13">
-        <v>55.92</v>
-      </c>
-      <c r="G18" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>1859</v>
+      </c>
+      <c r="D18">
+        <v>3016</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <v>15.83</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3.5E-28</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>933</v>
@@ -18063,8 +18296,8 @@
       <c r="L18" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N18" s="17" t="s">
-        <v>931</v>
+      <c r="N18" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>2447</v>
@@ -18072,31 +18305,31 @@
       <c r="R18" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T18" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="T18" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>32</v>
+        <v>1931</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1860</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="13">
-        <v>1792</v>
-      </c>
-      <c r="E19" s="13">
-        <v>33</v>
-      </c>
-      <c r="F19" s="13">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="G19" s="14">
-        <v>4.0000000000000003E-5</v>
+        <v>1861</v>
+      </c>
+      <c r="D19">
+        <v>5431</v>
+      </c>
+      <c r="E19">
+        <v>89</v>
+      </c>
+      <c r="F19">
+        <v>28.51</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5.5000000000000005E-26</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>933</v>
@@ -18104,8 +18337,11 @@
       <c r="J19" t="s">
         <v>931</v>
       </c>
-      <c r="N19" s="17" t="s">
+      <c r="L19" s="17" t="s">
         <v>931</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>2447</v>
@@ -18113,34 +18349,31 @@
       <c r="R19" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T19" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="U19" t="s">
-        <v>2451</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="T19" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>34</v>
+        <v>1931</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1864</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>938</v>
-      </c>
-      <c r="D20" s="13">
-        <v>16</v>
-      </c>
-      <c r="E20" s="13">
-        <v>3</v>
-      </c>
-      <c r="F20" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="G20" s="14">
-        <v>4.5000000000000003E-5</v>
+        <v>1865</v>
+      </c>
+      <c r="D20">
+        <v>5893</v>
+      </c>
+      <c r="E20">
+        <v>85</v>
+      </c>
+      <c r="F20">
+        <v>30.94</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6.4999999999999996E-13</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>933</v>
@@ -18148,11 +18381,11 @@
       <c r="J20" t="s">
         <v>931</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="L20" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N20" s="16" t="s">
         <v>2436</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>931</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>2447</v>
@@ -18160,31 +18393,31 @@
       <c r="R20" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T20" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="T20" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>35</v>
+        <v>1931</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1866</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="13">
-        <v>18</v>
-      </c>
-      <c r="E21" s="13">
-        <v>3</v>
-      </c>
-      <c r="F21" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1.3999999999999999E-4</v>
+        <v>1867</v>
+      </c>
+      <c r="D21">
+        <v>20261</v>
+      </c>
+      <c r="E21">
+        <v>150</v>
+      </c>
+      <c r="F21">
+        <v>106.37</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1.1E-12</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>933</v>
@@ -18195,8 +18428,8 @@
       <c r="L21" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N21" s="17" t="s">
-        <v>931</v>
+      <c r="N21" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>2447</v>
@@ -18204,35 +18437,38 @@
       <c r="R21" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T21" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="T21" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>37</v>
+        <v>1931</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1880</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="13">
-        <v>15584</v>
-      </c>
-      <c r="E22" s="13">
-        <v>120</v>
-      </c>
-      <c r="F22" s="13">
-        <v>75.06</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1.4999999999999999E-4</v>
+        <v>1881</v>
+      </c>
+      <c r="D22">
+        <v>1985</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+      <c r="F22">
+        <v>10.42</v>
+      </c>
+      <c r="G22" s="1">
+        <v>6.4000000000000001E-7</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I22" s="13" t="s">
+        <v>1824</v>
+      </c>
       <c r="J22" t="s">
         <v>931</v>
       </c>
@@ -18242,128 +18478,131 @@
       <c r="N22" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P22" s="9" t="s">
-        <v>2447</v>
-      </c>
-      <c r="R22" s="16" t="s">
+      <c r="P22" s="16" t="s">
         <v>2436</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="T22" s="15" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>39</v>
+        <v>1931</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1886</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="13">
-        <v>286</v>
-      </c>
-      <c r="E23" s="13">
-        <v>8</v>
-      </c>
-      <c r="F23" s="13">
-        <v>1.38</v>
-      </c>
-      <c r="G23" s="13">
-        <v>5.0000000000000001E-4</v>
+        <v>1887</v>
+      </c>
+      <c r="D23">
+        <v>3056</v>
+      </c>
+      <c r="E23">
+        <v>42</v>
+      </c>
+      <c r="F23">
+        <v>16.04</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.1E-5</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I23" s="13" t="s">
+        <v>1823</v>
+      </c>
       <c r="J23" t="s">
         <v>931</v>
       </c>
-      <c r="L23" s="17" t="s">
-        <v>931</v>
+      <c r="L23" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="N23" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P23" s="9" t="s">
-        <v>2447</v>
+      <c r="P23" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R23" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="S23" t="s">
-        <v>2441</v>
-      </c>
-      <c r="T23" s="16" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="T23" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>41</v>
+        <v>1931</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1896</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="13">
-        <v>53</v>
-      </c>
-      <c r="E24" s="13">
-        <v>3</v>
-      </c>
-      <c r="F24" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G24" s="13">
-        <v>9.3000000000000005E-4</v>
+        <v>1897</v>
+      </c>
+      <c r="D24">
+        <v>1969</v>
+      </c>
+      <c r="E24">
+        <v>35</v>
+      </c>
+      <c r="F24">
+        <v>10.34</v>
+      </c>
+      <c r="G24">
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>933</v>
       </c>
+      <c r="I24" s="13" t="s">
+        <v>1825</v>
+      </c>
       <c r="J24" t="s">
         <v>931</v>
       </c>
       <c r="L24" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N24" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>2447</v>
+      <c r="N24" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>2448</v>
       </c>
       <c r="R24" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T24" s="17" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="T24" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>1933</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D25" s="13">
-        <v>484</v>
+        <v>5027</v>
       </c>
       <c r="E25" s="13">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F25" s="13">
-        <v>2.33</v>
-      </c>
-      <c r="G25" s="13">
-        <v>1.48E-3</v>
+        <v>24.21</v>
+      </c>
+      <c r="G25" s="14">
+        <v>2.0999999999999998E-15</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>933</v>
@@ -18374,8 +18613,8 @@
       <c r="L25" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N25" s="17" t="s">
-        <v>931</v>
+      <c r="N25" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>2447</v>
@@ -18387,27 +18626,27 @@
         <v>931</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>1933</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D26" s="13">
-        <v>53</v>
+        <v>5610</v>
       </c>
       <c r="E26" s="13">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="F26" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G26" s="13">
-        <v>2.16E-3</v>
+        <v>27.02</v>
+      </c>
+      <c r="G26" s="14">
+        <v>6.2999999999999998E-15</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>933</v>
@@ -18418,8 +18657,8 @@
       <c r="L26" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N26" s="17" t="s">
-        <v>931</v>
+      <c r="N26" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>2447</v>
@@ -18431,27 +18670,27 @@
         <v>931</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>1933</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>939</v>
+        <v>8</v>
       </c>
       <c r="D27" s="13">
-        <v>53</v>
+        <v>7650</v>
       </c>
       <c r="E27" s="13">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F27" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="G27" s="13">
-        <v>2.5000000000000001E-3</v>
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G27" s="14">
+        <v>3.6999999999999999E-13</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>933</v>
@@ -18462,8 +18701,8 @@
       <c r="L27" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N27" s="17" t="s">
-        <v>931</v>
+      <c r="N27" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>2447</v>
@@ -18475,33 +18714,30 @@
         <v>931</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
         <v>1933</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D28" s="13">
-        <v>16705</v>
+        <v>6883</v>
       </c>
       <c r="E28" s="13">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F28" s="13">
-        <v>80.459999999999994</v>
-      </c>
-      <c r="G28" s="13">
-        <v>4.13E-3</v>
+        <v>33.15</v>
+      </c>
+      <c r="G28" s="14">
+        <v>8.9000000000000004E-13</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="J28" t="s">
         <v>931</v>
@@ -18509,84 +18745,84 @@
       <c r="L28" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="N28" s="15" t="s">
-        <v>933</v>
+      <c r="N28" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R28" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="T28" s="15" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="R28" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T28" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
         <v>1933</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>948</v>
       </c>
       <c r="D29" s="13">
-        <v>33</v>
+        <v>5574</v>
       </c>
       <c r="E29" s="13">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="F29" s="13">
-        <v>0.16</v>
-      </c>
-      <c r="G29" s="13">
-        <v>4.3899999999999998E-3</v>
-      </c>
-      <c r="H29" s="10" t="s">
+        <v>26.85</v>
+      </c>
+      <c r="G29" s="14">
+        <v>3.2000000000000001E-12</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J29" t="s">
         <v>931</v>
-      </c>
-      <c r="J29" t="s">
-        <v>933</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N29" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>2448</v>
+      <c r="N29" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R29" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T29" s="16" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="T29" s="17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>1933</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>949</v>
+        <v>13</v>
       </c>
       <c r="D30" s="13">
-        <v>118</v>
+        <v>590</v>
       </c>
       <c r="E30" s="13">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F30" s="13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G30" s="13">
-        <v>5.4999999999999997E-3</v>
+        <v>2.84</v>
+      </c>
+      <c r="G30" s="14">
+        <v>7.5E-10</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>933</v>
@@ -18610,27 +18846,27 @@
         <v>931</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:20">
       <c r="A31" t="s">
         <v>1933</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D31" s="13">
-        <v>118</v>
+        <v>8498</v>
       </c>
       <c r="E31" s="13">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F31" s="13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G31" s="13">
-        <v>7.0499999999999998E-3</v>
+        <v>40.93</v>
+      </c>
+      <c r="G31" s="14">
+        <v>2.2999999999999999E-9</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>933</v>
@@ -18654,45 +18890,48 @@
         <v>931</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
         <v>1933</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="D32" s="13">
-        <v>70</v>
+        <v>9084</v>
       </c>
       <c r="E32" s="13">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="F32" s="13">
-        <v>0.34</v>
-      </c>
-      <c r="G32" s="13">
-        <v>7.3400000000000002E-3</v>
-      </c>
-      <c r="H32" s="10" t="s">
+        <v>43.75</v>
+      </c>
+      <c r="G32" s="14">
+        <v>2.7999999999999998E-9</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J32" t="s">
         <v>931</v>
-      </c>
-      <c r="J32" t="s">
-        <v>933</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="P32" s="10" t="s">
-        <v>2448</v>
+      <c r="N32" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R32" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T32" s="16" t="s">
-        <v>2436</v>
+      <c r="T32" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -18700,28 +18939,25 @@
         <v>1933</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="D33" s="13">
-        <v>250</v>
+        <v>10620</v>
       </c>
       <c r="E33" s="13">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="F33" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="G33" s="13">
-        <v>8.0599999999999995E-3</v>
+        <v>51.15</v>
+      </c>
+      <c r="G33" s="14">
+        <v>5.1E-8</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="J33" t="s">
         <v>931</v>
@@ -18729,8 +18965,8 @@
       <c r="L33" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N33" s="17" t="s">
-        <v>931</v>
+      <c r="N33" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>2447</v>
@@ -18747,34 +18983,31 @@
         <v>1933</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>60</v>
+        <v>936</v>
       </c>
       <c r="D34" s="13">
-        <v>1397</v>
+        <v>3882</v>
       </c>
       <c r="E34" s="13">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="F34" s="13">
-        <v>6.73</v>
-      </c>
-      <c r="G34" s="13">
-        <v>8.3400000000000002E-3</v>
+        <v>18.7</v>
+      </c>
+      <c r="G34" s="14">
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>934</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="J34" t="s">
         <v>931</v>
       </c>
-      <c r="L34" s="15" t="s">
-        <v>933</v>
+      <c r="L34" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N34" s="17" t="s">
         <v>931</v>
@@ -18782,31 +19015,34 @@
       <c r="P34" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="Q34" t="s">
-        <v>2449</v>
+      <c r="R34" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T34" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="35" spans="1:21" s="13" customFormat="1">
       <c r="A35" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1916</v>
+        <v>1933</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1917</v>
-      </c>
-      <c r="D35">
-        <v>1722</v>
-      </c>
-      <c r="E35">
-        <v>72</v>
-      </c>
-      <c r="F35">
-        <v>8.66</v>
-      </c>
-      <c r="G35" t="s">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="D35" s="13">
+        <v>8663</v>
+      </c>
+      <c r="E35" s="13">
+        <v>91</v>
+      </c>
+      <c r="F35" s="13">
+        <v>41.72</v>
+      </c>
+      <c r="G35" s="14">
+        <v>2.7000000000000001E-7</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>933</v>
@@ -18819,8 +19055,8 @@
         <v>931</v>
       </c>
       <c r="M35"/>
-      <c r="N35" s="16" t="s">
-        <v>2436</v>
+      <c r="N35" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="O35"/>
       <c r="P35" s="9" t="s">
@@ -18831,32 +19067,32 @@
         <v>931</v>
       </c>
       <c r="S35"/>
-      <c r="T35" s="16" t="s">
-        <v>2436</v>
+      <c r="T35" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="U35"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B36" t="s">
-        <v>1918</v>
+        <v>1933</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1919</v>
-      </c>
-      <c r="D36">
-        <v>1357</v>
-      </c>
-      <c r="E36">
-        <v>72</v>
-      </c>
-      <c r="F36">
-        <v>6.82</v>
-      </c>
-      <c r="G36" s="1">
-        <v>2.4E-8</v>
+        <v>937</v>
+      </c>
+      <c r="D36" s="13">
+        <v>11</v>
+      </c>
+      <c r="E36" s="13">
+        <v>3</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="G36" s="14">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>933</v>
@@ -18864,11 +19100,11 @@
       <c r="J36" t="s">
         <v>931</v>
       </c>
-      <c r="L36" s="17" t="s">
+      <c r="L36" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N36" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>2436</v>
       </c>
       <c r="P36" s="9" t="s">
         <v>2447</v>
@@ -18882,25 +19118,25 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1920</v>
+        <v>1933</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>1921</v>
-      </c>
-      <c r="D37">
-        <v>1495</v>
-      </c>
-      <c r="E37">
-        <v>21</v>
-      </c>
-      <c r="F37">
-        <v>7.52</v>
-      </c>
-      <c r="G37" s="1">
-        <v>7.0000000000000005E-8</v>
+        <v>31</v>
+      </c>
+      <c r="D37" s="13">
+        <v>11611</v>
+      </c>
+      <c r="E37" s="13">
+        <v>105</v>
+      </c>
+      <c r="F37" s="13">
+        <v>55.92</v>
+      </c>
+      <c r="G37" s="14">
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>933</v>
@@ -18908,43 +19144,43 @@
       <c r="J37" t="s">
         <v>931</v>
       </c>
-      <c r="L37" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="N37" s="16" t="s">
-        <v>2436</v>
+      <c r="L37" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P37" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R37" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="T37" s="16" t="s">
-        <v>2436</v>
+      <c r="R37" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T37" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1922</v>
+        <v>1933</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1923</v>
-      </c>
-      <c r="D38">
-        <v>42</v>
-      </c>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38">
-        <v>0.21</v>
-      </c>
-      <c r="G38" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>33</v>
+      </c>
+      <c r="D38" s="13">
+        <v>1792</v>
+      </c>
+      <c r="E38" s="13">
+        <v>33</v>
+      </c>
+      <c r="F38" s="13">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="G38" s="14">
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>933</v>
@@ -18952,37 +19188,43 @@
       <c r="J38" t="s">
         <v>931</v>
       </c>
-      <c r="L38" s="17" t="s">
+      <c r="N38" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N38" s="15" t="s">
-        <v>933</v>
       </c>
       <c r="P38" s="9" t="s">
         <v>2447</v>
       </c>
+      <c r="R38" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T38" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U38" t="s">
+        <v>2451</v>
+      </c>
     </row>
     <row r="39" spans="1:21">
       <c r="A39" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1924</v>
+        <v>1933</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1925</v>
-      </c>
-      <c r="D39">
-        <v>42</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="F39">
-        <v>0.21</v>
-      </c>
-      <c r="G39" s="1">
-        <v>2.5999999999999998E-5</v>
+        <v>938</v>
+      </c>
+      <c r="D39" s="13">
+        <v>16</v>
+      </c>
+      <c r="E39" s="13">
+        <v>3</v>
+      </c>
+      <c r="F39" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="G39" s="14">
+        <v>4.5000000000000003E-5</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>933</v>
@@ -18990,37 +19232,43 @@
       <c r="J39" t="s">
         <v>931</v>
       </c>
-      <c r="L39" s="17" t="s">
+      <c r="L39" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N39" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="N39" s="15" t="s">
-        <v>933</v>
       </c>
       <c r="P39" s="9" t="s">
         <v>2447</v>
       </c>
+      <c r="R39" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T39" s="17" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1926</v>
+        <v>1933</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1927</v>
-      </c>
-      <c r="D40">
-        <v>42</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40">
-        <v>0.21</v>
-      </c>
-      <c r="G40" s="1">
-        <v>4.3999999999999999E-5</v>
+        <v>36</v>
+      </c>
+      <c r="D40" s="13">
+        <v>18</v>
+      </c>
+      <c r="E40" s="13">
+        <v>3</v>
+      </c>
+      <c r="F40" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="G40" s="13">
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>933</v>
@@ -19031,81 +19279,84 @@
       <c r="L40" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N40" s="15" t="s">
-        <v>933</v>
+      <c r="N40" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P40" s="9" t="s">
         <v>2447</v>
       </c>
+      <c r="R40" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T40" s="17" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="13" t="s">
-        <v>1932</v>
+      <c r="A41" t="s">
+        <v>1933</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>1929</v>
+        <v>41</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D41" s="13">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="E41" s="13">
         <v>3</v>
       </c>
       <c r="F41" s="13">
-        <v>0.09</v>
+        <v>0.26</v>
       </c>
       <c r="G41" s="13">
-        <v>2.3E-3</v>
-      </c>
-      <c r="H41" s="10" t="s">
+        <v>9.3000000000000005E-4</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>933</v>
+      </c>
+      <c r="J41" t="s">
         <v>931</v>
       </c>
-      <c r="J41" s="13" t="s">
-        <v>933</v>
-      </c>
-      <c r="K41" s="13"/>
-      <c r="L41" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="M41" s="13"/>
-      <c r="N41" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>2448</v>
-      </c>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="T41" s="15" t="s">
-        <v>933</v>
+      <c r="L41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>2447</v>
+      </c>
+      <c r="R41" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="T41" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1848</v>
+        <v>1933</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>1849</v>
-      </c>
-      <c r="D42">
-        <v>1151</v>
-      </c>
-      <c r="E42">
-        <v>69</v>
-      </c>
-      <c r="F42">
-        <v>6.04</v>
-      </c>
-      <c r="G42" t="s">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="D42" s="13">
+        <v>484</v>
+      </c>
+      <c r="E42" s="13">
+        <v>8</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2.33</v>
+      </c>
+      <c r="G42" s="13">
+        <v>1.48E-3</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>933</v>
@@ -19116,8 +19367,8 @@
       <c r="L42" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N42" s="16" t="s">
-        <v>2436</v>
+      <c r="N42" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P42" s="9" t="s">
         <v>2447</v>
@@ -19125,31 +19376,31 @@
       <c r="R42" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T42" s="16" t="s">
-        <v>2436</v>
+      <c r="T42" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1850</v>
+        <v>1933</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>1851</v>
-      </c>
-      <c r="D43">
-        <v>1066</v>
-      </c>
-      <c r="E43">
-        <v>66</v>
-      </c>
-      <c r="F43">
-        <v>5.6</v>
-      </c>
-      <c r="G43" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="D43" s="13">
+        <v>53</v>
+      </c>
+      <c r="E43" s="13">
+        <v>3</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0.26</v>
+      </c>
+      <c r="G43" s="13">
+        <v>2.16E-3</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>933</v>
@@ -19160,8 +19411,8 @@
       <c r="L43" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N43" s="16" t="s">
-        <v>2436</v>
+      <c r="N43" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P43" s="9" t="s">
         <v>2447</v>
@@ -19175,25 +19426,25 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1852</v>
+        <v>1933</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>1853</v>
-      </c>
-      <c r="D44">
-        <v>1767</v>
-      </c>
-      <c r="E44">
-        <v>75</v>
-      </c>
-      <c r="F44">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="G44" t="s">
-        <v>2</v>
+        <v>939</v>
+      </c>
+      <c r="D44" s="13">
+        <v>53</v>
+      </c>
+      <c r="E44" s="13">
+        <v>3</v>
+      </c>
+      <c r="F44" s="13">
+        <v>0.26</v>
+      </c>
+      <c r="G44" s="13">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>933</v>
@@ -19204,8 +19455,8 @@
       <c r="L44" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N44" s="16" t="s">
-        <v>2436</v>
+      <c r="N44" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P44" s="9" t="s">
         <v>2447</v>
@@ -19213,31 +19464,31 @@
       <c r="R44" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T44" s="16" t="s">
-        <v>2436</v>
+      <c r="T44" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1854</v>
+        <v>1933</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>1855</v>
-      </c>
-      <c r="D45">
-        <v>1595</v>
-      </c>
-      <c r="E45">
-        <v>73</v>
-      </c>
-      <c r="F45">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="G45" t="s">
-        <v>2</v>
+        <v>949</v>
+      </c>
+      <c r="D45" s="13">
+        <v>118</v>
+      </c>
+      <c r="E45" s="13">
+        <v>3</v>
+      </c>
+      <c r="F45" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G45" s="13">
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>933</v>
@@ -19248,8 +19499,8 @@
       <c r="L45" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N45" s="16" t="s">
-        <v>2436</v>
+      <c r="N45" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P45" s="9" t="s">
         <v>2447</v>
@@ -19257,31 +19508,31 @@
       <c r="R45" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T45" s="16" t="s">
-        <v>2436</v>
+      <c r="T45" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1856</v>
+        <v>1933</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>1857</v>
-      </c>
-      <c r="D46">
-        <v>3016</v>
-      </c>
-      <c r="E46">
-        <v>80</v>
-      </c>
-      <c r="F46">
-        <v>15.83</v>
-      </c>
-      <c r="G46" s="1">
-        <v>3.4000000000000001E-28</v>
+        <v>54</v>
+      </c>
+      <c r="D46" s="13">
+        <v>118</v>
+      </c>
+      <c r="E46" s="13">
+        <v>3</v>
+      </c>
+      <c r="F46" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G46" s="13">
+        <v>7.0499999999999998E-3</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>933</v>
@@ -19292,8 +19543,8 @@
       <c r="L46" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N46" s="16" t="s">
-        <v>2436</v>
+      <c r="N46" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P46" s="9" t="s">
         <v>2447</v>
@@ -19301,34 +19552,37 @@
       <c r="R46" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T46" s="16" t="s">
-        <v>2436</v>
+      <c r="T46" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1858</v>
+        <v>1933</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1859</v>
-      </c>
-      <c r="D47">
-        <v>3016</v>
-      </c>
-      <c r="E47">
-        <v>80</v>
-      </c>
-      <c r="F47">
-        <v>15.83</v>
-      </c>
-      <c r="G47" s="1">
-        <v>3.5E-28</v>
+        <v>58</v>
+      </c>
+      <c r="D47" s="13">
+        <v>250</v>
+      </c>
+      <c r="E47" s="13">
+        <v>4</v>
+      </c>
+      <c r="F47" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="G47" s="13">
+        <v>8.0599999999999995E-3</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>943</v>
       </c>
       <c r="J47" t="s">
         <v>931</v>
@@ -19336,8 +19590,8 @@
       <c r="L47" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N47" s="16" t="s">
-        <v>2436</v>
+      <c r="N47" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P47" s="9" t="s">
         <v>2447</v>
@@ -19345,31 +19599,31 @@
       <c r="R47" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T47" s="16" t="s">
-        <v>2436</v>
+      <c r="T47" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B48" t="s">
-        <v>1860</v>
+        <v>1918</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>1861</v>
+        <v>1919</v>
       </c>
       <c r="D48">
-        <v>5431</v>
+        <v>1357</v>
       </c>
       <c r="E48">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F48">
-        <v>28.51</v>
+        <v>6.82</v>
       </c>
       <c r="G48" s="1">
-        <v>5.5000000000000005E-26</v>
+        <v>2.4E-8</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>933</v>
@@ -19389,8 +19643,8 @@
       <c r="R48" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T48" s="16" t="s">
-        <v>2436</v>
+      <c r="T48" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -19398,22 +19652,22 @@
         <v>1931</v>
       </c>
       <c r="B49" t="s">
-        <v>1862</v>
+        <v>1850</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1863</v>
+        <v>1851</v>
       </c>
       <c r="D49">
-        <v>10580</v>
+        <v>1066</v>
       </c>
       <c r="E49">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="F49">
-        <v>55.55</v>
-      </c>
-      <c r="G49" s="1">
-        <v>1.8000000000000001E-19</v>
+        <v>5.6</v>
+      </c>
+      <c r="G49" t="s">
+        <v>2</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>933</v>
@@ -19442,22 +19696,22 @@
         <v>1931</v>
       </c>
       <c r="B50" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="D50">
-        <v>5893</v>
+        <v>10580</v>
       </c>
       <c r="E50">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="F50">
-        <v>30.94</v>
+        <v>55.55</v>
       </c>
       <c r="G50" s="1">
-        <v>6.4999999999999996E-13</v>
+        <v>1.8000000000000001E-19</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>933</v>
@@ -19477,8 +19731,8 @@
       <c r="R50" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T50" s="16" t="s">
-        <v>2436</v>
+      <c r="T50" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -19486,22 +19740,22 @@
         <v>1931</v>
       </c>
       <c r="B51" t="s">
-        <v>1866</v>
+        <v>1868</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1867</v>
+        <v>1869</v>
       </c>
       <c r="D51">
-        <v>20261</v>
+        <v>10569</v>
       </c>
       <c r="E51">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="F51">
-        <v>106.37</v>
+        <v>55.49</v>
       </c>
       <c r="G51" s="1">
-        <v>1.1E-12</v>
+        <v>1.3E-11</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>933</v>
@@ -19512,40 +19766,43 @@
       <c r="L51" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N51" s="16" t="s">
-        <v>2436</v>
-      </c>
+      <c r="N51" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="O51" s="13"/>
       <c r="P51" s="9" t="s">
         <v>2447</v>
       </c>
       <c r="R51" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T51" s="16" t="s">
-        <v>2436</v>
-      </c>
+      <c r="S51" s="13"/>
+      <c r="T51" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="U51" s="13"/>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" t="s">
         <v>1931</v>
       </c>
       <c r="B52" t="s">
-        <v>1868</v>
+        <v>1870</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>1869</v>
+        <v>1871</v>
       </c>
       <c r="D52">
-        <v>10569</v>
+        <v>1115</v>
       </c>
       <c r="E52">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="F52">
-        <v>55.49</v>
+        <v>5.85</v>
       </c>
       <c r="G52" s="1">
-        <v>1.3E-11</v>
+        <v>2.9000000000000002E-8</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>933</v>
@@ -19559,40 +19816,37 @@
       <c r="N52" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="O52" s="13"/>
       <c r="P52" s="9" t="s">
         <v>2447</v>
       </c>
       <c r="R52" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="S52" s="13"/>
       <c r="T52" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="U52" s="13"/>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>1870</v>
+        <v>1872</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1871</v>
+        <v>1873</v>
       </c>
       <c r="D53">
-        <v>1115</v>
+        <v>1411</v>
       </c>
       <c r="E53">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="F53">
-        <v>5.85</v>
+        <v>7.41</v>
       </c>
       <c r="G53" s="1">
-        <v>2.9000000000000002E-8</v>
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>933</v>
@@ -19621,22 +19875,22 @@
         <v>1931</v>
       </c>
       <c r="B54" t="s">
-        <v>1872</v>
+        <v>1876</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>1873</v>
+        <v>1877</v>
       </c>
       <c r="D54">
-        <v>1411</v>
+        <v>2318</v>
       </c>
       <c r="E54">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F54">
-        <v>7.41</v>
+        <v>12.17</v>
       </c>
       <c r="G54" s="1">
-        <v>1.1000000000000001E-7</v>
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>933</v>
@@ -19644,11 +19898,11 @@
       <c r="J54" t="s">
         <v>931</v>
       </c>
-      <c r="L54" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>931</v>
+      <c r="L54" s="16" t="s">
+        <v>2436</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P54" s="9" t="s">
         <v>2447</v>
@@ -19665,10 +19919,10 @@
         <v>1931</v>
       </c>
       <c r="B55" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="D55">
         <v>2318</v>
@@ -19688,8 +19942,8 @@
       <c r="J55" t="s">
         <v>931</v>
       </c>
-      <c r="L55" s="16" t="s">
-        <v>2436</v>
+      <c r="L55" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N55" s="16" t="s">
         <v>2436</v>
@@ -19709,22 +19963,22 @@
         <v>1931</v>
       </c>
       <c r="B56" t="s">
-        <v>1874</v>
+        <v>1878</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>1875</v>
+        <v>1879</v>
       </c>
       <c r="D56">
-        <v>2318</v>
+        <v>23508</v>
       </c>
       <c r="E56">
-        <v>33</v>
+        <v>160</v>
       </c>
       <c r="F56">
-        <v>12.17</v>
+        <v>123.42</v>
       </c>
       <c r="G56" s="1">
-        <v>1.4000000000000001E-7</v>
+        <v>5.6000000000000004E-7</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>933</v>
@@ -19753,22 +20007,22 @@
         <v>1931</v>
       </c>
       <c r="B57" t="s">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>1879</v>
+        <v>1883</v>
       </c>
       <c r="D57">
-        <v>23508</v>
+        <v>11959</v>
       </c>
       <c r="E57">
-        <v>160</v>
+        <v>94</v>
       </c>
       <c r="F57">
-        <v>123.42</v>
+        <v>62.79</v>
       </c>
       <c r="G57" s="1">
-        <v>5.6000000000000004E-7</v>
+        <v>1.1999999999999999E-6</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>933</v>
@@ -19779,8 +20033,8 @@
       <c r="L57" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N57" s="16" t="s">
-        <v>2436</v>
+      <c r="N57" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P57" s="9" t="s">
         <v>2447</v>
@@ -19797,46 +20051,43 @@
         <v>1931</v>
       </c>
       <c r="B58" t="s">
-        <v>1880</v>
+        <v>1884</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>1881</v>
+        <v>1885</v>
       </c>
       <c r="D58">
-        <v>1985</v>
+        <v>23774</v>
       </c>
       <c r="E58">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="F58">
-        <v>10.42</v>
+        <v>124.82</v>
       </c>
       <c r="G58" s="1">
-        <v>6.4000000000000001E-7</v>
+        <v>2.3999999999999999E-6</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I58" s="13" t="s">
-        <v>1824</v>
-      </c>
       <c r="J58" t="s">
         <v>931</v>
       </c>
-      <c r="L58" s="16" t="s">
-        <v>2436</v>
+      <c r="L58" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="N58" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P58" s="16" t="s">
-        <v>2436</v>
+      <c r="P58" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R58" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T58" s="15" t="s">
-        <v>933</v>
+      <c r="T58" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -19844,22 +20095,22 @@
         <v>1931</v>
       </c>
       <c r="B59" t="s">
-        <v>1882</v>
+        <v>1888</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>1883</v>
+        <v>1889</v>
       </c>
       <c r="D59">
-        <v>11959</v>
+        <v>27911</v>
       </c>
       <c r="E59">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="F59">
-        <v>62.79</v>
+        <v>146.54</v>
       </c>
       <c r="G59" s="1">
-        <v>1.1999999999999999E-6</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>933</v>
@@ -19870,8 +20121,8 @@
       <c r="L59" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N59" s="17" t="s">
-        <v>931</v>
+      <c r="N59" s="16" t="s">
+        <v>2436</v>
       </c>
       <c r="P59" s="9" t="s">
         <v>2447</v>
@@ -19888,22 +20139,22 @@
         <v>1931</v>
       </c>
       <c r="B60" t="s">
-        <v>1884</v>
+        <v>1890</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>1885</v>
+        <v>1891</v>
       </c>
       <c r="D60">
-        <v>23774</v>
+        <v>27911</v>
       </c>
       <c r="E60">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F60">
-        <v>124.82</v>
+        <v>146.54</v>
       </c>
       <c r="G60" s="1">
-        <v>2.3999999999999999E-6</v>
+        <v>1.8E-5</v>
       </c>
       <c r="H60" s="9" t="s">
         <v>933</v>
@@ -19932,29 +20183,26 @@
         <v>1931</v>
       </c>
       <c r="B61" t="s">
-        <v>1886</v>
+        <v>1892</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>1887</v>
+        <v>1893</v>
       </c>
       <c r="D61">
-        <v>3056</v>
+        <v>3492</v>
       </c>
       <c r="E61">
         <v>42</v>
       </c>
       <c r="F61">
-        <v>16.04</v>
+        <v>18.329999999999998</v>
       </c>
       <c r="G61" s="1">
-        <v>1.1E-5</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="H61" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I61" s="13" t="s">
-        <v>1823</v>
-      </c>
       <c r="J61" t="s">
         <v>931</v>
       </c>
@@ -19964,14 +20212,14 @@
       <c r="N61" s="16" t="s">
         <v>2436</v>
       </c>
-      <c r="P61" s="10" t="s">
-        <v>2448</v>
+      <c r="P61" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R61" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T61" s="15" t="s">
-        <v>933</v>
+      <c r="T61" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -19979,22 +20227,22 @@
         <v>1931</v>
       </c>
       <c r="B62" t="s">
-        <v>1888</v>
+        <v>1894</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>1889</v>
+        <v>1895</v>
       </c>
       <c r="D62">
-        <v>27911</v>
+        <v>720</v>
       </c>
       <c r="E62">
-        <v>166</v>
+        <v>11</v>
       </c>
       <c r="F62">
-        <v>146.54</v>
-      </c>
-      <c r="G62" s="1">
-        <v>1.8E-5</v>
+        <v>3.78</v>
+      </c>
+      <c r="G62">
+        <v>1.1E-4</v>
       </c>
       <c r="H62" s="9" t="s">
         <v>933</v>
@@ -20005,14 +20253,17 @@
       <c r="L62" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N62" s="16" t="s">
-        <v>2436</v>
+      <c r="N62" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P62" s="9" t="s">
         <v>2447</v>
       </c>
       <c r="R62" s="17" t="s">
         <v>931</v>
+      </c>
+      <c r="S62" t="s">
+        <v>2442</v>
       </c>
       <c r="T62" s="17" t="s">
         <v>931</v>
@@ -20023,22 +20274,22 @@
         <v>1931</v>
       </c>
       <c r="B63" t="s">
-        <v>1890</v>
+        <v>1898</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>1891</v>
+        <v>1899</v>
       </c>
       <c r="D63">
-        <v>27911</v>
+        <v>1480</v>
       </c>
       <c r="E63">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="F63">
-        <v>146.54</v>
-      </c>
-      <c r="G63" s="1">
-        <v>1.8E-5</v>
+        <v>7.77</v>
+      </c>
+      <c r="G63">
+        <v>1.65E-3</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>933</v>
@@ -20049,8 +20300,8 @@
       <c r="L63" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N63" s="16" t="s">
-        <v>2436</v>
+      <c r="N63" s="17" t="s">
+        <v>931</v>
       </c>
       <c r="P63" s="9" t="s">
         <v>2447</v>
@@ -20067,22 +20318,22 @@
         <v>1931</v>
       </c>
       <c r="B64" t="s">
-        <v>1892</v>
+        <v>1900</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>1893</v>
+        <v>1901</v>
       </c>
       <c r="D64">
-        <v>3492</v>
+        <v>20252</v>
       </c>
       <c r="E64">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="F64">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="G64" s="1">
-        <v>4.8000000000000001E-5</v>
+        <v>106.33</v>
+      </c>
+      <c r="G64">
+        <v>1.7700000000000001E-3</v>
       </c>
       <c r="H64" s="9" t="s">
         <v>933</v>
@@ -20090,14 +20341,14 @@
       <c r="J64" t="s">
         <v>931</v>
       </c>
-      <c r="L64" s="16" t="s">
+      <c r="L64" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P64" s="16" t="s">
         <v>2436</v>
-      </c>
-      <c r="N64" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P64" s="9" t="s">
-        <v>2447</v>
       </c>
       <c r="R64" s="17" t="s">
         <v>931</v>
@@ -20111,28 +20362,28 @@
         <v>1931</v>
       </c>
       <c r="B65" t="s">
-        <v>1894</v>
+        <v>1902</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>1895</v>
+        <v>1903</v>
       </c>
       <c r="D65">
-        <v>720</v>
+        <v>361</v>
       </c>
       <c r="E65">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F65">
-        <v>3.78</v>
+        <v>1.9</v>
       </c>
       <c r="G65">
-        <v>1.1E-4</v>
+        <v>3.8800000000000002E-3</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J65" t="s">
-        <v>931</v>
+        <v>1827</v>
       </c>
       <c r="L65" s="17" t="s">
         <v>931</v>
@@ -20145,9 +20396,6 @@
       </c>
       <c r="R65" s="17" t="s">
         <v>931</v>
-      </c>
-      <c r="S65" t="s">
-        <v>2442</v>
       </c>
       <c r="T65" s="17" t="s">
         <v>931</v>
@@ -20158,46 +20406,43 @@
         <v>1931</v>
       </c>
       <c r="B66" t="s">
-        <v>1896</v>
+        <v>1904</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1897</v>
+        <v>1905</v>
       </c>
       <c r="D66">
-        <v>1969</v>
+        <v>361</v>
       </c>
       <c r="E66">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F66">
-        <v>10.34</v>
+        <v>1.9</v>
       </c>
       <c r="G66">
-        <v>1.7000000000000001E-4</v>
+        <v>4.13E-3</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>933</v>
       </c>
-      <c r="I66" s="13" t="s">
-        <v>1825</v>
-      </c>
       <c r="J66" t="s">
-        <v>931</v>
+        <v>1826</v>
       </c>
       <c r="L66" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N66" s="16" t="s">
-        <v>2436</v>
-      </c>
-      <c r="P66" s="10" t="s">
-        <v>2448</v>
+      <c r="N66" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R66" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="T66" s="15" t="s">
-        <v>933</v>
+      <c r="T66" s="17" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -20205,22 +20450,22 @@
         <v>1931</v>
       </c>
       <c r="B67" t="s">
-        <v>1898</v>
+        <v>1906</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>1899</v>
+        <v>1907</v>
       </c>
       <c r="D67">
-        <v>1480</v>
+        <v>32</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F67">
-        <v>7.77</v>
+        <v>0.17</v>
       </c>
       <c r="G67">
-        <v>1.65E-3</v>
+        <v>4.8300000000000001E-3</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>933</v>
@@ -20249,22 +20494,22 @@
         <v>1931</v>
       </c>
       <c r="B68" t="s">
-        <v>1900</v>
+        <v>1908</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1901</v>
+        <v>1909</v>
       </c>
       <c r="D68">
-        <v>20252</v>
+        <v>20703</v>
       </c>
       <c r="E68">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F68">
-        <v>106.33</v>
+        <v>108.69</v>
       </c>
       <c r="G68">
-        <v>1.7700000000000001E-3</v>
+        <v>5.6499999999999996E-3</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>933</v>
@@ -20278,8 +20523,8 @@
       <c r="N68" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="P68" s="16" t="s">
-        <v>2436</v>
+      <c r="P68" s="9" t="s">
+        <v>2447</v>
       </c>
       <c r="R68" s="17" t="s">
         <v>931</v>
@@ -20293,31 +20538,31 @@
         <v>1931</v>
       </c>
       <c r="B69" t="s">
-        <v>1902</v>
+        <v>1910</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>1903</v>
+        <v>1911</v>
       </c>
       <c r="D69">
-        <v>361</v>
+        <v>32</v>
       </c>
       <c r="E69">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>1.9</v>
+        <v>0.17</v>
       </c>
       <c r="G69">
-        <v>3.8800000000000002E-3</v>
+        <v>6.6699999999999997E-3</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J69" t="s">
-        <v>1827</v>
-      </c>
-      <c r="L69" s="17" t="s">
         <v>931</v>
+      </c>
+      <c r="L69" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="N69" s="17" t="s">
         <v>931</v>
@@ -20330,6 +20575,9 @@
       </c>
       <c r="T69" s="17" t="s">
         <v>931</v>
+      </c>
+      <c r="U69" t="s">
+        <v>2443</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -20337,28 +20585,28 @@
         <v>1931</v>
       </c>
       <c r="B70" t="s">
-        <v>1904</v>
+        <v>1914</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1905</v>
+        <v>1915</v>
       </c>
       <c r="D70">
-        <v>361</v>
+        <v>19850</v>
       </c>
       <c r="E70">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="F70">
-        <v>1.9</v>
+        <v>104.21</v>
       </c>
       <c r="G70">
-        <v>4.13E-3</v>
+        <v>8.0300000000000007E-3</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>933</v>
       </c>
       <c r="J70" t="s">
-        <v>1826</v>
+        <v>931</v>
       </c>
       <c r="L70" s="17" t="s">
         <v>931</v>
@@ -20381,22 +20629,22 @@
         <v>1931</v>
       </c>
       <c r="B71" t="s">
-        <v>1906</v>
+        <v>1912</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1907</v>
+        <v>1913</v>
       </c>
       <c r="D71">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E71">
         <v>3</v>
       </c>
       <c r="F71">
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G71">
-        <v>4.8300000000000001E-3</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>933</v>
@@ -20404,8 +20652,8 @@
       <c r="J71" t="s">
         <v>931</v>
       </c>
-      <c r="L71" s="17" t="s">
-        <v>931</v>
+      <c r="L71" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="N71" s="17" t="s">
         <v>931</v>
@@ -20413,43 +20661,43 @@
       <c r="P71" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R71" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T71" s="17" t="s">
-        <v>931</v>
+      <c r="T71" s="15" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="72" spans="1:21">
       <c r="A72" t="s">
-        <v>1931</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1908</v>
+        <v>1933</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>1909</v>
-      </c>
-      <c r="D72">
-        <v>20703</v>
-      </c>
-      <c r="E72">
-        <v>151</v>
-      </c>
-      <c r="F72">
-        <v>108.69</v>
-      </c>
-      <c r="G72">
-        <v>5.6499999999999996E-3</v>
+        <v>60</v>
+      </c>
+      <c r="D72" s="13">
+        <v>1397</v>
+      </c>
+      <c r="E72" s="13">
+        <v>11</v>
+      </c>
+      <c r="F72" s="13">
+        <v>6.73</v>
+      </c>
+      <c r="G72" s="13">
+        <v>8.3400000000000002E-3</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="I72" s="13" t="s">
+        <v>942</v>
       </c>
       <c r="J72" t="s">
         <v>931</v>
       </c>
-      <c r="L72" s="17" t="s">
-        <v>931</v>
+      <c r="L72" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="N72" s="17" t="s">
         <v>931</v>
@@ -20457,34 +20705,31 @@
       <c r="P72" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R72" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T72" s="17" t="s">
-        <v>931</v>
+      <c r="Q72" t="s">
+        <v>2449</v>
       </c>
     </row>
     <row r="73" spans="1:21">
       <c r="A73" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B73" t="s">
-        <v>1910</v>
+        <v>1922</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>1911</v>
+        <v>1923</v>
       </c>
       <c r="D73">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F73">
-        <v>0.17</v>
-      </c>
-      <c r="G73">
-        <v>6.6699999999999997E-3</v>
+        <v>0.21</v>
+      </c>
+      <c r="G73" s="1">
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>933</v>
@@ -20492,46 +20737,37 @@
       <c r="J73" t="s">
         <v>931</v>
       </c>
-      <c r="L73" s="15" t="s">
+      <c r="L73" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N73" s="15" t="s">
         <v>933</v>
-      </c>
-      <c r="N73" s="17" t="s">
-        <v>931</v>
       </c>
       <c r="P73" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R73" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T73" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="U73" t="s">
-        <v>2443</v>
-      </c>
     </row>
     <row r="74" spans="1:21">
       <c r="A74" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B74" t="s">
-        <v>1912</v>
+        <v>1924</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>1913</v>
+        <v>1925</v>
       </c>
       <c r="D74">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E74">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F74">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G74">
-        <v>6.7499999999999999E-3</v>
+        <v>0.21</v>
+      </c>
+      <c r="G74" s="1">
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>933</v>
@@ -20539,40 +20775,37 @@
       <c r="J74" t="s">
         <v>931</v>
       </c>
-      <c r="L74" s="15" t="s">
+      <c r="L74" s="17" t="s">
+        <v>931</v>
+      </c>
+      <c r="N74" s="15" t="s">
         <v>933</v>
-      </c>
-      <c r="N74" s="17" t="s">
-        <v>931</v>
       </c>
       <c r="P74" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="T74" s="15" t="s">
-        <v>933</v>
-      </c>
     </row>
     <row r="75" spans="1:21">
       <c r="A75" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B75" t="s">
-        <v>1914</v>
+        <v>1926</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>1915</v>
+        <v>1927</v>
       </c>
       <c r="D75">
-        <v>19850</v>
+        <v>42</v>
       </c>
       <c r="E75">
-        <v>146</v>
+        <v>4</v>
       </c>
       <c r="F75">
-        <v>104.21</v>
-      </c>
-      <c r="G75">
-        <v>8.0300000000000007E-3</v>
+        <v>0.21</v>
+      </c>
+      <c r="G75" s="1">
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>933</v>
@@ -20583,23 +20816,19 @@
       <c r="L75" s="17" t="s">
         <v>931</v>
       </c>
-      <c r="N75" s="17" t="s">
-        <v>931</v>
+      <c r="N75" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="P75" s="9" t="s">
         <v>2447</v>
       </c>
-      <c r="R75" s="17" t="s">
-        <v>931</v>
-      </c>
-      <c r="T75" s="17" t="s">
-        <v>931</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="A2:U75">
-    <sortCondition ref="A2:A75" customList="BP,MF,CC"/>
-    <sortCondition ref="G2:G75"/>
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="R2:R75" dxfId="5"/>
+    <sortCondition sortBy="cellColor" ref="T2:T75" dxfId="4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>